<commit_message>
added courses added survey added more data samples
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanaBoscolo\source\repos\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1514529D-6972-456B-B603-53FE860E9EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AACE68-D389-4C63-8F78-52DDFC2AC392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="4008" windowWidth="23016" windowHeight="11580" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="3825" yWindow="10800" windowWidth="25695" windowHeight="15795" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="361">
   <si>
     <t>ItemID</t>
   </si>
@@ -223,9 +223,6 @@
   </si>
   <si>
     <t>Ich quittiere die Lieferung.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 - 1 - 3 - 2 </t>
   </si>
   <si>
     <t xml:space="preserve">Fachkraft für Lagerlogistik </t>
@@ -1113,6 +1110,21 @@
   </si>
   <si>
     <t>SK34B01_Sicherheitshinweis_Schuhe.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4a - 1b - 3c - 2d </t>
+  </si>
+  <si>
+    <t>Bertelsmann Stiftung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Fachkraft Lagerlogistik (Fachlagerist) </t>
+  </si>
+  <si>
+    <t>Mit diesem kurzen Test kannst du deine Fähigkeiten prüfen. Das Ergebniss zeigt dir wie viel Erfahrung du in den verschiedenen Bereichen des Berufes mitbringst. Aufbauend auf deinen Kompetenzen können wir dir passende Vorschläge für Weiterbildungen zeigen.</t>
+  </si>
+  <si>
+    <t>Die Fragen beantwortest du, indem du entweder die passende Antwort auswählst, eine richtige Reihenfolge herstellst oder die passenden Paare bildest. Probiere es aus!</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1358,17 +1370,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2242,19 +2246,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
   <dimension ref="A1:BO29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
-      <selection activeCell="BP1" sqref="BP1:BP1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BH2" sqref="BH2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.44140625" customWidth="1"/>
-    <col min="46" max="46" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" customWidth="1"/>
+    <col min="46" max="46" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:67" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2418,56 +2422,55 @@
         <v>53</v>
       </c>
       <c r="BC1" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="BD1" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="BJ1" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="BK1" s="22" t="s">
+      <c r="BK1" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="BL1" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="BL1" s="22" t="s">
+      <c r="BM1" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="BM1" s="22" t="s">
+      <c r="BN1" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="BN1" s="22" t="s">
+      <c r="BO1" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="BO1" s="22" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="D2" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="16"/>
       <c r="J2" t="s">
         <v>57</v>
       </c>
@@ -2477,110 +2480,133 @@
       <c r="N2">
         <v>4</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="O2" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="19" t="s">
+      <c r="P2" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="R2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="21" t="s">
-        <v>62</v>
+      <c r="U2" t="s">
+        <v>356</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>2</v>
+      </c>
+      <c r="AC2">
+        <v>3</v>
+      </c>
+      <c r="AD2">
+        <v>4</v>
       </c>
       <c r="AK2">
         <v>1</v>
       </c>
       <c r="AQ2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS2">
         <v>51312</v>
       </c>
       <c r="AT2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU2" t="s">
         <v>64</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="BC2">
+        <v>0</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>359</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>360</v>
+      </c>
+      <c r="BF2">
+        <v>20</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>357</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>358</v>
+      </c>
+      <c r="BK2">
+        <v>3</v>
+      </c>
+      <c r="BL2">
+        <v>0</v>
+      </c>
+      <c r="BM2">
+        <v>0</v>
+      </c>
+      <c r="BN2">
+        <v>0</v>
+      </c>
+      <c r="BO2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>65</v>
       </c>
-      <c r="BC2">
-        <v>0</v>
-      </c>
-      <c r="BK2">
-        <v>3</v>
-      </c>
-      <c r="BL2">
-        <v>0</v>
-      </c>
-      <c r="BM2">
-        <v>0</v>
-      </c>
-      <c r="BN2">
-        <v>0</v>
-      </c>
-      <c r="BO2" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
       <c r="C3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="J3" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>334</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
         <v>69</v>
       </c>
-      <c r="L3">
-        <v>4</v>
-      </c>
-      <c r="N3">
-        <v>3</v>
-      </c>
-      <c r="O3" s="19" t="s">
+      <c r="P3" t="s">
         <v>70</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="Q3" t="s">
         <v>71</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="R3" t="s">
         <v>72</v>
       </c>
-      <c r="R3" s="19" t="s">
+      <c r="U3" t="s">
         <v>73</v>
-      </c>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="21" t="s">
-        <v>74</v>
       </c>
       <c r="AK3">
         <v>1</v>
       </c>
       <c r="AQ3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS3">
         <v>51312</v>
       </c>
       <c r="AT3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AU3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BC3">
         <v>0</v>
@@ -2597,210 +2623,203 @@
       <c r="BN3">
         <v>0</v>
       </c>
-      <c r="BO3" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
         <v>76</v>
       </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="J4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="16"/>
-      <c r="J4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L4">
-        <v>4</v>
-      </c>
-      <c r="N4">
-        <v>3</v>
-      </c>
-      <c r="O4" s="19" t="s">
+      <c r="P4" t="s">
         <v>78</v>
       </c>
-      <c r="P4" s="19" t="s">
+      <c r="Q4" t="s">
         <v>79</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="R4" t="s">
         <v>80</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="U4" t="s">
         <v>81</v>
-      </c>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="21" t="s">
-        <v>82</v>
       </c>
       <c r="AK4">
         <v>1</v>
       </c>
       <c r="AQ4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS4">
         <v>51312</v>
       </c>
       <c r="AT4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AU4" t="s">
+        <v>82</v>
+      </c>
+      <c r="BC4">
+        <v>0</v>
+      </c>
+      <c r="BK4">
+        <v>3</v>
+      </c>
+      <c r="BL4">
+        <v>0</v>
+      </c>
+      <c r="BM4">
+        <v>0</v>
+      </c>
+      <c r="BN4">
+        <v>0</v>
+      </c>
+      <c r="BO4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>83</v>
       </c>
-      <c r="BC4">
-        <v>0</v>
-      </c>
-      <c r="BK4" s="21">
-        <v>3</v>
-      </c>
-      <c r="BL4">
-        <v>0</v>
-      </c>
-      <c r="BM4">
-        <v>0</v>
-      </c>
-      <c r="BN4">
-        <v>0</v>
-      </c>
-      <c r="BO4" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
         <v>84</v>
       </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" s="17"/>
+      <c r="J5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="J5" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5">
-        <v>4</v>
-      </c>
-      <c r="N5">
-        <v>3</v>
-      </c>
-      <c r="O5" s="19" t="s">
+      <c r="P5" t="s">
         <v>86</v>
       </c>
-      <c r="P5" s="19" t="s">
+      <c r="Q5" t="s">
         <v>87</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="R5" t="s">
         <v>88</v>
       </c>
-      <c r="R5" s="19" t="s">
+      <c r="U5" t="s">
         <v>89</v>
-      </c>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="21" t="s">
-        <v>90</v>
       </c>
       <c r="AK5">
         <v>1</v>
       </c>
       <c r="AQ5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS5">
         <v>51312</v>
       </c>
       <c r="AT5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AU5" t="s">
+        <v>90</v>
+      </c>
+      <c r="BC5">
+        <v>0</v>
+      </c>
+      <c r="BK5">
+        <v>3</v>
+      </c>
+      <c r="BL5">
+        <v>0</v>
+      </c>
+      <c r="BM5">
+        <v>0</v>
+      </c>
+      <c r="BN5">
+        <v>0</v>
+      </c>
+      <c r="BO5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>91</v>
       </c>
-      <c r="BC5">
-        <v>0</v>
-      </c>
-      <c r="BK5" s="21">
-        <v>3</v>
-      </c>
-      <c r="BL5">
-        <v>0</v>
-      </c>
-      <c r="BM5">
-        <v>0</v>
-      </c>
-      <c r="BN5">
-        <v>0</v>
-      </c>
-      <c r="BO5" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D6" t="s">
         <v>92</v>
       </c>
-      <c r="C6" t="s">
-        <v>331</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="F6" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="J6" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
         <v>93</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>356</v>
-      </c>
-      <c r="J6" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6">
-        <v>4</v>
-      </c>
-      <c r="N6">
-        <v>3</v>
-      </c>
-      <c r="O6" s="19" t="s">
+      <c r="P6" t="s">
         <v>94</v>
       </c>
-      <c r="P6" s="19" t="s">
+      <c r="Q6" t="s">
         <v>95</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="R6" t="s">
         <v>96</v>
       </c>
-      <c r="R6" s="19" t="s">
+      <c r="U6" t="s">
         <v>97</v>
-      </c>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="21" t="s">
-        <v>98</v>
       </c>
       <c r="AK6">
         <v>1</v>
       </c>
       <c r="AQ6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS6">
         <v>51312</v>
       </c>
       <c r="AT6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AU6" t="s">
         <v>99</v>
       </c>
-      <c r="AU6" t="s">
-        <v>100</v>
-      </c>
       <c r="BC6">
         <v>0</v>
       </c>
-      <c r="BK6" s="21">
+      <c r="BK6">
         <v>3</v>
       </c>
       <c r="BL6">
@@ -2812,68 +2831,66 @@
       <c r="BN6">
         <v>0</v>
       </c>
-      <c r="BO6" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>330</v>
+      </c>
+      <c r="D7" t="s">
         <v>101</v>
       </c>
-      <c r="C7" t="s">
-        <v>331</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="F7" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="J7" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>335</v>
-      </c>
-      <c r="J7" t="s">
-        <v>69</v>
-      </c>
-      <c r="L7">
-        <v>4</v>
-      </c>
-      <c r="N7">
-        <v>3</v>
-      </c>
-      <c r="O7" s="19" t="s">
+      <c r="P7" t="s">
         <v>103</v>
       </c>
-      <c r="P7" s="19" t="s">
+      <c r="Q7" t="s">
         <v>104</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="R7" t="s">
         <v>105</v>
       </c>
-      <c r="R7" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="21" t="s">
-        <v>82</v>
+      <c r="U7" t="s">
+        <v>81</v>
       </c>
       <c r="AK7">
         <v>1</v>
       </c>
       <c r="AQ7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS7">
         <v>51312</v>
       </c>
       <c r="AT7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AU7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BC7">
         <v>0</v>
       </c>
-      <c r="BK7" s="21">
+      <c r="BK7">
         <v>3</v>
       </c>
       <c r="BL7">
@@ -2885,23 +2902,22 @@
       <c r="BN7">
         <v>0</v>
       </c>
-      <c r="BO7" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>331</v>
+      </c>
+      <c r="D8" t="s">
         <v>108</v>
       </c>
-      <c r="C8" t="s">
-        <v>332</v>
-      </c>
-      <c r="D8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8" s="16"/>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L8">
         <v>4</v>
@@ -2909,42 +2925,40 @@
       <c r="N8">
         <v>3</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="P8" s="16" t="s">
         <v>339</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="Q8" s="16" t="s">
         <v>340</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="R8" s="16" t="s">
         <v>341</v>
       </c>
-      <c r="R8" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="21" t="s">
-        <v>90</v>
+      <c r="U8" t="s">
+        <v>89</v>
       </c>
       <c r="AK8">
         <v>1</v>
       </c>
       <c r="AQ8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS8">
         <v>51312</v>
       </c>
       <c r="AT8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AU8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="BC8">
         <v>0</v>
       </c>
-      <c r="BK8" s="21">
+      <c r="BK8">
         <v>3</v>
       </c>
       <c r="BL8">
@@ -2956,68 +2970,66 @@
       <c r="BN8">
         <v>4</v>
       </c>
-      <c r="BO8" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" t="s">
+        <v>330</v>
+      </c>
+      <c r="D9" t="s">
         <v>111</v>
       </c>
-      <c r="C9" t="s">
-        <v>331</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F9" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="J9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9" t="s">
         <v>112</v>
       </c>
-      <c r="F9" s="17" t="s">
-        <v>336</v>
-      </c>
-      <c r="J9" t="s">
-        <v>69</v>
-      </c>
-      <c r="L9">
-        <v>4</v>
-      </c>
-      <c r="N9">
-        <v>3</v>
-      </c>
-      <c r="O9" s="19" t="s">
+      <c r="P9" t="s">
         <v>113</v>
       </c>
-      <c r="P9" s="19" t="s">
+      <c r="Q9" t="s">
         <v>114</v>
       </c>
-      <c r="Q9" s="19" t="s">
+      <c r="R9" t="s">
         <v>115</v>
       </c>
-      <c r="R9" s="19" t="s">
+      <c r="U9" t="s">
         <v>116</v>
-      </c>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="21" t="s">
-        <v>117</v>
       </c>
       <c r="AK9">
         <v>1</v>
       </c>
       <c r="AQ9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS9">
         <v>51312</v>
       </c>
       <c r="AT9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AU9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="BC9">
         <v>0</v>
       </c>
-      <c r="BK9" s="21">
+      <c r="BK9">
         <v>3</v>
       </c>
       <c r="BL9">
@@ -3029,78 +3041,75 @@
       <c r="BN9">
         <v>0</v>
       </c>
-      <c r="BO9" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" t="s">
         <v>119</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>120</v>
       </c>
-      <c r="D10" t="s">
+      <c r="J10" t="s">
         <v>121</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="J10" t="s">
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10" t="s">
+        <v>123</v>
+      </c>
+      <c r="P10" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>125</v>
+      </c>
+      <c r="R10" t="s">
+        <v>126</v>
+      </c>
+      <c r="U10" t="s">
         <v>122</v>
       </c>
-      <c r="L10">
-        <v>4</v>
-      </c>
-      <c r="N10">
-        <v>4</v>
-      </c>
-      <c r="O10" t="s">
-        <v>124</v>
-      </c>
-      <c r="P10" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>126</v>
-      </c>
-      <c r="R10" t="s">
-        <v>127</v>
-      </c>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA10" s="24" t="s">
+      <c r="AA10" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="AB10" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="AB10" s="24" t="s">
+      <c r="AC10" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="AC10" s="24" t="s">
+      <c r="AD10" s="18" t="s">
         <v>318</v>
-      </c>
-      <c r="AD10" s="24" t="s">
-        <v>319</v>
       </c>
       <c r="AK10">
         <v>1</v>
       </c>
       <c r="AQ10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS10">
         <v>51312</v>
       </c>
       <c r="AT10" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU10" t="s">
         <v>128</v>
       </c>
-      <c r="AU10" t="s">
-        <v>129</v>
-      </c>
       <c r="BC10">
         <v>0</v>
       </c>
-      <c r="BK10" s="21">
+      <c r="BK10">
         <v>3</v>
       </c>
       <c r="BL10">
@@ -3112,66 +3121,63 @@
       <c r="BN10">
         <v>4</v>
       </c>
-      <c r="BO10" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
         <v>130</v>
       </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="J11" t="s">
+        <v>68</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11" t="s">
+        <v>311</v>
+      </c>
+      <c r="P11" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>313</v>
+      </c>
+      <c r="R11" t="s">
+        <v>314</v>
+      </c>
+      <c r="U11" t="s">
         <v>131</v>
-      </c>
-      <c r="F11" s="16"/>
-      <c r="J11" t="s">
-        <v>69</v>
-      </c>
-      <c r="L11">
-        <v>4</v>
-      </c>
-      <c r="N11">
-        <v>3</v>
-      </c>
-      <c r="O11" s="19" t="s">
-        <v>312</v>
-      </c>
-      <c r="P11" s="19" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q11" s="19" t="s">
-        <v>314</v>
-      </c>
-      <c r="R11" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="S11" s="19"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="21" t="s">
-        <v>132</v>
       </c>
       <c r="AK11">
         <v>1</v>
       </c>
       <c r="AQ11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS11">
         <v>51312</v>
       </c>
       <c r="AT11" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU11" t="s">
         <v>128</v>
       </c>
-      <c r="AU11" t="s">
-        <v>129</v>
-      </c>
       <c r="BC11">
         <v>0</v>
       </c>
-      <c r="BK11" s="21">
+      <c r="BK11">
         <v>3</v>
       </c>
       <c r="BL11">
@@ -3183,66 +3189,63 @@
       <c r="BN11">
         <v>0</v>
       </c>
-      <c r="BO11" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" t="s">
+        <v>330</v>
+      </c>
+      <c r="D12" t="s">
         <v>133</v>
       </c>
-      <c r="C12" t="s">
-        <v>331</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="F12" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="J12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12" t="s">
         <v>134</v>
       </c>
-      <c r="F12" s="17" t="s">
-        <v>337</v>
-      </c>
-      <c r="J12" t="s">
-        <v>69</v>
-      </c>
-      <c r="L12">
-        <v>4</v>
-      </c>
-      <c r="N12">
-        <v>3</v>
-      </c>
-      <c r="O12" s="19" t="s">
+      <c r="P12" t="s">
         <v>135</v>
       </c>
-      <c r="P12" s="19" t="s">
+      <c r="Q12" t="s">
         <v>136</v>
       </c>
-      <c r="Q12" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="21" t="s">
-        <v>117</v>
+      <c r="U12" t="s">
+        <v>116</v>
       </c>
       <c r="AK12">
         <v>1</v>
       </c>
       <c r="AQ12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS12">
         <v>51312</v>
       </c>
       <c r="AT12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AU12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BC12">
         <v>0</v>
       </c>
-      <c r="BK12" s="21">
+      <c r="BK12">
         <v>3</v>
       </c>
       <c r="BL12">
@@ -3254,66 +3257,63 @@
       <c r="BN12">
         <v>0</v>
       </c>
-      <c r="BO12" s="21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
         <v>139</v>
       </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="J13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13" t="s">
         <v>140</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="J13" t="s">
-        <v>69</v>
-      </c>
-      <c r="L13">
-        <v>4</v>
-      </c>
-      <c r="N13">
-        <v>3</v>
-      </c>
-      <c r="O13" s="19" t="s">
+      <c r="P13" t="s">
         <v>141</v>
       </c>
-      <c r="P13" s="19" t="s">
+      <c r="Q13" t="s">
         <v>142</v>
       </c>
-      <c r="Q13" s="19" t="s">
+      <c r="R13" t="s">
         <v>143</v>
       </c>
-      <c r="R13" s="19" t="s">
+      <c r="U13" t="s">
         <v>144</v>
-      </c>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="21" t="s">
-        <v>145</v>
       </c>
       <c r="AK13">
         <v>1</v>
       </c>
       <c r="AQ13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS13">
         <v>51312</v>
       </c>
       <c r="AT13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AU13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BC13">
         <v>0</v>
       </c>
-      <c r="BK13" s="21">
+      <c r="BK13">
         <v>3</v>
       </c>
       <c r="BL13">
@@ -3325,210 +3325,202 @@
       <c r="BN13">
         <v>0</v>
       </c>
-      <c r="BO13" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
         <v>147</v>
       </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="J14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14" t="s">
         <v>148</v>
       </c>
-      <c r="F14" s="16"/>
-      <c r="J14" t="s">
-        <v>69</v>
-      </c>
-      <c r="L14">
-        <v>4</v>
-      </c>
-      <c r="N14">
-        <v>3</v>
-      </c>
-      <c r="O14" s="19" t="s">
+      <c r="P14" t="s">
         <v>149</v>
       </c>
-      <c r="P14" s="19" t="s">
+      <c r="Q14" t="s">
         <v>150</v>
       </c>
-      <c r="Q14" s="19" t="s">
+      <c r="R14" t="s">
         <v>151</v>
       </c>
-      <c r="R14" s="19" t="s">
+      <c r="U14" t="s">
         <v>152</v>
-      </c>
-      <c r="S14" s="19"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="21" t="s">
-        <v>153</v>
       </c>
       <c r="AK14">
         <v>1</v>
       </c>
       <c r="AQ14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS14">
         <v>51312</v>
       </c>
       <c r="AT14" t="s">
+        <v>153</v>
+      </c>
+      <c r="AU14" t="s">
         <v>154</v>
       </c>
-      <c r="AU14" t="s">
+      <c r="BC14">
+        <v>0</v>
+      </c>
+      <c r="BK14">
+        <v>2</v>
+      </c>
+      <c r="BL14">
+        <v>3</v>
+      </c>
+      <c r="BM14">
+        <v>0</v>
+      </c>
+      <c r="BN14">
+        <v>0</v>
+      </c>
+      <c r="BO14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>155</v>
       </c>
-      <c r="BC14">
-        <v>0</v>
-      </c>
-      <c r="BK14" s="21">
-        <v>2</v>
-      </c>
-      <c r="BL14">
-        <v>3</v>
-      </c>
-      <c r="BM14">
-        <v>0</v>
-      </c>
-      <c r="BN14">
-        <v>0</v>
-      </c>
-      <c r="BO14" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
         <v>156</v>
       </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="J15" t="s">
+        <v>68</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+      <c r="O15" t="s">
         <v>157</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="J15" t="s">
-        <v>69</v>
-      </c>
-      <c r="L15">
-        <v>4</v>
-      </c>
-      <c r="N15">
-        <v>3</v>
-      </c>
-      <c r="O15" s="19" t="s">
+      <c r="P15" t="s">
         <v>158</v>
       </c>
-      <c r="P15" s="19" t="s">
+      <c r="Q15" t="s">
         <v>159</v>
       </c>
-      <c r="Q15" s="19" t="s">
+      <c r="R15" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="R15" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="21" t="s">
-        <v>153</v>
+      <c r="U15" t="s">
+        <v>152</v>
       </c>
       <c r="AK15">
         <v>1</v>
       </c>
       <c r="AQ15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS15">
         <v>51312</v>
       </c>
       <c r="AT15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AU15" t="s">
+        <v>161</v>
+      </c>
+      <c r="BC15">
+        <v>0</v>
+      </c>
+      <c r="BK15">
+        <v>2</v>
+      </c>
+      <c r="BL15">
+        <v>3</v>
+      </c>
+      <c r="BM15">
+        <v>0</v>
+      </c>
+      <c r="BN15">
+        <v>0</v>
+      </c>
+      <c r="BO15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>162</v>
       </c>
-      <c r="BC15">
-        <v>0</v>
-      </c>
-      <c r="BK15" s="21">
-        <v>2</v>
-      </c>
-      <c r="BL15">
-        <v>3</v>
-      </c>
-      <c r="BM15">
-        <v>0</v>
-      </c>
-      <c r="BN15">
-        <v>0</v>
-      </c>
-      <c r="BO15" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16" t="s">
         <v>163</v>
       </c>
-      <c r="C16" t="s">
-        <v>333</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="F16" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="J16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
+      <c r="O16" t="s">
         <v>164</v>
       </c>
-      <c r="F16" s="17" t="s">
-        <v>338</v>
-      </c>
-      <c r="J16" t="s">
-        <v>69</v>
-      </c>
-      <c r="L16">
-        <v>4</v>
-      </c>
-      <c r="N16">
-        <v>3</v>
-      </c>
-      <c r="O16" s="19" t="s">
+      <c r="P16" t="s">
         <v>165</v>
       </c>
-      <c r="P16" s="19" t="s">
+      <c r="Q16" t="s">
         <v>166</v>
       </c>
-      <c r="Q16" s="19" t="s">
+      <c r="R16" t="s">
         <v>167</v>
       </c>
-      <c r="R16" s="19" t="s">
+      <c r="U16" t="s">
         <v>168</v>
-      </c>
-      <c r="S16" s="19"/>
-      <c r="T16" s="19"/>
-      <c r="U16" s="21" t="s">
-        <v>169</v>
       </c>
       <c r="AK16">
         <v>1</v>
       </c>
       <c r="AQ16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS16">
         <v>51312</v>
       </c>
       <c r="AT16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AU16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BC16">
         <v>0</v>
       </c>
-      <c r="BK16" s="21">
+      <c r="BK16">
         <v>2</v>
       </c>
       <c r="BL16">
@@ -3540,23 +3532,22 @@
       <c r="BN16">
         <v>0</v>
       </c>
-      <c r="BO16" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" t="s">
+        <v>331</v>
+      </c>
+      <c r="D17" t="s">
         <v>170</v>
       </c>
-      <c r="C17" t="s">
-        <v>332</v>
-      </c>
-      <c r="D17" t="s">
-        <v>171</v>
-      </c>
-      <c r="F17" s="16"/>
       <c r="J17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L17">
         <v>4</v>
@@ -3564,141 +3555,135 @@
       <c r="N17">
         <v>3</v>
       </c>
-      <c r="O17" s="19" t="s">
+      <c r="O17" t="s">
+        <v>342</v>
+      </c>
+      <c r="P17" t="s">
         <v>343</v>
       </c>
-      <c r="P17" s="19" t="s">
+      <c r="Q17" t="s">
         <v>344</v>
       </c>
-      <c r="Q17" s="19" t="s">
+      <c r="R17" t="s">
         <v>345</v>
       </c>
-      <c r="R17" s="19" t="s">
-        <v>346</v>
-      </c>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="23" t="s">
-        <v>117</v>
+      <c r="U17" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="AK17">
         <v>1</v>
       </c>
       <c r="AQ17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS17">
         <v>51312</v>
       </c>
       <c r="AT17" t="s">
+        <v>171</v>
+      </c>
+      <c r="AU17" t="s">
         <v>172</v>
       </c>
-      <c r="AU17" t="s">
+      <c r="BC17">
+        <v>0</v>
+      </c>
+      <c r="BK17">
+        <v>3</v>
+      </c>
+      <c r="BL17">
+        <v>4</v>
+      </c>
+      <c r="BM17">
+        <v>0</v>
+      </c>
+      <c r="BN17">
+        <v>4</v>
+      </c>
+      <c r="BO17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>173</v>
       </c>
-      <c r="BC17">
-        <v>0</v>
-      </c>
-      <c r="BK17" s="21">
-        <v>3</v>
-      </c>
-      <c r="BL17">
-        <v>4</v>
-      </c>
-      <c r="BM17">
-        <v>0</v>
-      </c>
-      <c r="BN17">
-        <v>4</v>
-      </c>
-      <c r="BO17" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
         <v>174</v>
       </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="J18" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18" t="s">
         <v>175</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="J18" t="s">
-        <v>69</v>
-      </c>
-      <c r="L18">
-        <v>4</v>
-      </c>
-      <c r="N18">
-        <v>3</v>
-      </c>
-      <c r="O18" s="19" t="s">
+      <c r="P18" t="s">
         <v>176</v>
       </c>
-      <c r="P18" s="19" t="s">
+      <c r="Q18" t="s">
         <v>177</v>
       </c>
-      <c r="Q18" s="19" t="s">
+      <c r="R18" t="s">
         <v>178</v>
       </c>
-      <c r="R18" s="19" t="s">
+      <c r="U18" t="s">
         <v>179</v>
-      </c>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="21" t="s">
-        <v>180</v>
       </c>
       <c r="AK18">
         <v>1</v>
       </c>
       <c r="AQ18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS18">
         <v>51312</v>
       </c>
       <c r="AT18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AU18" t="s">
+        <v>180</v>
+      </c>
+      <c r="BC18">
+        <v>0</v>
+      </c>
+      <c r="BK18">
+        <v>3</v>
+      </c>
+      <c r="BL18">
+        <v>4</v>
+      </c>
+      <c r="BM18">
+        <v>0</v>
+      </c>
+      <c r="BN18">
+        <v>0</v>
+      </c>
+      <c r="BO18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>181</v>
       </c>
-      <c r="BC18">
-        <v>0</v>
-      </c>
-      <c r="BK18" s="21">
-        <v>3</v>
-      </c>
-      <c r="BL18">
-        <v>4</v>
-      </c>
-      <c r="BM18">
-        <v>0</v>
-      </c>
-      <c r="BN18">
-        <v>0</v>
-      </c>
-      <c r="BO18" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C19" t="s">
+        <v>331</v>
+      </c>
+      <c r="D19" t="s">
         <v>182</v>
       </c>
-      <c r="C19" t="s">
-        <v>332</v>
-      </c>
-      <c r="D19" t="s">
-        <v>183</v>
-      </c>
-      <c r="F19" s="16"/>
       <c r="J19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L19">
         <v>4</v>
@@ -3706,184 +3691,177 @@
       <c r="N19">
         <v>3</v>
       </c>
-      <c r="O19" s="19" t="s">
+      <c r="O19" t="s">
+        <v>346</v>
+      </c>
+      <c r="P19" t="s">
         <v>347</v>
       </c>
-      <c r="P19" s="19" t="s">
+      <c r="Q19" t="s">
         <v>348</v>
       </c>
-      <c r="Q19" s="19" t="s">
+      <c r="R19" t="s">
         <v>349</v>
       </c>
-      <c r="R19" s="19" t="s">
-        <v>350</v>
-      </c>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="21" t="s">
-        <v>117</v>
+      <c r="U19" t="s">
+        <v>116</v>
       </c>
       <c r="AK19">
         <v>1</v>
       </c>
       <c r="AQ19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS19">
         <v>51312</v>
       </c>
       <c r="AT19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AU19" t="s">
+        <v>183</v>
+      </c>
+      <c r="BC19">
+        <v>0</v>
+      </c>
+      <c r="BK19">
+        <v>3</v>
+      </c>
+      <c r="BL19">
+        <v>4</v>
+      </c>
+      <c r="BM19">
+        <v>0</v>
+      </c>
+      <c r="BN19">
+        <v>4</v>
+      </c>
+      <c r="BO19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>184</v>
       </c>
-      <c r="BC19">
-        <v>0</v>
-      </c>
-      <c r="BK19" s="21">
-        <v>3</v>
-      </c>
-      <c r="BL19">
-        <v>4</v>
-      </c>
-      <c r="BM19">
-        <v>0</v>
-      </c>
-      <c r="BN19">
-        <v>4</v>
-      </c>
-      <c r="BO19" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
         <v>185</v>
       </c>
-      <c r="C20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="J20" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+      <c r="O20" t="s">
         <v>186</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="J20" t="s">
-        <v>69</v>
-      </c>
-      <c r="L20">
-        <v>4</v>
-      </c>
-      <c r="N20">
-        <v>3</v>
-      </c>
-      <c r="O20" s="19" t="s">
+      <c r="P20" t="s">
         <v>187</v>
       </c>
-      <c r="P20" s="19" t="s">
+      <c r="Q20" t="s">
         <v>188</v>
       </c>
-      <c r="Q20" s="19" t="s">
+      <c r="R20" t="s">
         <v>189</v>
       </c>
-      <c r="R20" s="19" t="s">
+      <c r="U20" t="s">
         <v>190</v>
-      </c>
-      <c r="S20" s="19"/>
-      <c r="T20" s="19"/>
-      <c r="U20" s="21" t="s">
-        <v>191</v>
       </c>
       <c r="AK20">
         <v>1</v>
       </c>
       <c r="AQ20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS20">
         <v>51312</v>
       </c>
       <c r="AT20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AU20" t="s">
+        <v>191</v>
+      </c>
+      <c r="BC20">
+        <v>0</v>
+      </c>
+      <c r="BK20">
+        <v>3</v>
+      </c>
+      <c r="BL20">
+        <v>4</v>
+      </c>
+      <c r="BM20">
+        <v>0</v>
+      </c>
+      <c r="BN20">
+        <v>0</v>
+      </c>
+      <c r="BO20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>192</v>
       </c>
-      <c r="BC20">
-        <v>0</v>
-      </c>
-      <c r="BK20" s="21">
-        <v>3</v>
-      </c>
-      <c r="BL20">
-        <v>4</v>
-      </c>
-      <c r="BM20">
-        <v>0</v>
-      </c>
-      <c r="BN20">
-        <v>0</v>
-      </c>
-      <c r="BO20" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" t="s">
         <v>193</v>
       </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="F21" s="17"/>
+      <c r="J21" t="s">
+        <v>68</v>
+      </c>
+      <c r="L21">
+        <v>4</v>
+      </c>
+      <c r="N21">
+        <v>3</v>
+      </c>
+      <c r="O21" t="s">
         <v>194</v>
       </c>
-      <c r="F21" s="18"/>
-      <c r="J21" t="s">
-        <v>69</v>
-      </c>
-      <c r="L21">
-        <v>4</v>
-      </c>
-      <c r="N21">
-        <v>3</v>
-      </c>
-      <c r="O21" s="19" t="s">
+      <c r="P21" t="s">
         <v>195</v>
       </c>
-      <c r="P21" s="19" t="s">
+      <c r="Q21" t="s">
         <v>196</v>
       </c>
-      <c r="Q21" s="19" t="s">
+      <c r="R21" t="s">
         <v>197</v>
       </c>
-      <c r="R21" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="21" t="s">
-        <v>98</v>
+      <c r="U21" t="s">
+        <v>97</v>
       </c>
       <c r="AK21">
         <v>1</v>
       </c>
       <c r="AQ21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS21">
         <v>51312</v>
       </c>
       <c r="AT21" t="s">
+        <v>198</v>
+      </c>
+      <c r="AU21" t="s">
         <v>199</v>
       </c>
-      <c r="AU21" t="s">
-        <v>200</v>
-      </c>
       <c r="BC21">
         <v>0</v>
       </c>
-      <c r="BK21" s="21">
+      <c r="BK21">
         <v>3</v>
       </c>
       <c r="BL21">
@@ -3895,66 +3873,64 @@
       <c r="BN21">
         <v>0</v>
       </c>
-      <c r="BO21" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
         <v>201</v>
       </c>
-      <c r="C22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="F22" s="17"/>
+      <c r="J22" t="s">
+        <v>68</v>
+      </c>
+      <c r="L22">
+        <v>4</v>
+      </c>
+      <c r="N22">
+        <v>3</v>
+      </c>
+      <c r="O22" t="s">
         <v>202</v>
       </c>
-      <c r="F22" s="18"/>
-      <c r="J22" t="s">
-        <v>69</v>
-      </c>
-      <c r="L22">
-        <v>4</v>
-      </c>
-      <c r="N22">
-        <v>3</v>
-      </c>
-      <c r="O22" s="19" t="s">
+      <c r="P22" t="s">
         <v>203</v>
       </c>
-      <c r="P22" s="19" t="s">
+      <c r="Q22" t="s">
         <v>204</v>
       </c>
-      <c r="Q22" s="19" t="s">
+      <c r="R22" t="s">
         <v>205</v>
       </c>
-      <c r="R22" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="S22" s="19"/>
-      <c r="T22" s="19"/>
-      <c r="U22" s="21" t="s">
-        <v>153</v>
+      <c r="U22" t="s">
+        <v>152</v>
       </c>
       <c r="AK22">
         <v>1</v>
       </c>
       <c r="AQ22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS22">
         <v>51312</v>
       </c>
       <c r="AT22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AU22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="BC22">
         <v>0</v>
       </c>
-      <c r="BK22" s="21">
+      <c r="BK22">
         <v>3</v>
       </c>
       <c r="BL22">
@@ -3966,66 +3942,64 @@
       <c r="BN22">
         <v>0</v>
       </c>
-      <c r="BO22" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>207</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
         <v>208</v>
       </c>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="F23" s="17"/>
+      <c r="J23" t="s">
+        <v>68</v>
+      </c>
+      <c r="L23">
+        <v>4</v>
+      </c>
+      <c r="N23">
+        <v>3</v>
+      </c>
+      <c r="O23" t="s">
         <v>209</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="J23" t="s">
-        <v>69</v>
-      </c>
-      <c r="L23">
-        <v>4</v>
-      </c>
-      <c r="N23">
-        <v>3</v>
-      </c>
-      <c r="O23" s="19" t="s">
+      <c r="P23" t="s">
         <v>210</v>
       </c>
-      <c r="P23" s="19" t="s">
+      <c r="Q23" t="s">
         <v>211</v>
       </c>
-      <c r="Q23" s="19" t="s">
+      <c r="R23" t="s">
         <v>212</v>
       </c>
-      <c r="R23" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="S23" s="19"/>
-      <c r="T23" s="19"/>
-      <c r="U23" s="21" t="s">
-        <v>132</v>
+      <c r="U23" t="s">
+        <v>131</v>
       </c>
       <c r="AK23">
         <v>1</v>
       </c>
       <c r="AQ23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS23">
         <v>51312</v>
       </c>
       <c r="AT23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AU23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="BC23">
         <v>0</v>
       </c>
-      <c r="BK23" s="21">
+      <c r="BK23">
         <v>3</v>
       </c>
       <c r="BL23">
@@ -4037,68 +4011,66 @@
       <c r="BN23">
         <v>0</v>
       </c>
-      <c r="BO23" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>214</v>
+      </c>
+      <c r="C24" t="s">
+        <v>330</v>
+      </c>
+      <c r="D24" t="s">
         <v>215</v>
       </c>
-      <c r="C24" t="s">
-        <v>331</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="F24" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="J24" t="s">
+        <v>68</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="N24">
+        <v>3</v>
+      </c>
+      <c r="O24" t="s">
         <v>216</v>
       </c>
-      <c r="F24" s="17" t="s">
-        <v>322</v>
-      </c>
-      <c r="J24" t="s">
-        <v>69</v>
-      </c>
-      <c r="L24">
-        <v>4</v>
-      </c>
-      <c r="N24">
-        <v>3</v>
-      </c>
-      <c r="O24" s="19" t="s">
+      <c r="P24" t="s">
         <v>217</v>
       </c>
-      <c r="P24" s="19" t="s">
+      <c r="Q24" t="s">
         <v>218</v>
       </c>
-      <c r="Q24" s="19" t="s">
+      <c r="R24" t="s">
         <v>219</v>
       </c>
-      <c r="R24" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="S24" s="19"/>
-      <c r="T24" s="19"/>
-      <c r="U24" s="21" t="s">
-        <v>117</v>
+      <c r="U24" t="s">
+        <v>116</v>
       </c>
       <c r="AK24">
         <v>1</v>
       </c>
       <c r="AQ24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS24">
         <v>51312</v>
       </c>
       <c r="AT24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AU24" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="BC24">
         <v>0</v>
       </c>
-      <c r="BK24" s="21">
+      <c r="BK24">
         <v>3</v>
       </c>
       <c r="BL24">
@@ -4110,68 +4082,66 @@
       <c r="BN24">
         <v>0</v>
       </c>
-      <c r="BO24" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C25" t="s">
+        <v>330</v>
+      </c>
+      <c r="D25" t="s">
         <v>222</v>
       </c>
-      <c r="C25" t="s">
-        <v>331</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="F25" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="J25" t="s">
+        <v>68</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25" t="s">
         <v>223</v>
       </c>
-      <c r="F25" s="17" t="s">
-        <v>320</v>
-      </c>
-      <c r="J25" t="s">
-        <v>69</v>
-      </c>
-      <c r="L25">
-        <v>4</v>
-      </c>
-      <c r="N25">
-        <v>3</v>
-      </c>
-      <c r="O25" s="19" t="s">
+      <c r="P25" t="s">
         <v>224</v>
       </c>
-      <c r="P25" s="19" t="s">
+      <c r="Q25" t="s">
         <v>225</v>
       </c>
-      <c r="Q25" s="19" t="s">
+      <c r="R25" t="s">
         <v>226</v>
       </c>
-      <c r="R25" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="21" t="s">
-        <v>117</v>
+      <c r="U25" t="s">
+        <v>116</v>
       </c>
       <c r="AK25">
         <v>1</v>
       </c>
       <c r="AQ25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS25">
         <v>51312</v>
       </c>
       <c r="AT25" t="s">
+        <v>227</v>
+      </c>
+      <c r="AU25" t="s">
         <v>228</v>
       </c>
-      <c r="AU25" t="s">
-        <v>229</v>
-      </c>
       <c r="BC25">
         <v>0</v>
       </c>
-      <c r="BK25" s="21">
+      <c r="BK25">
         <v>3</v>
       </c>
       <c r="BL25">
@@ -4183,66 +4153,64 @@
       <c r="BN25">
         <v>0</v>
       </c>
-      <c r="BO25" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C26" t="s">
         <v>55</v>
       </c>
       <c r="D26" t="s">
+        <v>230</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="J26" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26">
+        <v>4</v>
+      </c>
+      <c r="N26">
+        <v>4</v>
+      </c>
+      <c r="O26" t="s">
         <v>231</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="J26" t="s">
-        <v>69</v>
-      </c>
-      <c r="L26">
-        <v>4</v>
-      </c>
-      <c r="N26">
-        <v>4</v>
-      </c>
-      <c r="O26" s="19" t="s">
+      <c r="P26" t="s">
         <v>232</v>
       </c>
-      <c r="P26" s="19" t="s">
+      <c r="Q26" t="s">
         <v>233</v>
       </c>
-      <c r="Q26" s="19" t="s">
+      <c r="R26" t="s">
         <v>234</v>
       </c>
-      <c r="R26" s="19" t="s">
+      <c r="U26" t="s">
         <v>235</v>
-      </c>
-      <c r="S26" s="19"/>
-      <c r="T26" s="19"/>
-      <c r="U26" s="21" t="s">
-        <v>236</v>
       </c>
       <c r="AK26">
         <v>1</v>
       </c>
       <c r="AQ26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS26">
         <v>51312</v>
       </c>
       <c r="AT26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AU26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="BC26">
         <v>0</v>
       </c>
-      <c r="BK26" s="21">
+      <c r="BK26">
         <v>3</v>
       </c>
       <c r="BL26">
@@ -4254,68 +4222,66 @@
       <c r="BN26">
         <v>0</v>
       </c>
-      <c r="BO26" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>237</v>
+      </c>
+      <c r="C27" t="s">
+        <v>330</v>
+      </c>
+      <c r="D27" t="s">
         <v>238</v>
       </c>
-      <c r="C27" t="s">
-        <v>331</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="F27" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="J27" t="s">
+        <v>68</v>
+      </c>
+      <c r="L27">
+        <v>4</v>
+      </c>
+      <c r="N27">
+        <v>3</v>
+      </c>
+      <c r="O27" t="s">
         <v>239</v>
       </c>
-      <c r="F27" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="J27" t="s">
-        <v>69</v>
-      </c>
-      <c r="L27">
-        <v>4</v>
-      </c>
-      <c r="N27">
-        <v>3</v>
-      </c>
-      <c r="O27" s="19" t="s">
+      <c r="P27" t="s">
         <v>240</v>
       </c>
-      <c r="P27" s="19" t="s">
+      <c r="Q27" t="s">
         <v>241</v>
       </c>
-      <c r="Q27" s="19" t="s">
+      <c r="R27" t="s">
         <v>242</v>
       </c>
-      <c r="R27" s="19" t="s">
-        <v>243</v>
-      </c>
-      <c r="S27" s="19"/>
-      <c r="T27" s="19"/>
-      <c r="U27" s="21" t="s">
-        <v>132</v>
+      <c r="U27" t="s">
+        <v>131</v>
       </c>
       <c r="AK27">
         <v>1</v>
       </c>
       <c r="AQ27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS27">
         <v>51312</v>
       </c>
       <c r="AT27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AU27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="BC27">
         <v>0</v>
       </c>
-      <c r="BK27" s="21">
+      <c r="BK27">
         <v>3</v>
       </c>
       <c r="BL27">
@@ -4327,66 +4293,64 @@
       <c r="BN27">
         <v>0</v>
       </c>
-      <c r="BO27" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>244</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
         <v>245</v>
       </c>
-      <c r="C28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="F28" s="17"/>
+      <c r="J28" t="s">
+        <v>68</v>
+      </c>
+      <c r="L28">
+        <v>4</v>
+      </c>
+      <c r="N28">
+        <v>3</v>
+      </c>
+      <c r="O28" t="s">
         <v>246</v>
       </c>
-      <c r="F28" s="18"/>
-      <c r="J28" t="s">
-        <v>69</v>
-      </c>
-      <c r="L28">
-        <v>4</v>
-      </c>
-      <c r="N28">
-        <v>3</v>
-      </c>
-      <c r="O28" s="19" t="s">
+      <c r="P28" t="s">
         <v>247</v>
       </c>
-      <c r="P28" s="19" t="s">
+      <c r="Q28" t="s">
         <v>248</v>
       </c>
-      <c r="Q28" s="19" t="s">
+      <c r="R28" t="s">
         <v>249</v>
       </c>
-      <c r="R28" s="19" t="s">
-        <v>250</v>
-      </c>
-      <c r="S28" s="19"/>
-      <c r="T28" s="19"/>
-      <c r="U28" s="21" t="s">
-        <v>153</v>
+      <c r="U28" t="s">
+        <v>152</v>
       </c>
       <c r="AK28">
         <v>1</v>
       </c>
       <c r="AQ28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS28">
         <v>51312</v>
       </c>
       <c r="AT28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AU28" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="BC28">
         <v>0</v>
       </c>
-      <c r="BK28" s="21">
+      <c r="BK28">
         <v>3</v>
       </c>
       <c r="BL28">
@@ -4398,66 +4362,64 @@
       <c r="BN28">
         <v>0</v>
       </c>
-      <c r="BO28" s="21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BO28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>251</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" t="s">
         <v>252</v>
       </c>
-      <c r="C29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="F29" s="17"/>
+      <c r="J29" t="s">
+        <v>68</v>
+      </c>
+      <c r="L29">
+        <v>4</v>
+      </c>
+      <c r="N29">
+        <v>3</v>
+      </c>
+      <c r="O29" t="s">
         <v>253</v>
       </c>
-      <c r="F29" s="18"/>
-      <c r="J29" t="s">
-        <v>69</v>
-      </c>
-      <c r="L29">
-        <v>4</v>
-      </c>
-      <c r="N29">
-        <v>3</v>
-      </c>
-      <c r="O29" s="19" t="s">
+      <c r="P29" t="s">
         <v>254</v>
       </c>
-      <c r="P29" s="19" t="s">
+      <c r="Q29" t="s">
         <v>255</v>
       </c>
-      <c r="Q29" s="19" t="s">
+      <c r="R29" t="s">
         <v>256</v>
       </c>
-      <c r="R29" s="19" t="s">
-        <v>257</v>
-      </c>
-      <c r="S29" s="19"/>
-      <c r="T29" s="19"/>
-      <c r="U29" s="21" t="s">
-        <v>191</v>
+      <c r="U29" t="s">
+        <v>190</v>
       </c>
       <c r="AK29">
         <v>1</v>
       </c>
       <c r="AQ29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AS29">
         <v>51312</v>
       </c>
       <c r="AT29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AU29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="BC29">
         <v>0</v>
       </c>
-      <c r="BK29" s="21">
+      <c r="BK29">
         <v>3</v>
       </c>
       <c r="BL29">
@@ -4469,7 +4431,7 @@
       <c r="BN29">
         <v>0</v>
       </c>
-      <c r="BO29" s="21">
+      <c r="BO29">
         <v>4</v>
       </c>
     </row>
@@ -4492,377 +4454,377 @@
       <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="F2" s="13" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="7">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="B3" s="7">
-        <v>4</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="10"/>
       <c r="F4" s="6"/>
       <c r="G4" s="11" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="10"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="10"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B7" s="8">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="8">
-        <v>4</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>277</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>278</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="B11" s="7">
-        <v>4</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>285</v>
-      </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="B14" s="8">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="B14" s="8">
-        <v>3</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>291</v>
-      </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="B16" s="7">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="B16" s="7">
-        <v>4</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>295</v>
-      </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B20" s="8">
+        <v>4</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="B20" s="8">
-        <v>4</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="F20" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="23.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="23.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B24" s="7">
         <v>5</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" display="https://www.biwe-bbq.de/weiterbildungsportal/themen/coaching-qualifizierung/einzelansicht/tq-lagerlogistik" xr:uid="{508EE104-A0F6-4678-8237-1AA62422A333}"/>
@@ -4878,26 +4840,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100879B58D3C23DCA4AAEF47596CA4D8E48" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee8b9d8723b80ccc4cb578ffd4faacc7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02625a54-df84-4a3b-b049-0bb7e92cde0d" xmlns:ns3="c90f9e10-81f0-426e-b8bb-fc89022b3796" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64b8ed4db9a6e136c161da669116b9cc" ns2:_="" ns3:_="">
     <xsd:import namespace="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
@@ -5106,7 +5048,46 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
+    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -5123,29 +5104,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
-    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed UseCase Data and Creation
- Added Publisher
- Added Duration
- Fixed Assessment Type
- Fixed QuestionItems -> AnswerItems -> Layout Mapping
- Fixed Answer Result for EAFrequency, Survey and Rating
- Fixed Minor Datastruc Issue in AssessmentService

Co-Authored-By: talisi <5801746+talisi@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanaBoscolo\source\repos\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3AACE68-D389-4C63-8F78-52DDFC2AC392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D956CA0-8DE2-421B-8601-92FCB72F8858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="10800" windowWidth="25695" windowHeight="15795" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="3312" yWindow="7848" windowWidth="40428" windowHeight="22476" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="362">
   <si>
     <t>ItemID</t>
   </si>
@@ -1125,13 +1125,16 @@
   </si>
   <si>
     <t>Die Fragen beantwortest du, indem du entweder die passende Antwort auswählst, eine richtige Reihenfolge herstellst oder die passenden Paare bildest. Probiere es aus!</t>
+  </si>
+  <si>
+    <t>SKILL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1198,6 +1201,12 @@
       <color theme="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFC9A26D"/>
+      <name val="MesloLGM NF"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1329,7 +1338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1373,6 +1382,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2246,19 +2258,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
   <dimension ref="A1:BO29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BH2" sqref="BH2"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BF31" sqref="BF31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" customWidth="1"/>
-    <col min="46" max="46" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.44140625" customWidth="1"/>
+    <col min="46" max="46" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:67" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2461,7 +2473,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2522,8 +2534,8 @@
       <c r="AU2" t="s">
         <v>64</v>
       </c>
-      <c r="BC2">
-        <v>0</v>
+      <c r="BC2" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BD2" t="s">
         <v>359</v>
@@ -2556,7 +2568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -2608,8 +2620,8 @@
       <c r="AU3" t="s">
         <v>74</v>
       </c>
-      <c r="BC3">
-        <v>0</v>
+      <c r="BC3" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK3">
         <v>3</v>
@@ -2627,7 +2639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -2676,8 +2688,8 @@
       <c r="AU4" t="s">
         <v>82</v>
       </c>
-      <c r="BC4">
-        <v>0</v>
+      <c r="BC4" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK4">
         <v>3</v>
@@ -2695,7 +2707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -2745,8 +2757,8 @@
       <c r="AU5" t="s">
         <v>90</v>
       </c>
-      <c r="BC5">
-        <v>0</v>
+      <c r="BC5" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK5">
         <v>3</v>
@@ -2764,7 +2776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -2816,8 +2828,8 @@
       <c r="AU6" t="s">
         <v>99</v>
       </c>
-      <c r="BC6">
-        <v>0</v>
+      <c r="BC6" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK6">
         <v>3</v>
@@ -2835,7 +2847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>100</v>
       </c>
@@ -2887,8 +2899,8 @@
       <c r="AU7" t="s">
         <v>106</v>
       </c>
-      <c r="BC7">
-        <v>0</v>
+      <c r="BC7" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK7">
         <v>3</v>
@@ -2906,7 +2918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -2955,8 +2967,8 @@
       <c r="AU8" t="s">
         <v>109</v>
       </c>
-      <c r="BC8">
-        <v>0</v>
+      <c r="BC8" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK8">
         <v>3</v>
@@ -2974,7 +2986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>110</v>
       </c>
@@ -3026,8 +3038,8 @@
       <c r="AU9" t="s">
         <v>117</v>
       </c>
-      <c r="BC9">
-        <v>0</v>
+      <c r="BC9" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK9">
         <v>3</v>
@@ -3045,7 +3057,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>118</v>
       </c>
@@ -3106,8 +3118,8 @@
       <c r="AU10" t="s">
         <v>128</v>
       </c>
-      <c r="BC10">
-        <v>0</v>
+      <c r="BC10" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK10">
         <v>3</v>
@@ -3125,7 +3137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -3174,8 +3186,8 @@
       <c r="AU11" t="s">
         <v>128</v>
       </c>
-      <c r="BC11">
-        <v>0</v>
+      <c r="BC11" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK11">
         <v>3</v>
@@ -3193,7 +3205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>132</v>
       </c>
@@ -3242,8 +3254,8 @@
       <c r="AU12" t="s">
         <v>137</v>
       </c>
-      <c r="BC12">
-        <v>0</v>
+      <c r="BC12" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK12">
         <v>3</v>
@@ -3261,7 +3273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>138</v>
       </c>
@@ -3310,8 +3322,8 @@
       <c r="AU13" t="s">
         <v>145</v>
       </c>
-      <c r="BC13">
-        <v>0</v>
+      <c r="BC13" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK13">
         <v>3</v>
@@ -3329,7 +3341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>146</v>
       </c>
@@ -3378,8 +3390,8 @@
       <c r="AU14" t="s">
         <v>154</v>
       </c>
-      <c r="BC14">
-        <v>0</v>
+      <c r="BC14" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK14">
         <v>2</v>
@@ -3397,7 +3409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -3446,8 +3458,8 @@
       <c r="AU15" t="s">
         <v>161</v>
       </c>
-      <c r="BC15">
-        <v>0</v>
+      <c r="BC15" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK15">
         <v>2</v>
@@ -3465,7 +3477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>162</v>
       </c>
@@ -3517,8 +3529,8 @@
       <c r="AU16" t="s">
         <v>161</v>
       </c>
-      <c r="BC16">
-        <v>0</v>
+      <c r="BC16" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK16">
         <v>2</v>
@@ -3536,7 +3548,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>169</v>
       </c>
@@ -3585,8 +3597,8 @@
       <c r="AU17" t="s">
         <v>172</v>
       </c>
-      <c r="BC17">
-        <v>0</v>
+      <c r="BC17" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK17">
         <v>3</v>
@@ -3604,7 +3616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>173</v>
       </c>
@@ -3653,8 +3665,8 @@
       <c r="AU18" t="s">
         <v>180</v>
       </c>
-      <c r="BC18">
-        <v>0</v>
+      <c r="BC18" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK18">
         <v>3</v>
@@ -3672,7 +3684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>181</v>
       </c>
@@ -3721,8 +3733,8 @@
       <c r="AU19" t="s">
         <v>183</v>
       </c>
-      <c r="BC19">
-        <v>0</v>
+      <c r="BC19" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK19">
         <v>3</v>
@@ -3740,7 +3752,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>184</v>
       </c>
@@ -3789,8 +3801,8 @@
       <c r="AU20" t="s">
         <v>191</v>
       </c>
-      <c r="BC20">
-        <v>0</v>
+      <c r="BC20" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK20">
         <v>3</v>
@@ -3808,7 +3820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>192</v>
       </c>
@@ -3858,8 +3870,8 @@
       <c r="AU21" t="s">
         <v>199</v>
       </c>
-      <c r="BC21">
-        <v>0</v>
+      <c r="BC21" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK21">
         <v>3</v>
@@ -3877,7 +3889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>200</v>
       </c>
@@ -3927,8 +3939,8 @@
       <c r="AU22" t="s">
         <v>206</v>
       </c>
-      <c r="BC22">
-        <v>0</v>
+      <c r="BC22" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK22">
         <v>3</v>
@@ -3946,7 +3958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>207</v>
       </c>
@@ -3996,8 +4008,8 @@
       <c r="AU23" t="s">
         <v>213</v>
       </c>
-      <c r="BC23">
-        <v>0</v>
+      <c r="BC23" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK23">
         <v>3</v>
@@ -4015,7 +4027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>214</v>
       </c>
@@ -4067,8 +4079,8 @@
       <c r="AU24" t="s">
         <v>220</v>
       </c>
-      <c r="BC24">
-        <v>0</v>
+      <c r="BC24" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK24">
         <v>3</v>
@@ -4086,7 +4098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>221</v>
       </c>
@@ -4138,8 +4150,8 @@
       <c r="AU25" t="s">
         <v>228</v>
       </c>
-      <c r="BC25">
-        <v>0</v>
+      <c r="BC25" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK25">
         <v>3</v>
@@ -4157,7 +4169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>229</v>
       </c>
@@ -4207,8 +4219,8 @@
       <c r="AU26" t="s">
         <v>236</v>
       </c>
-      <c r="BC26">
-        <v>0</v>
+      <c r="BC26" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK26">
         <v>3</v>
@@ -4226,7 +4238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>237</v>
       </c>
@@ -4278,8 +4290,8 @@
       <c r="AU27" t="s">
         <v>243</v>
       </c>
-      <c r="BC27">
-        <v>0</v>
+      <c r="BC27" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK27">
         <v>3</v>
@@ -4297,7 +4309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>244</v>
       </c>
@@ -4347,8 +4359,8 @@
       <c r="AU28" t="s">
         <v>250</v>
       </c>
-      <c r="BC28">
-        <v>0</v>
+      <c r="BC28" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK28">
         <v>3</v>
@@ -4366,7 +4378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>251</v>
       </c>
@@ -4416,8 +4428,8 @@
       <c r="AU29" t="s">
         <v>257</v>
       </c>
-      <c r="BC29">
-        <v>0</v>
+      <c r="BC29" s="19" t="s">
+        <v>361</v>
       </c>
       <c r="BK29">
         <v>3</v>
@@ -4454,24 +4466,24 @@
       <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>258</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>259</v>
       </c>
@@ -4491,7 +4503,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>265</v>
       </c>
@@ -4514,7 +4526,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
@@ -4527,7 +4539,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
@@ -4537,7 +4549,7 @@
       <c r="E5" s="10"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
@@ -4547,7 +4559,7 @@
       <c r="E6" s="10"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>275</v>
       </c>
@@ -4568,7 +4580,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
@@ -4578,7 +4590,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
@@ -4588,7 +4600,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
@@ -4598,7 +4610,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>282</v>
       </c>
@@ -4616,7 +4628,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
@@ -4626,7 +4638,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
@@ -4636,7 +4648,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>287</v>
       </c>
@@ -4654,7 +4666,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
@@ -4664,7 +4676,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>292</v>
       </c>
@@ -4682,7 +4694,7 @@
       </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
@@ -4692,7 +4704,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
@@ -4702,7 +4714,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
@@ -4712,7 +4724,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>298</v>
       </c>
@@ -4732,7 +4744,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
@@ -4742,7 +4754,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="23.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="23.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
@@ -4752,7 +4764,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
@@ -4762,7 +4774,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>305</v>
       </c>
@@ -4780,7 +4792,7 @@
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
@@ -4790,7 +4802,7 @@
       <c r="E25" s="7"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
@@ -4800,7 +4812,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
@@ -4810,7 +4822,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
@@ -4820,11 +4832,11 @@
       <c r="E28" s="7"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" display="https://www.biwe-bbq.de/weiterbildungsportal/themen/coaching-qualifizierung/einzelansicht/tq-lagerlogistik" xr:uid="{508EE104-A0F6-4678-8237-1AA62422A333}"/>
@@ -4840,6 +4852,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100879B58D3C23DCA4AAEF47596CA4D8E48" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee8b9d8723b80ccc4cb578ffd4faacc7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02625a54-df84-4a3b-b049-0bb7e92cde0d" xmlns:ns3="c90f9e10-81f0-426e-b8bb-fc89022b3796" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64b8ed4db9a6e136c161da669116b9cc" ns2:_="" ns3:_="">
     <xsd:import namespace="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
@@ -5048,17 +5071,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5069,6 +5081,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5087,23 +5116,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed Associate Item Generation
Fixed Associate
Fixed Associate Generation
SORT for Dez. Testing is like Associate

Co-Authored-By: talisi <5801746+talisi@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D956CA0-8DE2-421B-8601-92FCB72F8858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C647EEB-F157-4E16-A9CE-CF25937CD39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="7848" windowWidth="40428" windowHeight="22476" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="5472" yWindow="3744" windowWidth="30036" windowHeight="17352" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="359">
   <si>
     <t>ItemID</t>
   </si>
@@ -204,15 +204,9 @@
     <t>SK34A01</t>
   </si>
   <si>
-    <t>SORT</t>
-  </si>
-  <si>
     <t>Ein LKW möchte Ware am Wareneingang abliefern. Wie gehst du vor?</t>
   </si>
   <si>
-    <t>Bitte bringe die Liste in die richtige Reihenfolge.</t>
-  </si>
-  <si>
     <t>Ich überprüfe die Packstückzahl auf den Begleitpapieren.</t>
   </si>
   <si>
@@ -742,9 +736,6 @@
   </si>
   <si>
     <t>Geschenktüten</t>
-  </si>
-  <si>
-    <t>3 - 1 - 2 - 4</t>
   </si>
   <si>
     <t>Bestellverfahren anmelden</t>
@@ -1040,9 +1031,6 @@
     <t>CHOICE_AP</t>
   </si>
   <si>
-    <t>IMAGEMAP</t>
-  </si>
-  <si>
     <t>SK34A02_Karton_eingerissen.png</t>
   </si>
   <si>
@@ -1112,9 +1100,6 @@
     <t>SK34B01_Sicherheitshinweis_Schuhe.png</t>
   </si>
   <si>
-    <t xml:space="preserve">4a - 1b - 3c - 2d </t>
-  </si>
-  <si>
     <t>Bertelsmann Stiftung</t>
   </si>
   <si>
@@ -1128,6 +1113,12 @@
   </si>
   <si>
     <t>SKILL</t>
+  </si>
+  <si>
+    <t>3a - 1b - 2c - 4d</t>
+  </si>
+  <si>
+    <t>Bitte bringe die Liste in die richtige Reihenfolge durch ziehen der Antworten auf die Positionsnummer.</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1381,16 +1372,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="17">
     <dxf>
       <font>
         <b val="0"/>
@@ -1724,6 +1716,18 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="8"/>
@@ -1869,7 +1873,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}" name="Tabelle5" displayName="Tabelle5" ref="A1:BO29" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}" name="Tabelle5" displayName="Tabelle5" ref="A1:BO29" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14">
   <autoFilter ref="A1:BO29" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}"/>
   <tableColumns count="67">
     <tableColumn id="1" xr3:uid="{5027A3BA-AE24-48AB-84F1-2B75CE07B771}" name="ItemID"/>
@@ -1898,10 +1902,10 @@
     <tableColumn id="24" xr3:uid="{23F67FFD-2BC1-4D27-AD0C-B74E3C199457}" name="ScoringOption_4"/>
     <tableColumn id="19" xr3:uid="{9A785364-30D3-4C59-BCD1-D4FFEC8F1707}" name="ScoringOption_5"/>
     <tableColumn id="18" xr3:uid="{12E16906-642F-4B65-983F-E28178158A3D}" name="ScoringOption_6"/>
-    <tableColumn id="30" xr3:uid="{EEA04AEC-E395-4676-8F4F-E92FD755CDB3}" name="HTMLDistractorSecondary_1"/>
-    <tableColumn id="31" xr3:uid="{3BD60383-F0F2-4323-A646-1CB0A0F0E965}" name="HTMLDistractorSecondary_2"/>
-    <tableColumn id="32" xr3:uid="{4DFF9692-CB08-4C05-9225-A6BAFC73F4AC}" name="HTMLDistractorSecondary_3"/>
-    <tableColumn id="33" xr3:uid="{28B2B166-5249-498D-B10A-F00697BCD1DD}" name="HTMLDistractorSecondary_4"/>
+    <tableColumn id="30" xr3:uid="{EEA04AEC-E395-4676-8F4F-E92FD755CDB3}" name="HTMLDistractorSecondary_1" dataDxfId="13"/>
+    <tableColumn id="31" xr3:uid="{3BD60383-F0F2-4323-A646-1CB0A0F0E965}" name="HTMLDistractorSecondary_2" dataDxfId="12"/>
+    <tableColumn id="32" xr3:uid="{4DFF9692-CB08-4C05-9225-A6BAFC73F4AC}" name="HTMLDistractorSecondary_3" dataDxfId="11"/>
+    <tableColumn id="33" xr3:uid="{28B2B166-5249-498D-B10A-F00697BCD1DD}" name="HTMLDistractorSecondary_4" dataDxfId="10"/>
     <tableColumn id="39" xr3:uid="{A54267EF-5227-4A2B-BDED-36FA6A511406}" name="ImageMapResourceName"/>
     <tableColumn id="40" xr3:uid="{5DC7515C-E283-48F3-B632-2A8312C441C4}" name="ImageMapForm"/>
     <tableColumn id="41" xr3:uid="{46A6C32A-C01A-4C08-A9A2-67CF0A53B61D}" name="ImageMapFormDetails_1"/>
@@ -2258,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
   <dimension ref="A1:BO29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BF31" sqref="BF31"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2267,6 +2271,7 @@
     <col min="4" max="4" width="15.5546875" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.44140625" customWidth="1"/>
+    <col min="27" max="27" width="16.6640625" customWidth="1"/>
     <col min="46" max="46" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2434,43 +2439,43 @@
         <v>53</v>
       </c>
       <c r="BC1" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="BF1" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="BH1" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="BI1" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="BJ1" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="BK1" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="BO1" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="BL1" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="BM1" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="BN1" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="BO1" s="2" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.25">
@@ -2478,79 +2483,79 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" t="s">
+        <v>358</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2" t="s">
         <v>56</v>
       </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
         <v>57</v>
       </c>
-      <c r="L2">
-        <v>4</v>
-      </c>
-      <c r="N2">
-        <v>4</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="Q2" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>61</v>
-      </c>
       <c r="U2" t="s">
-        <v>356</v>
-      </c>
-      <c r="AA2">
+        <v>120</v>
+      </c>
+      <c r="AA2" s="19">
         <v>1</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="19">
         <v>2</v>
       </c>
-      <c r="AC2">
-        <v>3</v>
-      </c>
-      <c r="AD2">
+      <c r="AC2" s="19">
+        <v>3</v>
+      </c>
+      <c r="AD2" s="19">
         <v>4</v>
       </c>
       <c r="AK2">
         <v>1</v>
       </c>
       <c r="AQ2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS2">
         <v>51312</v>
       </c>
       <c r="AT2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AU2" t="s">
-        <v>64</v>
-      </c>
-      <c r="BC2" s="19" t="s">
-        <v>361</v>
+        <v>62</v>
+      </c>
+      <c r="BC2" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BD2" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="BE2" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="BF2">
         <v>20</v>
       </c>
       <c r="BI2" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="BJ2" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="BK2">
         <v>3</v>
@@ -2570,58 +2575,62 @@
     </row>
     <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D3" t="s">
         <v>65</v>
       </c>
-      <c r="C3" t="s">
-        <v>330</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" s="16" t="s">
+        <v>329</v>
+      </c>
+      <c r="J3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>333</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="P3" t="s">
         <v>68</v>
       </c>
-      <c r="L3">
-        <v>4</v>
-      </c>
-      <c r="N3">
-        <v>3</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>69</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>70</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="U3" t="s">
         <v>71</v>
       </c>
-      <c r="R3" t="s">
-        <v>72</v>
-      </c>
-      <c r="U3" t="s">
-        <v>73</v>
-      </c>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
       <c r="AK3">
         <v>1</v>
       </c>
       <c r="AQ3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS3">
         <v>51312</v>
       </c>
       <c r="AT3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AU3" t="s">
-        <v>74</v>
-      </c>
-      <c r="BC3" s="19" t="s">
-        <v>361</v>
+        <v>72</v>
+      </c>
+      <c r="BC3" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK3">
         <v>3</v>
@@ -2641,55 +2650,59 @@
     </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="P4" t="s">
         <v>76</v>
       </c>
-      <c r="J4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4">
-        <v>4</v>
-      </c>
-      <c r="N4">
-        <v>3</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>77</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>78</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="U4" t="s">
         <v>79</v>
       </c>
-      <c r="R4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U4" t="s">
-        <v>81</v>
-      </c>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
       <c r="AK4">
         <v>1</v>
       </c>
       <c r="AQ4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS4">
         <v>51312</v>
       </c>
       <c r="AT4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AU4" t="s">
-        <v>82</v>
-      </c>
-      <c r="BC4" s="19" t="s">
-        <v>361</v>
+        <v>80</v>
+      </c>
+      <c r="BC4" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK4">
         <v>3</v>
@@ -2709,17 +2722,17 @@
     </row>
     <row r="5" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F5" s="17"/>
       <c r="J5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -2728,37 +2741,41 @@
         <v>3</v>
       </c>
       <c r="O5" t="s">
+        <v>83</v>
+      </c>
+      <c r="P5" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q5" t="s">
         <v>85</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>86</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="U5" t="s">
         <v>87</v>
       </c>
-      <c r="R5" t="s">
-        <v>88</v>
-      </c>
-      <c r="U5" t="s">
-        <v>89</v>
-      </c>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
       <c r="AK5">
         <v>1</v>
       </c>
       <c r="AQ5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS5">
         <v>51312</v>
       </c>
       <c r="AT5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AU5" t="s">
-        <v>90</v>
-      </c>
-      <c r="BC5" s="19" t="s">
-        <v>361</v>
+        <v>88</v>
+      </c>
+      <c r="BC5" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK5">
         <v>3</v>
@@ -2778,58 +2795,62 @@
     </row>
     <row r="6" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>327</v>
+      </c>
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="J6" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
         <v>91</v>
       </c>
-      <c r="C6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="P6" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>355</v>
-      </c>
-      <c r="J6" t="s">
-        <v>68</v>
-      </c>
-      <c r="L6">
-        <v>4</v>
-      </c>
-      <c r="N6">
-        <v>3</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>93</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>94</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="U6" t="s">
         <v>95</v>
       </c>
-      <c r="R6" t="s">
-        <v>96</v>
-      </c>
-      <c r="U6" t="s">
-        <v>97</v>
-      </c>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
       <c r="AK6">
         <v>1</v>
       </c>
       <c r="AQ6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS6">
         <v>51312</v>
       </c>
       <c r="AT6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AU6" t="s">
-        <v>99</v>
-      </c>
-      <c r="BC6" s="19" t="s">
-        <v>361</v>
+        <v>97</v>
+      </c>
+      <c r="BC6" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK6">
         <v>3</v>
@@ -2849,58 +2870,62 @@
     </row>
     <row r="7" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>327</v>
+      </c>
+      <c r="D7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="J7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7" t="s">
         <v>100</v>
       </c>
-      <c r="C7" t="s">
-        <v>330</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="P7" t="s">
         <v>101</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>334</v>
-      </c>
-      <c r="J7" t="s">
-        <v>68</v>
-      </c>
-      <c r="L7">
-        <v>4</v>
-      </c>
-      <c r="N7">
-        <v>3</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>102</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>103</v>
       </c>
-      <c r="Q7" t="s">
-        <v>104</v>
-      </c>
-      <c r="R7" t="s">
-        <v>105</v>
-      </c>
       <c r="U7" t="s">
-        <v>81</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="19"/>
       <c r="AK7">
         <v>1</v>
       </c>
       <c r="AQ7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS7">
         <v>51312</v>
       </c>
       <c r="AT7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AU7" t="s">
-        <v>106</v>
-      </c>
-      <c r="BC7" s="19" t="s">
-        <v>361</v>
+        <v>104</v>
+      </c>
+      <c r="BC7" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK7">
         <v>3</v>
@@ -2920,16 +2945,16 @@
     </row>
     <row r="8" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L8">
         <v>4</v>
@@ -2938,37 +2963,41 @@
         <v>3</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="P8" s="16" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="Q8" s="16" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="R8" s="16" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="U8" t="s">
-        <v>89</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="19"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="19"/>
       <c r="AK8">
         <v>1</v>
       </c>
       <c r="AQ8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS8">
         <v>51312</v>
       </c>
       <c r="AT8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AU8" t="s">
-        <v>109</v>
-      </c>
-      <c r="BC8" s="19" t="s">
-        <v>361</v>
+        <v>107</v>
+      </c>
+      <c r="BC8" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK8">
         <v>3</v>
@@ -2988,58 +3017,62 @@
     </row>
     <row r="9" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" t="s">
+        <v>327</v>
+      </c>
+      <c r="D9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>331</v>
+      </c>
+      <c r="J9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9" t="s">
         <v>110</v>
       </c>
-      <c r="C9" t="s">
-        <v>330</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="P9" t="s">
         <v>111</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>335</v>
-      </c>
-      <c r="J9" t="s">
-        <v>68</v>
-      </c>
-      <c r="L9">
-        <v>4</v>
-      </c>
-      <c r="N9">
-        <v>3</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>112</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>113</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="U9" t="s">
         <v>114</v>
       </c>
-      <c r="R9" t="s">
-        <v>115</v>
-      </c>
-      <c r="U9" t="s">
-        <v>116</v>
-      </c>
+      <c r="AA9" s="19"/>
+      <c r="AB9" s="19"/>
+      <c r="AC9" s="19"/>
+      <c r="AD9" s="19"/>
       <c r="AK9">
         <v>1</v>
       </c>
       <c r="AQ9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS9">
         <v>51312</v>
       </c>
       <c r="AT9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AU9" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC9" s="19" t="s">
-        <v>361</v>
+        <v>115</v>
+      </c>
+      <c r="BC9" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK9">
         <v>3</v>
@@ -3059,67 +3092,67 @@
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" t="s">
         <v>118</v>
       </c>
-      <c r="C10" t="s">
+      <c r="J10" t="s">
         <v>119</v>
       </c>
-      <c r="D10" t="s">
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10" t="s">
+        <v>121</v>
+      </c>
+      <c r="P10" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>123</v>
+      </c>
+      <c r="R10" t="s">
+        <v>124</v>
+      </c>
+      <c r="U10" t="s">
         <v>120</v>
       </c>
-      <c r="J10" t="s">
-        <v>121</v>
-      </c>
-      <c r="L10">
-        <v>4</v>
-      </c>
-      <c r="N10">
-        <v>4</v>
-      </c>
-      <c r="O10" t="s">
-        <v>123</v>
-      </c>
-      <c r="P10" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>125</v>
-      </c>
-      <c r="R10" t="s">
-        <v>126</v>
-      </c>
-      <c r="U10" t="s">
-        <v>122</v>
-      </c>
-      <c r="AA10" s="18" t="s">
+      <c r="AA10" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="AB10" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="AC10" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="AD10" s="20" t="s">
         <v>315</v>
-      </c>
-      <c r="AB10" s="18" t="s">
-        <v>316</v>
-      </c>
-      <c r="AC10" s="18" t="s">
-        <v>317</v>
-      </c>
-      <c r="AD10" s="18" t="s">
-        <v>318</v>
       </c>
       <c r="AK10">
         <v>1</v>
       </c>
       <c r="AQ10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS10">
         <v>51312</v>
       </c>
       <c r="AT10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AU10" t="s">
-        <v>128</v>
-      </c>
-      <c r="BC10" s="19" t="s">
-        <v>361</v>
+        <v>126</v>
+      </c>
+      <c r="BC10" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK10">
         <v>3</v>
@@ -3128,10 +3161,10 @@
         <v>2</v>
       </c>
       <c r="BM10">
+        <v>4</v>
+      </c>
+      <c r="BN10">
         <v>0</v>
-      </c>
-      <c r="BN10">
-        <v>4</v>
       </c>
       <c r="BO10">
         <v>4</v>
@@ -3139,55 +3172,59 @@
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>128</v>
+      </c>
+      <c r="J11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11" t="s">
+        <v>308</v>
+      </c>
+      <c r="P11" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>310</v>
+      </c>
+      <c r="R11" t="s">
+        <v>311</v>
+      </c>
+      <c r="U11" t="s">
         <v>129</v>
       </c>
-      <c r="C11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" t="s">
-        <v>130</v>
-      </c>
-      <c r="J11" t="s">
-        <v>68</v>
-      </c>
-      <c r="L11">
-        <v>4</v>
-      </c>
-      <c r="N11">
-        <v>3</v>
-      </c>
-      <c r="O11" t="s">
-        <v>311</v>
-      </c>
-      <c r="P11" t="s">
-        <v>312</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>313</v>
-      </c>
-      <c r="R11" t="s">
-        <v>314</v>
-      </c>
-      <c r="U11" t="s">
-        <v>131</v>
-      </c>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="19"/>
       <c r="AK11">
         <v>1</v>
       </c>
       <c r="AQ11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS11">
         <v>51312</v>
       </c>
       <c r="AT11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AU11" t="s">
-        <v>128</v>
-      </c>
-      <c r="BC11" s="19" t="s">
-        <v>361</v>
+        <v>126</v>
+      </c>
+      <c r="BC11" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK11">
         <v>3</v>
@@ -3207,55 +3244,59 @@
     </row>
     <row r="12" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" t="s">
+        <v>327</v>
+      </c>
+      <c r="D12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>332</v>
+      </c>
+      <c r="J12" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12" t="s">
         <v>132</v>
       </c>
-      <c r="C12" t="s">
-        <v>330</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="P12" t="s">
         <v>133</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="J12" t="s">
-        <v>68</v>
-      </c>
-      <c r="L12">
-        <v>4</v>
-      </c>
-      <c r="N12">
-        <v>3</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>134</v>
       </c>
-      <c r="P12" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>136</v>
-      </c>
       <c r="U12" t="s">
-        <v>116</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="19"/>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="19"/>
       <c r="AK12">
         <v>1</v>
       </c>
       <c r="AQ12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS12">
         <v>51312</v>
       </c>
       <c r="AT12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AU12" t="s">
-        <v>137</v>
-      </c>
-      <c r="BC12" s="19" t="s">
-        <v>361</v>
+        <v>135</v>
+      </c>
+      <c r="BC12" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK12">
         <v>3</v>
@@ -3275,55 +3316,59 @@
     </row>
     <row r="13" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+      <c r="J13" t="s">
+        <v>66</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13" t="s">
         <v>138</v>
       </c>
-      <c r="C13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="P13" t="s">
         <v>139</v>
       </c>
-      <c r="J13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L13">
-        <v>4</v>
-      </c>
-      <c r="N13">
-        <v>3</v>
-      </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>140</v>
       </c>
-      <c r="P13" t="s">
+      <c r="R13" t="s">
         <v>141</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="U13" t="s">
         <v>142</v>
       </c>
-      <c r="R13" t="s">
-        <v>143</v>
-      </c>
-      <c r="U13" t="s">
-        <v>144</v>
-      </c>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="19"/>
       <c r="AK13">
         <v>1</v>
       </c>
       <c r="AQ13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS13">
         <v>51312</v>
       </c>
       <c r="AT13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AU13" t="s">
-        <v>145</v>
-      </c>
-      <c r="BC13" s="19" t="s">
-        <v>361</v>
+        <v>143</v>
+      </c>
+      <c r="BC13" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK13">
         <v>3</v>
@@ -3343,55 +3388,59 @@
     </row>
     <row r="14" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>145</v>
+      </c>
+      <c r="J14" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14" t="s">
         <v>146</v>
       </c>
-      <c r="C14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="P14" t="s">
         <v>147</v>
       </c>
-      <c r="J14" t="s">
-        <v>68</v>
-      </c>
-      <c r="L14">
-        <v>4</v>
-      </c>
-      <c r="N14">
-        <v>3</v>
-      </c>
-      <c r="O14" t="s">
+      <c r="Q14" t="s">
         <v>148</v>
       </c>
-      <c r="P14" t="s">
+      <c r="R14" t="s">
         <v>149</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="U14" t="s">
         <v>150</v>
       </c>
-      <c r="R14" t="s">
-        <v>151</v>
-      </c>
-      <c r="U14" t="s">
-        <v>152</v>
-      </c>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
       <c r="AK14">
         <v>1</v>
       </c>
       <c r="AQ14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS14">
         <v>51312</v>
       </c>
       <c r="AT14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AU14" t="s">
-        <v>154</v>
-      </c>
-      <c r="BC14" s="19" t="s">
-        <v>361</v>
+        <v>152</v>
+      </c>
+      <c r="BC14" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK14">
         <v>2</v>
@@ -3411,55 +3460,59 @@
     </row>
     <row r="15" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>154</v>
+      </c>
+      <c r="J15" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+      <c r="O15" t="s">
         <v>155</v>
       </c>
-      <c r="C15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="P15" t="s">
         <v>156</v>
       </c>
-      <c r="J15" t="s">
-        <v>68</v>
-      </c>
-      <c r="L15">
-        <v>4</v>
-      </c>
-      <c r="N15">
-        <v>3</v>
-      </c>
-      <c r="O15" t="s">
+      <c r="Q15" t="s">
         <v>157</v>
       </c>
-      <c r="P15" t="s">
+      <c r="R15" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="Q15" t="s">
-        <v>159</v>
-      </c>
-      <c r="R15" s="16" t="s">
-        <v>160</v>
-      </c>
       <c r="U15" t="s">
-        <v>152</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
       <c r="AK15">
         <v>1</v>
       </c>
       <c r="AQ15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS15">
         <v>51312</v>
       </c>
       <c r="AT15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AU15" t="s">
-        <v>161</v>
-      </c>
-      <c r="BC15" s="19" t="s">
-        <v>361</v>
+        <v>159</v>
+      </c>
+      <c r="BC15" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK15">
         <v>2</v>
@@ -3479,58 +3532,62 @@
     </row>
     <row r="16" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" t="s">
+        <v>327</v>
+      </c>
+      <c r="D16" t="s">
+        <v>161</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="J16" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
+      <c r="O16" t="s">
         <v>162</v>
       </c>
-      <c r="C16" t="s">
-        <v>332</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="P16" t="s">
         <v>163</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>337</v>
-      </c>
-      <c r="J16" t="s">
-        <v>68</v>
-      </c>
-      <c r="L16">
-        <v>4</v>
-      </c>
-      <c r="N16">
-        <v>3</v>
-      </c>
-      <c r="O16" t="s">
+      <c r="Q16" t="s">
         <v>164</v>
       </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
         <v>165</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="U16" t="s">
         <v>166</v>
       </c>
-      <c r="R16" t="s">
-        <v>167</v>
-      </c>
-      <c r="U16" t="s">
-        <v>168</v>
-      </c>
+      <c r="AA16" s="19"/>
+      <c r="AB16" s="19"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="19"/>
       <c r="AK16">
         <v>1</v>
       </c>
       <c r="AQ16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS16">
         <v>51312</v>
       </c>
       <c r="AT16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AU16" t="s">
-        <v>161</v>
-      </c>
-      <c r="BC16" s="19" t="s">
-        <v>361</v>
+        <v>159</v>
+      </c>
+      <c r="BC16" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK16">
         <v>2</v>
@@ -3550,16 +3607,16 @@
     </row>
     <row r="17" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C17" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L17">
         <v>4</v>
@@ -3568,37 +3625,41 @@
         <v>3</v>
       </c>
       <c r="O17" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="P17" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="Q17" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="R17" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="U17" s="16" t="s">
-        <v>116</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="AA17" s="19"/>
+      <c r="AB17" s="19"/>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="19"/>
       <c r="AK17">
         <v>1</v>
       </c>
       <c r="AQ17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS17">
         <v>51312</v>
       </c>
       <c r="AT17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AU17" t="s">
-        <v>172</v>
-      </c>
-      <c r="BC17" s="19" t="s">
-        <v>361</v>
+        <v>170</v>
+      </c>
+      <c r="BC17" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK17">
         <v>3</v>
@@ -3618,55 +3679,59 @@
     </row>
     <row r="18" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>172</v>
+      </c>
+      <c r="J18" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18" t="s">
         <v>173</v>
       </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="P18" t="s">
         <v>174</v>
       </c>
-      <c r="J18" t="s">
-        <v>68</v>
-      </c>
-      <c r="L18">
-        <v>4</v>
-      </c>
-      <c r="N18">
-        <v>3</v>
-      </c>
-      <c r="O18" t="s">
+      <c r="Q18" t="s">
         <v>175</v>
       </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
         <v>176</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="U18" t="s">
         <v>177</v>
       </c>
-      <c r="R18" t="s">
-        <v>178</v>
-      </c>
-      <c r="U18" t="s">
-        <v>179</v>
-      </c>
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="19"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="19"/>
       <c r="AK18">
         <v>1</v>
       </c>
       <c r="AQ18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS18">
         <v>51312</v>
       </c>
       <c r="AT18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AU18" t="s">
-        <v>180</v>
-      </c>
-      <c r="BC18" s="19" t="s">
-        <v>361</v>
+        <v>178</v>
+      </c>
+      <c r="BC18" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK18">
         <v>3</v>
@@ -3686,16 +3751,16 @@
     </row>
     <row r="19" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C19" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L19">
         <v>4</v>
@@ -3704,37 +3769,41 @@
         <v>3</v>
       </c>
       <c r="O19" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="P19" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="Q19" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="R19" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="U19" t="s">
-        <v>116</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="19"/>
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="19"/>
       <c r="AK19">
         <v>1</v>
       </c>
       <c r="AQ19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS19">
         <v>51312</v>
       </c>
       <c r="AT19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AU19" t="s">
-        <v>183</v>
-      </c>
-      <c r="BC19" s="19" t="s">
-        <v>361</v>
+        <v>181</v>
+      </c>
+      <c r="BC19" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK19">
         <v>3</v>
@@ -3754,55 +3823,59 @@
     </row>
     <row r="20" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" t="s">
+        <v>183</v>
+      </c>
+      <c r="J20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L20">
+        <v>4</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+      <c r="O20" t="s">
         <v>184</v>
       </c>
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="P20" t="s">
         <v>185</v>
       </c>
-      <c r="J20" t="s">
-        <v>68</v>
-      </c>
-      <c r="L20">
-        <v>4</v>
-      </c>
-      <c r="N20">
-        <v>3</v>
-      </c>
-      <c r="O20" t="s">
+      <c r="Q20" t="s">
         <v>186</v>
       </c>
-      <c r="P20" t="s">
+      <c r="R20" t="s">
         <v>187</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="U20" t="s">
         <v>188</v>
       </c>
-      <c r="R20" t="s">
-        <v>189</v>
-      </c>
-      <c r="U20" t="s">
-        <v>190</v>
-      </c>
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="19"/>
+      <c r="AC20" s="19"/>
+      <c r="AD20" s="19"/>
       <c r="AK20">
         <v>1</v>
       </c>
       <c r="AQ20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS20">
         <v>51312</v>
       </c>
       <c r="AT20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AU20" t="s">
-        <v>191</v>
-      </c>
-      <c r="BC20" s="19" t="s">
-        <v>361</v>
+        <v>189</v>
+      </c>
+      <c r="BC20" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK20">
         <v>3</v>
@@ -3822,17 +3895,17 @@
     </row>
     <row r="21" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F21" s="17"/>
       <c r="J21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L21">
         <v>4</v>
@@ -3841,37 +3914,41 @@
         <v>3</v>
       </c>
       <c r="O21" t="s">
+        <v>192</v>
+      </c>
+      <c r="P21" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q21" t="s">
         <v>194</v>
       </c>
-      <c r="P21" t="s">
+      <c r="R21" t="s">
         <v>195</v>
       </c>
-      <c r="Q21" t="s">
-        <v>196</v>
-      </c>
-      <c r="R21" t="s">
-        <v>197</v>
-      </c>
       <c r="U21" t="s">
-        <v>97</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="AA21" s="19"/>
+      <c r="AB21" s="19"/>
+      <c r="AC21" s="19"/>
+      <c r="AD21" s="19"/>
       <c r="AK21">
         <v>1</v>
       </c>
       <c r="AQ21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS21">
         <v>51312</v>
       </c>
       <c r="AT21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AU21" t="s">
-        <v>199</v>
-      </c>
-      <c r="BC21" s="19" t="s">
-        <v>361</v>
+        <v>197</v>
+      </c>
+      <c r="BC21" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK21">
         <v>3</v>
@@ -3891,17 +3968,17 @@
     </row>
     <row r="22" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F22" s="17"/>
       <c r="J22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L22">
         <v>4</v>
@@ -3910,37 +3987,41 @@
         <v>3</v>
       </c>
       <c r="O22" t="s">
+        <v>200</v>
+      </c>
+      <c r="P22" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q22" t="s">
         <v>202</v>
       </c>
-      <c r="P22" t="s">
+      <c r="R22" t="s">
         <v>203</v>
       </c>
-      <c r="Q22" t="s">
-        <v>204</v>
-      </c>
-      <c r="R22" t="s">
-        <v>205</v>
-      </c>
       <c r="U22" t="s">
-        <v>152</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="AA22" s="19"/>
+      <c r="AB22" s="19"/>
+      <c r="AC22" s="19"/>
+      <c r="AD22" s="19"/>
       <c r="AK22">
         <v>1</v>
       </c>
       <c r="AQ22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS22">
         <v>51312</v>
       </c>
       <c r="AT22" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AU22" t="s">
-        <v>206</v>
-      </c>
-      <c r="BC22" s="19" t="s">
-        <v>361</v>
+        <v>204</v>
+      </c>
+      <c r="BC22" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK22">
         <v>3</v>
@@ -3960,17 +4041,17 @@
     </row>
     <row r="23" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F23" s="17"/>
       <c r="J23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L23">
         <v>4</v>
@@ -3979,37 +4060,41 @@
         <v>3</v>
       </c>
       <c r="O23" t="s">
+        <v>207</v>
+      </c>
+      <c r="P23" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q23" t="s">
         <v>209</v>
       </c>
-      <c r="P23" t="s">
+      <c r="R23" t="s">
         <v>210</v>
       </c>
-      <c r="Q23" t="s">
-        <v>211</v>
-      </c>
-      <c r="R23" t="s">
-        <v>212</v>
-      </c>
       <c r="U23" t="s">
-        <v>131</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="AA23" s="19"/>
+      <c r="AB23" s="19"/>
+      <c r="AC23" s="19"/>
+      <c r="AD23" s="19"/>
       <c r="AK23">
         <v>1</v>
       </c>
       <c r="AQ23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS23">
         <v>51312</v>
       </c>
       <c r="AT23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AU23" t="s">
-        <v>213</v>
-      </c>
-      <c r="BC23" s="19" t="s">
-        <v>361</v>
+        <v>211</v>
+      </c>
+      <c r="BC23" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK23">
         <v>3</v>
@@ -4029,58 +4114,62 @@
     </row>
     <row r="24" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>212</v>
+      </c>
+      <c r="C24" t="s">
+        <v>327</v>
+      </c>
+      <c r="D24" t="s">
+        <v>213</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="J24" t="s">
+        <v>66</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="N24">
+        <v>3</v>
+      </c>
+      <c r="O24" t="s">
         <v>214</v>
       </c>
-      <c r="C24" t="s">
-        <v>330</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="P24" t="s">
         <v>215</v>
       </c>
-      <c r="F24" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="J24" t="s">
-        <v>68</v>
-      </c>
-      <c r="L24">
-        <v>4</v>
-      </c>
-      <c r="N24">
-        <v>3</v>
-      </c>
-      <c r="O24" t="s">
+      <c r="Q24" t="s">
         <v>216</v>
       </c>
-      <c r="P24" t="s">
+      <c r="R24" t="s">
         <v>217</v>
       </c>
-      <c r="Q24" t="s">
-        <v>218</v>
-      </c>
-      <c r="R24" t="s">
-        <v>219</v>
-      </c>
       <c r="U24" t="s">
-        <v>116</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="AA24" s="19"/>
+      <c r="AB24" s="19"/>
+      <c r="AC24" s="19"/>
+      <c r="AD24" s="19"/>
       <c r="AK24">
         <v>1</v>
       </c>
       <c r="AQ24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS24">
         <v>51312</v>
       </c>
       <c r="AT24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AU24" t="s">
-        <v>220</v>
-      </c>
-      <c r="BC24" s="19" t="s">
-        <v>361</v>
+        <v>218</v>
+      </c>
+      <c r="BC24" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK24">
         <v>3</v>
@@ -4100,58 +4189,62 @@
     </row>
     <row r="25" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C25" t="s">
+        <v>327</v>
+      </c>
+      <c r="D25" t="s">
+        <v>220</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="J25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25" t="s">
         <v>221</v>
       </c>
-      <c r="C25" t="s">
-        <v>330</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="P25" t="s">
         <v>222</v>
       </c>
-      <c r="F25" s="16" t="s">
-        <v>319</v>
-      </c>
-      <c r="J25" t="s">
-        <v>68</v>
-      </c>
-      <c r="L25">
-        <v>4</v>
-      </c>
-      <c r="N25">
-        <v>3</v>
-      </c>
-      <c r="O25" t="s">
+      <c r="Q25" t="s">
         <v>223</v>
       </c>
-      <c r="P25" t="s">
+      <c r="R25" t="s">
         <v>224</v>
       </c>
-      <c r="Q25" t="s">
-        <v>225</v>
-      </c>
-      <c r="R25" t="s">
-        <v>226</v>
-      </c>
       <c r="U25" t="s">
-        <v>116</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="AA25" s="19"/>
+      <c r="AB25" s="19"/>
+      <c r="AC25" s="19"/>
+      <c r="AD25" s="19"/>
       <c r="AK25">
         <v>1</v>
       </c>
       <c r="AQ25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS25">
         <v>51312</v>
       </c>
       <c r="AT25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AU25" t="s">
-        <v>228</v>
-      </c>
-      <c r="BC25" s="19" t="s">
-        <v>361</v>
+        <v>226</v>
+      </c>
+      <c r="BC25" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK25">
         <v>3</v>
@@ -4171,17 +4264,17 @@
     </row>
     <row r="26" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>117</v>
       </c>
       <c r="D26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F26" s="16"/>
       <c r="J26" t="s">
-        <v>68</v>
+        <v>358</v>
       </c>
       <c r="L26">
         <v>4</v>
@@ -4190,37 +4283,49 @@
         <v>4</v>
       </c>
       <c r="O26" t="s">
+        <v>229</v>
+      </c>
+      <c r="P26" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q26" t="s">
         <v>231</v>
       </c>
-      <c r="P26" t="s">
+      <c r="R26" t="s">
         <v>232</v>
       </c>
-      <c r="Q26" t="s">
-        <v>233</v>
-      </c>
-      <c r="R26" t="s">
-        <v>234</v>
-      </c>
       <c r="U26" t="s">
-        <v>235</v>
+        <v>357</v>
+      </c>
+      <c r="AA26" s="19">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="19">
+        <v>2</v>
+      </c>
+      <c r="AC26" s="19">
+        <v>3</v>
+      </c>
+      <c r="AD26" s="19">
+        <v>4</v>
       </c>
       <c r="AK26">
         <v>1</v>
       </c>
       <c r="AQ26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS26">
         <v>51312</v>
       </c>
       <c r="AT26" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AU26" t="s">
-        <v>236</v>
-      </c>
-      <c r="BC26" s="19" t="s">
-        <v>361</v>
+        <v>233</v>
+      </c>
+      <c r="BC26" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK26">
         <v>3</v>
@@ -4240,58 +4345,62 @@
     </row>
     <row r="27" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" t="s">
+        <v>327</v>
+      </c>
+      <c r="D27" t="s">
+        <v>235</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="J27" t="s">
+        <v>66</v>
+      </c>
+      <c r="L27">
+        <v>4</v>
+      </c>
+      <c r="N27">
+        <v>3</v>
+      </c>
+      <c r="O27" t="s">
+        <v>236</v>
+      </c>
+      <c r="P27" t="s">
         <v>237</v>
       </c>
-      <c r="C27" t="s">
-        <v>330</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="Q27" t="s">
         <v>238</v>
       </c>
-      <c r="F27" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="J27" t="s">
-        <v>68</v>
-      </c>
-      <c r="L27">
-        <v>4</v>
-      </c>
-      <c r="N27">
-        <v>3</v>
-      </c>
-      <c r="O27" t="s">
+      <c r="R27" t="s">
         <v>239</v>
       </c>
-      <c r="P27" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>241</v>
-      </c>
-      <c r="R27" t="s">
-        <v>242</v>
-      </c>
       <c r="U27" t="s">
-        <v>131</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="AA27" s="19"/>
+      <c r="AB27" s="19"/>
+      <c r="AC27" s="19"/>
+      <c r="AD27" s="19"/>
       <c r="AK27">
         <v>1</v>
       </c>
       <c r="AQ27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS27">
         <v>51312</v>
       </c>
       <c r="AT27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AU27" t="s">
-        <v>243</v>
-      </c>
-      <c r="BC27" s="19" t="s">
-        <v>361</v>
+        <v>240</v>
+      </c>
+      <c r="BC27" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK27">
         <v>3</v>
@@ -4311,17 +4420,17 @@
     </row>
     <row r="28" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F28" s="17"/>
       <c r="J28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L28">
         <v>4</v>
@@ -4330,37 +4439,41 @@
         <v>3</v>
       </c>
       <c r="O28" t="s">
+        <v>243</v>
+      </c>
+      <c r="P28" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>245</v>
+      </c>
+      <c r="R28" t="s">
         <v>246</v>
       </c>
-      <c r="P28" t="s">
-        <v>247</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>248</v>
-      </c>
-      <c r="R28" t="s">
-        <v>249</v>
-      </c>
       <c r="U28" t="s">
-        <v>152</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="19"/>
+      <c r="AC28" s="19"/>
+      <c r="AD28" s="19"/>
       <c r="AK28">
         <v>1</v>
       </c>
       <c r="AQ28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS28">
         <v>51312</v>
       </c>
       <c r="AT28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AU28" t="s">
-        <v>250</v>
-      </c>
-      <c r="BC28" s="19" t="s">
-        <v>361</v>
+        <v>247</v>
+      </c>
+      <c r="BC28" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK28">
         <v>3</v>
@@ -4380,17 +4493,17 @@
     </row>
     <row r="29" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F29" s="17"/>
       <c r="J29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L29">
         <v>4</v>
@@ -4399,37 +4512,41 @@
         <v>3</v>
       </c>
       <c r="O29" t="s">
+        <v>250</v>
+      </c>
+      <c r="P29" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>252</v>
+      </c>
+      <c r="R29" t="s">
         <v>253</v>
       </c>
-      <c r="P29" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>255</v>
-      </c>
-      <c r="R29" t="s">
-        <v>256</v>
-      </c>
       <c r="U29" t="s">
-        <v>190</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="19"/>
+      <c r="AC29" s="19"/>
+      <c r="AD29" s="19"/>
       <c r="AK29">
         <v>1</v>
       </c>
       <c r="AQ29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="AS29">
         <v>51312</v>
       </c>
       <c r="AT29" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AU29" t="s">
-        <v>257</v>
-      </c>
-      <c r="BC29" s="19" t="s">
-        <v>361</v>
+        <v>254</v>
+      </c>
+      <c r="BC29" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="BK29">
         <v>3</v>
@@ -4478,72 +4595,72 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>261</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" s="7">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="B3" s="7">
-        <v>4</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="F3" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>267</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="10"/>
       <c r="F4" s="6"/>
       <c r="G4" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="10"/>
@@ -4553,7 +4670,7 @@
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="10"/>
@@ -4561,30 +4678,30 @@
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B7" s="8">
         <v>4</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -4594,7 +4711,7 @@
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -4604,7 +4721,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -4612,19 +4729,19 @@
     </row>
     <row r="11" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B11" s="7">
         <v>4</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F11" s="6"/>
     </row>
@@ -4632,7 +4749,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -4642,7 +4759,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -4650,19 +4767,19 @@
     </row>
     <row r="14" spans="1:7" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="B14" s="8">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>287</v>
-      </c>
-      <c r="B14" s="8">
-        <v>3</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>290</v>
       </c>
       <c r="F14" s="6"/>
     </row>
@@ -4670,7 +4787,7 @@
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
@@ -4678,19 +4795,19 @@
     </row>
     <row r="16" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B16" s="7">
         <v>4</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F16" s="6"/>
     </row>
@@ -4698,7 +4815,7 @@
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -4708,7 +4825,7 @@
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -4718,7 +4835,7 @@
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -4726,29 +4843,29 @@
     </row>
     <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B20" s="8">
+        <v>4</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>298</v>
-      </c>
-      <c r="B20" s="8">
-        <v>4</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -4758,7 +4875,7 @@
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -4768,7 +4885,7 @@
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -4776,19 +4893,19 @@
     </row>
     <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B24" s="7">
         <v>5</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F24" s="6"/>
     </row>
@@ -4796,7 +4913,7 @@
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -4806,7 +4923,7 @@
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -4816,7 +4933,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -4826,7 +4943,7 @@
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -4852,17 +4969,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100879B58D3C23DCA4AAEF47596CA4D8E48" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee8b9d8723b80ccc4cb578ffd4faacc7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02625a54-df84-4a3b-b049-0bb7e92cde0d" xmlns:ns3="c90f9e10-81f0-426e-b8bb-fc89022b3796" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64b8ed4db9a6e136c161da669116b9cc" ns2:_="" ns3:_="">
     <xsd:import namespace="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
@@ -5071,6 +5177,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5081,23 +5198,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5116,6 +5216,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed Issue on Terms Fixed Issue on Imprint Fixed Excel Booklet
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C647EEB-F157-4E16-A9CE-CF25937CD39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31671FE-BD64-4A77-9C5D-0D433B2C26F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5472" yWindow="3744" windowWidth="30036" windowHeight="17352" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="-96" yWindow="1260" windowWidth="26112" windowHeight="17352" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="359">
   <si>
     <t>ItemID</t>
   </si>
@@ -1100,9 +1100,6 @@
     <t>SK34B01_Sicherheitshinweis_Schuhe.png</t>
   </si>
   <si>
-    <t>Bertelsmann Stiftung</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test Fachkraft Lagerlogistik (Fachlagerist) </t>
   </si>
   <si>
@@ -1119,6 +1116,9 @@
   </si>
   <si>
     <t>Bitte bringe die Liste in die richtige Reihenfolge durch ziehen der Antworten auf die Positionsnummer.</t>
+  </si>
+  <si>
+    <t>Apollo App</t>
   </si>
 </sst>
 </file>
@@ -2262,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
   <dimension ref="A1:BO29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BI2" sqref="BI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2489,7 +2489,7 @@
         <v>55</v>
       </c>
       <c r="J2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L2">
         <v>4</v>
@@ -2540,22 +2540,22 @@
         <v>62</v>
       </c>
       <c r="BC2" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="BD2" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE2" t="s">
         <v>354</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>355</v>
       </c>
       <c r="BF2">
         <v>20</v>
       </c>
       <c r="BI2" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ2" t="s">
         <v>352</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>353</v>
       </c>
       <c r="BK2">
         <v>3</v>
@@ -2630,7 +2630,13 @@
         <v>72</v>
       </c>
       <c r="BC3" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>352</v>
       </c>
       <c r="BK3">
         <v>3</v>
@@ -2702,7 +2708,13 @@
         <v>80</v>
       </c>
       <c r="BC4" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>352</v>
       </c>
       <c r="BK4">
         <v>3</v>
@@ -2775,7 +2787,13 @@
         <v>88</v>
       </c>
       <c r="BC5" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>352</v>
       </c>
       <c r="BK5">
         <v>3</v>
@@ -2850,7 +2868,13 @@
         <v>97</v>
       </c>
       <c r="BC6" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>352</v>
       </c>
       <c r="BK6">
         <v>3</v>
@@ -2925,7 +2949,13 @@
         <v>104</v>
       </c>
       <c r="BC7" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ7" t="s">
+        <v>352</v>
       </c>
       <c r="BK7">
         <v>3</v>
@@ -2997,7 +3027,13 @@
         <v>107</v>
       </c>
       <c r="BC8" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI8" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ8" t="s">
+        <v>352</v>
       </c>
       <c r="BK8">
         <v>3</v>
@@ -3072,7 +3108,13 @@
         <v>115</v>
       </c>
       <c r="BC9" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ9" t="s">
+        <v>352</v>
       </c>
       <c r="BK9">
         <v>3</v>
@@ -3152,7 +3194,13 @@
         <v>126</v>
       </c>
       <c r="BC10" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI10" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>352</v>
       </c>
       <c r="BK10">
         <v>3</v>
@@ -3224,7 +3272,13 @@
         <v>126</v>
       </c>
       <c r="BC11" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI11" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ11" t="s">
+        <v>352</v>
       </c>
       <c r="BK11">
         <v>3</v>
@@ -3296,7 +3350,13 @@
         <v>135</v>
       </c>
       <c r="BC12" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI12" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ12" t="s">
+        <v>352</v>
       </c>
       <c r="BK12">
         <v>3</v>
@@ -3368,7 +3428,13 @@
         <v>143</v>
       </c>
       <c r="BC13" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI13" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ13" t="s">
+        <v>352</v>
       </c>
       <c r="BK13">
         <v>3</v>
@@ -3440,7 +3506,13 @@
         <v>152</v>
       </c>
       <c r="BC14" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI14" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ14" t="s">
+        <v>352</v>
       </c>
       <c r="BK14">
         <v>2</v>
@@ -3512,7 +3584,13 @@
         <v>159</v>
       </c>
       <c r="BC15" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI15" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ15" t="s">
+        <v>352</v>
       </c>
       <c r="BK15">
         <v>2</v>
@@ -3587,7 +3665,13 @@
         <v>159</v>
       </c>
       <c r="BC16" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI16" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ16" t="s">
+        <v>352</v>
       </c>
       <c r="BK16">
         <v>2</v>
@@ -3659,7 +3743,13 @@
         <v>170</v>
       </c>
       <c r="BC17" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI17" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ17" t="s">
+        <v>352</v>
       </c>
       <c r="BK17">
         <v>3</v>
@@ -3731,7 +3821,13 @@
         <v>178</v>
       </c>
       <c r="BC18" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI18" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ18" t="s">
+        <v>352</v>
       </c>
       <c r="BK18">
         <v>3</v>
@@ -3803,7 +3899,13 @@
         <v>181</v>
       </c>
       <c r="BC19" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI19" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ19" t="s">
+        <v>352</v>
       </c>
       <c r="BK19">
         <v>3</v>
@@ -3875,7 +3977,13 @@
         <v>189</v>
       </c>
       <c r="BC20" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI20" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ20" t="s">
+        <v>352</v>
       </c>
       <c r="BK20">
         <v>3</v>
@@ -3948,7 +4056,13 @@
         <v>197</v>
       </c>
       <c r="BC21" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI21" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ21" t="s">
+        <v>352</v>
       </c>
       <c r="BK21">
         <v>3</v>
@@ -4021,7 +4135,13 @@
         <v>204</v>
       </c>
       <c r="BC22" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI22" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ22" t="s">
+        <v>352</v>
       </c>
       <c r="BK22">
         <v>3</v>
@@ -4094,7 +4214,13 @@
         <v>211</v>
       </c>
       <c r="BC23" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI23" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ23" t="s">
+        <v>352</v>
       </c>
       <c r="BK23">
         <v>3</v>
@@ -4169,7 +4295,13 @@
         <v>218</v>
       </c>
       <c r="BC24" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI24" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ24" t="s">
+        <v>352</v>
       </c>
       <c r="BK24">
         <v>3</v>
@@ -4244,7 +4376,13 @@
         <v>226</v>
       </c>
       <c r="BC25" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI25" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ25" t="s">
+        <v>352</v>
       </c>
       <c r="BK25">
         <v>3</v>
@@ -4274,7 +4412,7 @@
       </c>
       <c r="F26" s="16"/>
       <c r="J26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L26">
         <v>4</v>
@@ -4295,7 +4433,7 @@
         <v>232</v>
       </c>
       <c r="U26" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AA26" s="19">
         <v>1</v>
@@ -4325,7 +4463,13 @@
         <v>233</v>
       </c>
       <c r="BC26" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ26" t="s">
+        <v>352</v>
       </c>
       <c r="BK26">
         <v>3</v>
@@ -4400,7 +4544,13 @@
         <v>240</v>
       </c>
       <c r="BC27" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI27" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ27" t="s">
+        <v>352</v>
       </c>
       <c r="BK27">
         <v>3</v>
@@ -4473,7 +4623,13 @@
         <v>247</v>
       </c>
       <c r="BC28" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI28" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ28" t="s">
+        <v>352</v>
       </c>
       <c r="BK28">
         <v>3</v>
@@ -4546,7 +4702,13 @@
         <v>254</v>
       </c>
       <c r="BC29" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
+      </c>
+      <c r="BI29" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ29" t="s">
+        <v>352</v>
       </c>
       <c r="BK29">
         <v>3</v>
@@ -4969,6 +5131,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100879B58D3C23DCA4AAEF47596CA4D8E48" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee8b9d8723b80ccc4cb578ffd4faacc7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02625a54-df84-4a3b-b049-0bb7e92cde0d" xmlns:ns3="c90f9e10-81f0-426e-b8bb-fc89022b3796" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64b8ed4db9a6e136c161da669116b9cc" ns2:_="" ns3:_="">
     <xsd:import namespace="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
@@ -5177,17 +5350,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5198,6 +5360,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5216,23 +5395,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fake Assessments Teil 1
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanaBoscolo\source\repos\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF3A7E9-830E-4DDE-A00E-0E028B6B4BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B561EE3A-4D0F-4361-98C8-BC0114C7CD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27420" yWindow="5115" windowWidth="23820" windowHeight="19830" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="392">
   <si>
     <t>ItemID</t>
   </si>
@@ -1128,6 +1128,96 @@
   </si>
   <si>
     <t>UseCaseId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testfrage? </t>
+  </si>
+  <si>
+    <t>Antwort 1</t>
+  </si>
+  <si>
+    <t>Antwort 2</t>
+  </si>
+  <si>
+    <t>Antwort 3</t>
+  </si>
+  <si>
+    <t>Antwort 4</t>
+  </si>
+  <si>
+    <t>Kaufmann/Kauffrau im E-Commerce</t>
+  </si>
+  <si>
+    <t>Test Kaufmann/Kauffrau im E-Commerce</t>
+  </si>
+  <si>
+    <t>SKUC200A01</t>
+  </si>
+  <si>
+    <t>SKUC200B01</t>
+  </si>
+  <si>
+    <t>SKUC200D01</t>
+  </si>
+  <si>
+    <t>SKUC200A02</t>
+  </si>
+  <si>
+    <t>SKUC200A03</t>
+  </si>
+  <si>
+    <t>SKUC200A04</t>
+  </si>
+  <si>
+    <t>SKUC200A05</t>
+  </si>
+  <si>
+    <t>SKUC200B02</t>
+  </si>
+  <si>
+    <t>SKUC200B03</t>
+  </si>
+  <si>
+    <t>SKUC200B04</t>
+  </si>
+  <si>
+    <t>SKUC200B05</t>
+  </si>
+  <si>
+    <t>SKUC200C01</t>
+  </si>
+  <si>
+    <t>SKUC200C02</t>
+  </si>
+  <si>
+    <t>SKUC200C03</t>
+  </si>
+  <si>
+    <t>SKUC200C04</t>
+  </si>
+  <si>
+    <t>SKUC200D02</t>
+  </si>
+  <si>
+    <t>SKUC200D03</t>
+  </si>
+  <si>
+    <t>SKUC200D04</t>
+  </si>
+  <si>
+    <t>Warenwirtschaftliche Prozesse im Onlinehandel durchführen</t>
+  </si>
+  <si>
+    <t>Mit Kunden im Onlinehandel kommunizieren</t>
+  </si>
+  <si>
+    <t>Verkaufsfördernde Maßnahmen im Onlinehandel durchführen</t>
+  </si>
+  <si>
+    <t>Onlineaktivitäten kaufmännisch steuern und kontrollieren</t>
+  </si>
+  <si>
+    <t>Im Onlinehandel projektorientiert arbeiten</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1299,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1286,6 +1376,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -1380,7 +1476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1435,6 +1531,13 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2327,14 +2430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
-  <dimension ref="A1:BR29"/>
+  <dimension ref="A1:BR51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="BI2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AR1" sqref="AR1"/>
-      <selection pane="topRight" activeCell="AV1" sqref="AV1"/>
-      <selection pane="bottomLeft" activeCell="AR2" sqref="AR2"/>
-      <selection pane="bottomRight" activeCell="BQ1" sqref="BQ1:BQ1048576"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AU30" sqref="AU30:AU51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5057,6 +5156,2140 @@
       </c>
       <c r="BR29" s="27">
         <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="C30" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F30" s="29"/>
+      <c r="J30" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L30" s="26">
+        <v>4</v>
+      </c>
+      <c r="N30" s="26">
+        <v>3</v>
+      </c>
+      <c r="O30" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P30" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q30" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R30" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U30" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA30" s="30"/>
+      <c r="AB30" s="30"/>
+      <c r="AC30" s="30"/>
+      <c r="AD30" s="30"/>
+      <c r="AK30" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ30" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS30" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT30" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="AU30" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="BC30" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD30" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE30" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF30" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI30" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ30" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK30" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL30" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM30" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN30" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO30" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP30" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ30" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR30" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="26" t="s">
+        <v>372</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F31" s="29"/>
+      <c r="J31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L31" s="26">
+        <v>4</v>
+      </c>
+      <c r="N31" s="26">
+        <v>3</v>
+      </c>
+      <c r="O31" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P31" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q31" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R31" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U31" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA31" s="30"/>
+      <c r="AB31" s="30"/>
+      <c r="AC31" s="30"/>
+      <c r="AD31" s="30"/>
+      <c r="AK31" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ31" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS31" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT31" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="AU31" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="BC31" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD31" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE31" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF31" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI31" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ31" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK31" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL31" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM31" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN31" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO31" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP31" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ31" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR31" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="26" t="s">
+        <v>373</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F32" s="29"/>
+      <c r="J32" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L32" s="26">
+        <v>4</v>
+      </c>
+      <c r="N32" s="26">
+        <v>3</v>
+      </c>
+      <c r="O32" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P32" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q32" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R32" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U32" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA32" s="30"/>
+      <c r="AB32" s="30"/>
+      <c r="AC32" s="30"/>
+      <c r="AD32" s="30"/>
+      <c r="AK32" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ32" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS32" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT32" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="AU32" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="BC32" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD32" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE32" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF32" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI32" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ32" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK32" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL32" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM32" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN32" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO32" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP32" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ32" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR32" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F33" s="29"/>
+      <c r="J33" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L33" s="26">
+        <v>4</v>
+      </c>
+      <c r="N33" s="26">
+        <v>3</v>
+      </c>
+      <c r="O33" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P33" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q33" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R33" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U33" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA33" s="30"/>
+      <c r="AB33" s="30"/>
+      <c r="AC33" s="30"/>
+      <c r="AD33" s="30"/>
+      <c r="AK33" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ33" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS33" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT33" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="AU33" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="BC33" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD33" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE33" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF33" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI33" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ33" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK33" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL33" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM33" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN33" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO33" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP33" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ33" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR33" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F34" s="29"/>
+      <c r="J34" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L34" s="26">
+        <v>4</v>
+      </c>
+      <c r="N34" s="26">
+        <v>3</v>
+      </c>
+      <c r="O34" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P34" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q34" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R34" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U34" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA34" s="30"/>
+      <c r="AB34" s="30"/>
+      <c r="AC34" s="30"/>
+      <c r="AD34" s="30"/>
+      <c r="AK34" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ34" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS34" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT34" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="AU34" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="BC34" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD34" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE34" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF34" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI34" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ34" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK34" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL34" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM34" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN34" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO34" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP34" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ34" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR34" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>370</v>
+      </c>
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="s">
+        <v>362</v>
+      </c>
+      <c r="F35" s="17"/>
+      <c r="J35" t="s">
+        <v>66</v>
+      </c>
+      <c r="L35">
+        <v>4</v>
+      </c>
+      <c r="N35">
+        <v>3</v>
+      </c>
+      <c r="O35" t="s">
+        <v>363</v>
+      </c>
+      <c r="P35" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>365</v>
+      </c>
+      <c r="R35" t="s">
+        <v>366</v>
+      </c>
+      <c r="U35" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA35" s="19"/>
+      <c r="AB35" s="19"/>
+      <c r="AC35" s="19"/>
+      <c r="AD35" s="19"/>
+      <c r="AK35">
+        <v>1</v>
+      </c>
+      <c r="AQ35" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS35">
+        <v>0</v>
+      </c>
+      <c r="AT35" t="s">
+        <v>388</v>
+      </c>
+      <c r="AU35" t="s">
+        <v>388</v>
+      </c>
+      <c r="BC35" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD35" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE35" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF35" s="28">
+        <v>20</v>
+      </c>
+      <c r="BI35" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ35" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK35">
+        <v>0</v>
+      </c>
+      <c r="BL35" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BM35">
+        <v>0</v>
+      </c>
+      <c r="BN35">
+        <v>0</v>
+      </c>
+      <c r="BO35">
+        <v>0</v>
+      </c>
+      <c r="BP35">
+        <v>2</v>
+      </c>
+      <c r="BQ35" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BR35" s="27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>376</v>
+      </c>
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" t="s">
+        <v>362</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="J36" t="s">
+        <v>66</v>
+      </c>
+      <c r="L36">
+        <v>4</v>
+      </c>
+      <c r="N36">
+        <v>3</v>
+      </c>
+      <c r="O36" t="s">
+        <v>363</v>
+      </c>
+      <c r="P36" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>365</v>
+      </c>
+      <c r="R36" t="s">
+        <v>366</v>
+      </c>
+      <c r="U36" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA36" s="19"/>
+      <c r="AB36" s="19"/>
+      <c r="AC36" s="19"/>
+      <c r="AD36" s="19"/>
+      <c r="AK36">
+        <v>1</v>
+      </c>
+      <c r="AQ36" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS36">
+        <v>0</v>
+      </c>
+      <c r="AT36" t="s">
+        <v>388</v>
+      </c>
+      <c r="AU36" t="s">
+        <v>388</v>
+      </c>
+      <c r="BC36" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD36" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE36" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF36" s="28">
+        <v>20</v>
+      </c>
+      <c r="BI36" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ36" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK36">
+        <v>0</v>
+      </c>
+      <c r="BL36" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BM36">
+        <v>0</v>
+      </c>
+      <c r="BN36">
+        <v>0</v>
+      </c>
+      <c r="BO36">
+        <v>0</v>
+      </c>
+      <c r="BP36">
+        <v>2</v>
+      </c>
+      <c r="BQ36" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BR36" s="27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>377</v>
+      </c>
+      <c r="C37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" t="s">
+        <v>362</v>
+      </c>
+      <c r="F37" s="17"/>
+      <c r="J37" t="s">
+        <v>66</v>
+      </c>
+      <c r="L37">
+        <v>4</v>
+      </c>
+      <c r="N37">
+        <v>3</v>
+      </c>
+      <c r="O37" t="s">
+        <v>363</v>
+      </c>
+      <c r="P37" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>365</v>
+      </c>
+      <c r="R37" t="s">
+        <v>366</v>
+      </c>
+      <c r="U37" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA37" s="19"/>
+      <c r="AB37" s="19"/>
+      <c r="AC37" s="19"/>
+      <c r="AD37" s="19"/>
+      <c r="AK37">
+        <v>1</v>
+      </c>
+      <c r="AQ37" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS37">
+        <v>0</v>
+      </c>
+      <c r="AT37" t="s">
+        <v>388</v>
+      </c>
+      <c r="AU37" t="s">
+        <v>388</v>
+      </c>
+      <c r="BC37" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD37" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE37" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF37" s="28">
+        <v>20</v>
+      </c>
+      <c r="BI37" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ37" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK37">
+        <v>0</v>
+      </c>
+      <c r="BL37" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BM37">
+        <v>0</v>
+      </c>
+      <c r="BN37">
+        <v>0</v>
+      </c>
+      <c r="BO37">
+        <v>0</v>
+      </c>
+      <c r="BP37">
+        <v>2</v>
+      </c>
+      <c r="BQ37" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BR37" s="27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>378</v>
+      </c>
+      <c r="C38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" t="s">
+        <v>362</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="J38" t="s">
+        <v>66</v>
+      </c>
+      <c r="L38">
+        <v>4</v>
+      </c>
+      <c r="N38">
+        <v>3</v>
+      </c>
+      <c r="O38" t="s">
+        <v>363</v>
+      </c>
+      <c r="P38" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>365</v>
+      </c>
+      <c r="R38" t="s">
+        <v>366</v>
+      </c>
+      <c r="U38" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA38" s="19"/>
+      <c r="AB38" s="19"/>
+      <c r="AC38" s="19"/>
+      <c r="AD38" s="19"/>
+      <c r="AK38">
+        <v>1</v>
+      </c>
+      <c r="AQ38" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS38">
+        <v>0</v>
+      </c>
+      <c r="AT38" t="s">
+        <v>388</v>
+      </c>
+      <c r="AU38" t="s">
+        <v>388</v>
+      </c>
+      <c r="BC38" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD38" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE38" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF38" s="28">
+        <v>20</v>
+      </c>
+      <c r="BI38" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ38" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK38">
+        <v>0</v>
+      </c>
+      <c r="BL38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BM38">
+        <v>0</v>
+      </c>
+      <c r="BN38">
+        <v>0</v>
+      </c>
+      <c r="BO38">
+        <v>0</v>
+      </c>
+      <c r="BP38">
+        <v>2</v>
+      </c>
+      <c r="BQ38" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BR38" s="27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>379</v>
+      </c>
+      <c r="C39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" t="s">
+        <v>362</v>
+      </c>
+      <c r="F39" s="17"/>
+      <c r="J39" t="s">
+        <v>66</v>
+      </c>
+      <c r="L39">
+        <v>4</v>
+      </c>
+      <c r="N39">
+        <v>3</v>
+      </c>
+      <c r="O39" t="s">
+        <v>363</v>
+      </c>
+      <c r="P39" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>365</v>
+      </c>
+      <c r="R39" t="s">
+        <v>366</v>
+      </c>
+      <c r="U39" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA39" s="19"/>
+      <c r="AB39" s="19"/>
+      <c r="AC39" s="19"/>
+      <c r="AD39" s="19"/>
+      <c r="AK39">
+        <v>1</v>
+      </c>
+      <c r="AQ39" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS39">
+        <v>0</v>
+      </c>
+      <c r="AT39" t="s">
+        <v>388</v>
+      </c>
+      <c r="AU39" t="s">
+        <v>388</v>
+      </c>
+      <c r="BC39" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD39" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE39" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF39" s="28">
+        <v>20</v>
+      </c>
+      <c r="BI39" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ39" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK39">
+        <v>0</v>
+      </c>
+      <c r="BL39" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BM39">
+        <v>0</v>
+      </c>
+      <c r="BN39">
+        <v>0</v>
+      </c>
+      <c r="BO39">
+        <v>0</v>
+      </c>
+      <c r="BP39">
+        <v>2</v>
+      </c>
+      <c r="BQ39" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BR39" s="27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F40" s="29"/>
+      <c r="J40" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L40" s="26">
+        <v>4</v>
+      </c>
+      <c r="N40" s="26">
+        <v>3</v>
+      </c>
+      <c r="O40" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P40" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q40" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R40" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U40" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA40" s="30"/>
+      <c r="AB40" s="30"/>
+      <c r="AC40" s="30"/>
+      <c r="AD40" s="30"/>
+      <c r="AK40" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ40" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS40" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT40" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="AU40" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="BC40" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD40" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE40" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF40" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI40" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ40" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK40" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL40" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM40" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN40" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO40" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP40" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ40" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR40" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F41" s="29"/>
+      <c r="J41" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L41" s="26">
+        <v>4</v>
+      </c>
+      <c r="N41" s="26">
+        <v>3</v>
+      </c>
+      <c r="O41" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P41" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q41" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R41" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U41" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA41" s="30"/>
+      <c r="AB41" s="30"/>
+      <c r="AC41" s="30"/>
+      <c r="AD41" s="30"/>
+      <c r="AK41" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ41" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS41" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT41" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="AU41" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="BC41" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD41" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE41" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF41" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI41" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ41" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK41" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL41" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM41" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN41" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO41" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP41" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ41" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR41" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F42" s="29"/>
+      <c r="J42" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L42" s="26">
+        <v>4</v>
+      </c>
+      <c r="N42" s="26">
+        <v>3</v>
+      </c>
+      <c r="O42" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P42" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q42" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R42" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U42" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA42" s="30"/>
+      <c r="AB42" s="30"/>
+      <c r="AC42" s="30"/>
+      <c r="AD42" s="30"/>
+      <c r="AK42" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ42" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS42" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT42" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="AU42" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="BC42" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD42" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE42" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF42" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI42" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ42" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK42" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL42" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM42" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN42" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO42" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP42" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ42" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR42" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F43" s="29"/>
+      <c r="J43" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L43" s="26">
+        <v>4</v>
+      </c>
+      <c r="N43" s="26">
+        <v>3</v>
+      </c>
+      <c r="O43" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P43" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q43" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R43" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U43" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA43" s="30"/>
+      <c r="AB43" s="30"/>
+      <c r="AC43" s="30"/>
+      <c r="AD43" s="30"/>
+      <c r="AK43" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ43" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS43" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT43" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="AU43" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="BC43" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD43" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE43" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF43" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI43" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ43" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK43" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL43" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM43" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN43" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO43" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP43" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ43" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR43" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>371</v>
+      </c>
+      <c r="C44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" t="s">
+        <v>362</v>
+      </c>
+      <c r="F44" s="17"/>
+      <c r="J44" t="s">
+        <v>66</v>
+      </c>
+      <c r="L44">
+        <v>4</v>
+      </c>
+      <c r="N44">
+        <v>3</v>
+      </c>
+      <c r="O44" t="s">
+        <v>363</v>
+      </c>
+      <c r="P44" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>365</v>
+      </c>
+      <c r="R44" t="s">
+        <v>366</v>
+      </c>
+      <c r="U44" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA44" s="19"/>
+      <c r="AB44" s="19"/>
+      <c r="AC44" s="19"/>
+      <c r="AD44" s="19"/>
+      <c r="AK44">
+        <v>1</v>
+      </c>
+      <c r="AQ44" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS44">
+        <v>0</v>
+      </c>
+      <c r="AT44" t="s">
+        <v>390</v>
+      </c>
+      <c r="AU44" t="s">
+        <v>390</v>
+      </c>
+      <c r="BC44" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD44" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE44" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF44" s="28">
+        <v>20</v>
+      </c>
+      <c r="BI44" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ44" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK44">
+        <v>0</v>
+      </c>
+      <c r="BL44" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BM44">
+        <v>0</v>
+      </c>
+      <c r="BN44">
+        <v>0</v>
+      </c>
+      <c r="BO44">
+        <v>0</v>
+      </c>
+      <c r="BP44">
+        <v>2</v>
+      </c>
+      <c r="BQ44" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BR44" s="27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>384</v>
+      </c>
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
+        <v>362</v>
+      </c>
+      <c r="F45" s="17"/>
+      <c r="J45" t="s">
+        <v>66</v>
+      </c>
+      <c r="L45">
+        <v>4</v>
+      </c>
+      <c r="N45">
+        <v>3</v>
+      </c>
+      <c r="O45" t="s">
+        <v>363</v>
+      </c>
+      <c r="P45" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>365</v>
+      </c>
+      <c r="R45" t="s">
+        <v>366</v>
+      </c>
+      <c r="U45" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA45" s="19"/>
+      <c r="AB45" s="19"/>
+      <c r="AC45" s="19"/>
+      <c r="AD45" s="19"/>
+      <c r="AK45">
+        <v>1</v>
+      </c>
+      <c r="AQ45" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS45">
+        <v>0</v>
+      </c>
+      <c r="AT45" t="s">
+        <v>390</v>
+      </c>
+      <c r="AU45" t="s">
+        <v>390</v>
+      </c>
+      <c r="BC45" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD45" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE45" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF45" s="28">
+        <v>20</v>
+      </c>
+      <c r="BI45" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ45" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK45">
+        <v>0</v>
+      </c>
+      <c r="BL45" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BM45">
+        <v>0</v>
+      </c>
+      <c r="BN45">
+        <v>0</v>
+      </c>
+      <c r="BO45">
+        <v>0</v>
+      </c>
+      <c r="BP45">
+        <v>2</v>
+      </c>
+      <c r="BQ45" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BR45" s="27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>385</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" t="s">
+        <v>362</v>
+      </c>
+      <c r="F46" s="17"/>
+      <c r="J46" t="s">
+        <v>66</v>
+      </c>
+      <c r="L46">
+        <v>4</v>
+      </c>
+      <c r="N46">
+        <v>3</v>
+      </c>
+      <c r="O46" t="s">
+        <v>363</v>
+      </c>
+      <c r="P46" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>365</v>
+      </c>
+      <c r="R46" t="s">
+        <v>366</v>
+      </c>
+      <c r="U46" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA46" s="19"/>
+      <c r="AB46" s="19"/>
+      <c r="AC46" s="19"/>
+      <c r="AD46" s="19"/>
+      <c r="AK46">
+        <v>1</v>
+      </c>
+      <c r="AQ46" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS46">
+        <v>0</v>
+      </c>
+      <c r="AT46" t="s">
+        <v>390</v>
+      </c>
+      <c r="AU46" t="s">
+        <v>390</v>
+      </c>
+      <c r="BC46" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD46" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE46" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF46" s="28">
+        <v>20</v>
+      </c>
+      <c r="BI46" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ46" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK46">
+        <v>0</v>
+      </c>
+      <c r="BL46" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BM46">
+        <v>0</v>
+      </c>
+      <c r="BN46">
+        <v>0</v>
+      </c>
+      <c r="BO46">
+        <v>0</v>
+      </c>
+      <c r="BP46">
+        <v>2</v>
+      </c>
+      <c r="BQ46" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BR46" s="27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>386</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" t="s">
+        <v>362</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="J47" t="s">
+        <v>66</v>
+      </c>
+      <c r="L47">
+        <v>4</v>
+      </c>
+      <c r="N47">
+        <v>3</v>
+      </c>
+      <c r="O47" t="s">
+        <v>363</v>
+      </c>
+      <c r="P47" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>365</v>
+      </c>
+      <c r="R47" t="s">
+        <v>366</v>
+      </c>
+      <c r="U47" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA47" s="19"/>
+      <c r="AB47" s="19"/>
+      <c r="AC47" s="19"/>
+      <c r="AD47" s="19"/>
+      <c r="AK47">
+        <v>1</v>
+      </c>
+      <c r="AQ47" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS47">
+        <v>0</v>
+      </c>
+      <c r="AT47" t="s">
+        <v>390</v>
+      </c>
+      <c r="AU47" t="s">
+        <v>390</v>
+      </c>
+      <c r="BC47" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD47" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE47" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF47" s="28">
+        <v>20</v>
+      </c>
+      <c r="BI47" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ47" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK47">
+        <v>0</v>
+      </c>
+      <c r="BL47" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BM47">
+        <v>0</v>
+      </c>
+      <c r="BN47">
+        <v>0</v>
+      </c>
+      <c r="BO47">
+        <v>0</v>
+      </c>
+      <c r="BP47">
+        <v>2</v>
+      </c>
+      <c r="BQ47" s="27">
+        <v>-1</v>
+      </c>
+      <c r="BR47" s="27">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="26" t="s">
+        <v>370</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F48" s="29"/>
+      <c r="J48" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L48" s="26">
+        <v>4</v>
+      </c>
+      <c r="N48" s="26">
+        <v>3</v>
+      </c>
+      <c r="O48" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P48" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q48" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R48" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U48" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA48" s="30"/>
+      <c r="AB48" s="30"/>
+      <c r="AC48" s="30"/>
+      <c r="AD48" s="30"/>
+      <c r="AK48" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ48" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS48" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT48" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="AU48" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="BC48" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD48" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE48" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF48" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI48" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ48" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK48" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL48" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM48" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN48" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO48" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP48" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ48" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR48" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F49" s="29"/>
+      <c r="J49" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L49" s="26">
+        <v>4</v>
+      </c>
+      <c r="N49" s="26">
+        <v>3</v>
+      </c>
+      <c r="O49" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P49" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q49" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R49" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U49" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA49" s="30"/>
+      <c r="AB49" s="30"/>
+      <c r="AC49" s="30"/>
+      <c r="AD49" s="30"/>
+      <c r="AK49" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ49" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS49" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT49" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="AU49" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="BC49" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD49" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE49" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF49" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI49" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ49" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK49" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL49" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM49" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN49" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO49" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP49" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ49" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR49" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F50" s="29"/>
+      <c r="J50" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L50" s="26">
+        <v>4</v>
+      </c>
+      <c r="N50" s="26">
+        <v>3</v>
+      </c>
+      <c r="O50" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P50" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q50" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R50" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U50" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA50" s="30"/>
+      <c r="AB50" s="30"/>
+      <c r="AC50" s="30"/>
+      <c r="AD50" s="30"/>
+      <c r="AK50" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ50" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS50" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT50" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="AU50" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="BC50" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD50" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE50" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF50" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI50" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ50" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK50" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL50" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM50" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN50" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO50" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP50" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ50" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR50" s="26">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="F51" s="29"/>
+      <c r="J51" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L51" s="26">
+        <v>4</v>
+      </c>
+      <c r="N51" s="26">
+        <v>3</v>
+      </c>
+      <c r="O51" s="26" t="s">
+        <v>363</v>
+      </c>
+      <c r="P51" s="26" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q51" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="R51" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="U51" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA51" s="30"/>
+      <c r="AB51" s="30"/>
+      <c r="AC51" s="30"/>
+      <c r="AD51" s="30"/>
+      <c r="AK51" s="26">
+        <v>1</v>
+      </c>
+      <c r="AQ51" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS51" s="26">
+        <v>0</v>
+      </c>
+      <c r="AT51" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="AU51" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="BC51" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="BD51" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="BE51" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF51" s="32">
+        <v>20</v>
+      </c>
+      <c r="BI51" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="BJ51" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="BK51" s="26">
+        <v>0</v>
+      </c>
+      <c r="BL51" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BM51" s="26">
+        <v>0</v>
+      </c>
+      <c r="BN51" s="26">
+        <v>0</v>
+      </c>
+      <c r="BO51" s="26">
+        <v>0</v>
+      </c>
+      <c r="BP51" s="26">
+        <v>2</v>
+      </c>
+      <c r="BQ51" s="26">
+        <v>-1</v>
+      </c>
+      <c r="BR51" s="26">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Publisher Name to Apollo App
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanaBoscolo\source\repos\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B561EE3A-4D0F-4361-98C8-BC0114C7CD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A1F4FD-EA29-42EE-8A9C-D8B2A7270167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="371">
   <si>
     <t>ItemID</t>
   </si>
@@ -1154,70 +1154,7 @@
     <t>SKUC200A01</t>
   </si>
   <si>
-    <t>SKUC200B01</t>
-  </si>
-  <si>
-    <t>SKUC200D01</t>
-  </si>
-  <si>
-    <t>SKUC200A02</t>
-  </si>
-  <si>
-    <t>SKUC200A03</t>
-  </si>
-  <si>
-    <t>SKUC200A04</t>
-  </si>
-  <si>
-    <t>SKUC200A05</t>
-  </si>
-  <si>
-    <t>SKUC200B02</t>
-  </si>
-  <si>
-    <t>SKUC200B03</t>
-  </si>
-  <si>
-    <t>SKUC200B04</t>
-  </si>
-  <si>
-    <t>SKUC200B05</t>
-  </si>
-  <si>
-    <t>SKUC200C01</t>
-  </si>
-  <si>
-    <t>SKUC200C02</t>
-  </si>
-  <si>
-    <t>SKUC200C03</t>
-  </si>
-  <si>
-    <t>SKUC200C04</t>
-  </si>
-  <si>
-    <t>SKUC200D02</t>
-  </si>
-  <si>
-    <t>SKUC200D03</t>
-  </si>
-  <si>
-    <t>SKUC200D04</t>
-  </si>
-  <si>
     <t>Warenwirtschaftliche Prozesse im Onlinehandel durchführen</t>
-  </si>
-  <si>
-    <t>Mit Kunden im Onlinehandel kommunizieren</t>
-  </si>
-  <si>
-    <t>Verkaufsfördernde Maßnahmen im Onlinehandel durchführen</t>
-  </si>
-  <si>
-    <t>Onlineaktivitäten kaufmännisch steuern und kontrollieren</t>
-  </si>
-  <si>
-    <t>Im Onlinehandel projektorientiert arbeiten</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1531,13 +1468,12 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2430,10 +2366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
-  <dimension ref="A1:BR51"/>
+  <dimension ref="A1:BR30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AU30" sqref="AU30:AU51"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5168,7 +5104,7 @@
       <c r="D30" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="F30" s="29"/>
+      <c r="F30" s="28"/>
       <c r="J30" s="26" t="s">
         <v>66</v>
       </c>
@@ -5193,10 +5129,10 @@
       <c r="U30" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="AA30" s="30"/>
-      <c r="AB30" s="30"/>
-      <c r="AC30" s="30"/>
-      <c r="AD30" s="30"/>
+      <c r="AA30" s="29"/>
+      <c r="AB30" s="29"/>
+      <c r="AC30" s="29"/>
+      <c r="AD30" s="29"/>
       <c r="AK30" s="26">
         <v>1</v>
       </c>
@@ -5207,21 +5143,21 @@
         <v>0</v>
       </c>
       <c r="AT30" s="26" t="s">
-        <v>387</v>
+        <v>370</v>
       </c>
       <c r="AU30" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="BC30" s="31" t="s">
+        <v>370</v>
+      </c>
+      <c r="BC30" s="30" t="s">
         <v>355</v>
       </c>
-      <c r="BD30" s="32" t="s">
+      <c r="BD30" s="31" t="s">
         <v>353</v>
       </c>
-      <c r="BE30" s="32" t="s">
+      <c r="BE30" s="31" t="s">
         <v>354</v>
       </c>
-      <c r="BF30" s="32">
+      <c r="BF30" s="31">
         <v>20</v>
       </c>
       <c r="BI30" s="26" t="s">
@@ -5252,2043 +5188,6 @@
         <v>-1</v>
       </c>
       <c r="BR30" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
-        <v>372</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F31" s="29"/>
-      <c r="J31" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L31" s="26">
-        <v>4</v>
-      </c>
-      <c r="N31" s="26">
-        <v>3</v>
-      </c>
-      <c r="O31" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P31" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q31" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R31" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U31" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA31" s="30"/>
-      <c r="AB31" s="30"/>
-      <c r="AC31" s="30"/>
-      <c r="AD31" s="30"/>
-      <c r="AK31" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ31" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS31" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT31" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="AU31" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="BC31" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD31" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE31" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF31" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI31" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ31" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK31" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL31" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM31" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN31" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO31" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP31" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ31" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR31" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="26" t="s">
-        <v>373</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F32" s="29"/>
-      <c r="J32" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L32" s="26">
-        <v>4</v>
-      </c>
-      <c r="N32" s="26">
-        <v>3</v>
-      </c>
-      <c r="O32" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P32" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q32" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R32" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U32" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA32" s="30"/>
-      <c r="AB32" s="30"/>
-      <c r="AC32" s="30"/>
-      <c r="AD32" s="30"/>
-      <c r="AK32" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ32" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS32" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT32" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="AU32" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="BC32" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD32" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE32" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF32" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI32" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ32" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK32" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL32" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM32" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN32" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO32" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP32" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ32" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR32" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="26" t="s">
-        <v>374</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F33" s="29"/>
-      <c r="J33" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L33" s="26">
-        <v>4</v>
-      </c>
-      <c r="N33" s="26">
-        <v>3</v>
-      </c>
-      <c r="O33" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P33" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q33" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R33" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U33" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA33" s="30"/>
-      <c r="AB33" s="30"/>
-      <c r="AC33" s="30"/>
-      <c r="AD33" s="30"/>
-      <c r="AK33" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ33" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS33" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT33" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="AU33" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="BC33" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD33" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE33" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF33" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI33" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ33" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK33" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL33" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM33" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN33" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO33" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP33" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ33" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR33" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="26" t="s">
-        <v>375</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F34" s="29"/>
-      <c r="J34" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L34" s="26">
-        <v>4</v>
-      </c>
-      <c r="N34" s="26">
-        <v>3</v>
-      </c>
-      <c r="O34" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P34" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q34" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R34" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U34" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA34" s="30"/>
-      <c r="AB34" s="30"/>
-      <c r="AC34" s="30"/>
-      <c r="AD34" s="30"/>
-      <c r="AK34" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ34" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS34" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT34" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="AU34" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="BC34" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD34" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE34" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF34" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI34" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ34" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK34" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL34" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM34" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN34" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO34" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP34" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ34" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR34" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>370</v>
-      </c>
-      <c r="C35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" t="s">
-        <v>362</v>
-      </c>
-      <c r="F35" s="17"/>
-      <c r="J35" t="s">
-        <v>66</v>
-      </c>
-      <c r="L35">
-        <v>4</v>
-      </c>
-      <c r="N35">
-        <v>3</v>
-      </c>
-      <c r="O35" t="s">
-        <v>363</v>
-      </c>
-      <c r="P35" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>365</v>
-      </c>
-      <c r="R35" t="s">
-        <v>366</v>
-      </c>
-      <c r="U35" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA35" s="19"/>
-      <c r="AB35" s="19"/>
-      <c r="AC35" s="19"/>
-      <c r="AD35" s="19"/>
-      <c r="AK35">
-        <v>1</v>
-      </c>
-      <c r="AQ35" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS35">
-        <v>0</v>
-      </c>
-      <c r="AT35" t="s">
-        <v>388</v>
-      </c>
-      <c r="AU35" t="s">
-        <v>388</v>
-      </c>
-      <c r="BC35" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD35" s="28" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE35" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF35" s="28">
-        <v>20</v>
-      </c>
-      <c r="BI35" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ35" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK35">
-        <v>0</v>
-      </c>
-      <c r="BL35" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BM35">
-        <v>0</v>
-      </c>
-      <c r="BN35">
-        <v>0</v>
-      </c>
-      <c r="BO35">
-        <v>0</v>
-      </c>
-      <c r="BP35">
-        <v>2</v>
-      </c>
-      <c r="BQ35" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BR35" s="27">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>376</v>
-      </c>
-      <c r="C36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" t="s">
-        <v>362</v>
-      </c>
-      <c r="F36" s="17"/>
-      <c r="J36" t="s">
-        <v>66</v>
-      </c>
-      <c r="L36">
-        <v>4</v>
-      </c>
-      <c r="N36">
-        <v>3</v>
-      </c>
-      <c r="O36" t="s">
-        <v>363</v>
-      </c>
-      <c r="P36" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>365</v>
-      </c>
-      <c r="R36" t="s">
-        <v>366</v>
-      </c>
-      <c r="U36" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA36" s="19"/>
-      <c r="AB36" s="19"/>
-      <c r="AC36" s="19"/>
-      <c r="AD36" s="19"/>
-      <c r="AK36">
-        <v>1</v>
-      </c>
-      <c r="AQ36" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS36">
-        <v>0</v>
-      </c>
-      <c r="AT36" t="s">
-        <v>388</v>
-      </c>
-      <c r="AU36" t="s">
-        <v>388</v>
-      </c>
-      <c r="BC36" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD36" s="28" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE36" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF36" s="28">
-        <v>20</v>
-      </c>
-      <c r="BI36" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ36" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK36">
-        <v>0</v>
-      </c>
-      <c r="BL36" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BM36">
-        <v>0</v>
-      </c>
-      <c r="BN36">
-        <v>0</v>
-      </c>
-      <c r="BO36">
-        <v>0</v>
-      </c>
-      <c r="BP36">
-        <v>2</v>
-      </c>
-      <c r="BQ36" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BR36" s="27">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>377</v>
-      </c>
-      <c r="C37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" t="s">
-        <v>362</v>
-      </c>
-      <c r="F37" s="17"/>
-      <c r="J37" t="s">
-        <v>66</v>
-      </c>
-      <c r="L37">
-        <v>4</v>
-      </c>
-      <c r="N37">
-        <v>3</v>
-      </c>
-      <c r="O37" t="s">
-        <v>363</v>
-      </c>
-      <c r="P37" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>365</v>
-      </c>
-      <c r="R37" t="s">
-        <v>366</v>
-      </c>
-      <c r="U37" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA37" s="19"/>
-      <c r="AB37" s="19"/>
-      <c r="AC37" s="19"/>
-      <c r="AD37" s="19"/>
-      <c r="AK37">
-        <v>1</v>
-      </c>
-      <c r="AQ37" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS37">
-        <v>0</v>
-      </c>
-      <c r="AT37" t="s">
-        <v>388</v>
-      </c>
-      <c r="AU37" t="s">
-        <v>388</v>
-      </c>
-      <c r="BC37" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD37" s="28" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE37" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF37" s="28">
-        <v>20</v>
-      </c>
-      <c r="BI37" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ37" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK37">
-        <v>0</v>
-      </c>
-      <c r="BL37" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BM37">
-        <v>0</v>
-      </c>
-      <c r="BN37">
-        <v>0</v>
-      </c>
-      <c r="BO37">
-        <v>0</v>
-      </c>
-      <c r="BP37">
-        <v>2</v>
-      </c>
-      <c r="BQ37" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BR37" s="27">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>378</v>
-      </c>
-      <c r="C38" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" t="s">
-        <v>362</v>
-      </c>
-      <c r="F38" s="17"/>
-      <c r="J38" t="s">
-        <v>66</v>
-      </c>
-      <c r="L38">
-        <v>4</v>
-      </c>
-      <c r="N38">
-        <v>3</v>
-      </c>
-      <c r="O38" t="s">
-        <v>363</v>
-      </c>
-      <c r="P38" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>365</v>
-      </c>
-      <c r="R38" t="s">
-        <v>366</v>
-      </c>
-      <c r="U38" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA38" s="19"/>
-      <c r="AB38" s="19"/>
-      <c r="AC38" s="19"/>
-      <c r="AD38" s="19"/>
-      <c r="AK38">
-        <v>1</v>
-      </c>
-      <c r="AQ38" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS38">
-        <v>0</v>
-      </c>
-      <c r="AT38" t="s">
-        <v>388</v>
-      </c>
-      <c r="AU38" t="s">
-        <v>388</v>
-      </c>
-      <c r="BC38" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD38" s="28" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE38" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF38" s="28">
-        <v>20</v>
-      </c>
-      <c r="BI38" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ38" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK38">
-        <v>0</v>
-      </c>
-      <c r="BL38" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BM38">
-        <v>0</v>
-      </c>
-      <c r="BN38">
-        <v>0</v>
-      </c>
-      <c r="BO38">
-        <v>0</v>
-      </c>
-      <c r="BP38">
-        <v>2</v>
-      </c>
-      <c r="BQ38" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BR38" s="27">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>379</v>
-      </c>
-      <c r="C39" t="s">
-        <v>64</v>
-      </c>
-      <c r="D39" t="s">
-        <v>362</v>
-      </c>
-      <c r="F39" s="17"/>
-      <c r="J39" t="s">
-        <v>66</v>
-      </c>
-      <c r="L39">
-        <v>4</v>
-      </c>
-      <c r="N39">
-        <v>3</v>
-      </c>
-      <c r="O39" t="s">
-        <v>363</v>
-      </c>
-      <c r="P39" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>365</v>
-      </c>
-      <c r="R39" t="s">
-        <v>366</v>
-      </c>
-      <c r="U39" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA39" s="19"/>
-      <c r="AB39" s="19"/>
-      <c r="AC39" s="19"/>
-      <c r="AD39" s="19"/>
-      <c r="AK39">
-        <v>1</v>
-      </c>
-      <c r="AQ39" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS39">
-        <v>0</v>
-      </c>
-      <c r="AT39" t="s">
-        <v>388</v>
-      </c>
-      <c r="AU39" t="s">
-        <v>388</v>
-      </c>
-      <c r="BC39" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD39" s="28" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE39" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF39" s="28">
-        <v>20</v>
-      </c>
-      <c r="BI39" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ39" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK39">
-        <v>0</v>
-      </c>
-      <c r="BL39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BM39">
-        <v>0</v>
-      </c>
-      <c r="BN39">
-        <v>0</v>
-      </c>
-      <c r="BO39">
-        <v>0</v>
-      </c>
-      <c r="BP39">
-        <v>2</v>
-      </c>
-      <c r="BQ39" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BR39" s="27">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="26" t="s">
-        <v>380</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F40" s="29"/>
-      <c r="J40" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L40" s="26">
-        <v>4</v>
-      </c>
-      <c r="N40" s="26">
-        <v>3</v>
-      </c>
-      <c r="O40" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P40" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q40" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R40" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U40" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA40" s="30"/>
-      <c r="AB40" s="30"/>
-      <c r="AC40" s="30"/>
-      <c r="AD40" s="30"/>
-      <c r="AK40" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ40" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS40" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT40" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="AU40" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="BC40" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD40" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE40" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF40" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI40" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ40" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK40" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL40" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM40" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN40" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO40" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP40" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ40" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR40" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="26" t="s">
-        <v>381</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F41" s="29"/>
-      <c r="J41" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L41" s="26">
-        <v>4</v>
-      </c>
-      <c r="N41" s="26">
-        <v>3</v>
-      </c>
-      <c r="O41" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P41" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q41" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R41" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U41" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA41" s="30"/>
-      <c r="AB41" s="30"/>
-      <c r="AC41" s="30"/>
-      <c r="AD41" s="30"/>
-      <c r="AK41" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ41" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS41" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT41" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="AU41" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="BC41" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD41" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE41" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF41" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI41" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ41" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK41" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL41" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM41" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN41" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO41" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP41" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ41" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR41" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="26" t="s">
-        <v>382</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F42" s="29"/>
-      <c r="J42" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L42" s="26">
-        <v>4</v>
-      </c>
-      <c r="N42" s="26">
-        <v>3</v>
-      </c>
-      <c r="O42" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P42" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q42" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R42" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U42" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA42" s="30"/>
-      <c r="AB42" s="30"/>
-      <c r="AC42" s="30"/>
-      <c r="AD42" s="30"/>
-      <c r="AK42" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ42" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS42" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT42" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="AU42" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="BC42" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD42" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE42" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF42" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI42" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ42" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK42" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL42" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM42" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN42" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO42" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP42" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ42" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR42" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="26" t="s">
-        <v>383</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F43" s="29"/>
-      <c r="J43" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L43" s="26">
-        <v>4</v>
-      </c>
-      <c r="N43" s="26">
-        <v>3</v>
-      </c>
-      <c r="O43" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P43" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q43" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R43" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U43" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA43" s="30"/>
-      <c r="AB43" s="30"/>
-      <c r="AC43" s="30"/>
-      <c r="AD43" s="30"/>
-      <c r="AK43" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ43" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS43" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT43" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="AU43" s="26" t="s">
-        <v>389</v>
-      </c>
-      <c r="BC43" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD43" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE43" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF43" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI43" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ43" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK43" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL43" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM43" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN43" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO43" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP43" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ43" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR43" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>371</v>
-      </c>
-      <c r="C44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" t="s">
-        <v>362</v>
-      </c>
-      <c r="F44" s="17"/>
-      <c r="J44" t="s">
-        <v>66</v>
-      </c>
-      <c r="L44">
-        <v>4</v>
-      </c>
-      <c r="N44">
-        <v>3</v>
-      </c>
-      <c r="O44" t="s">
-        <v>363</v>
-      </c>
-      <c r="P44" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>365</v>
-      </c>
-      <c r="R44" t="s">
-        <v>366</v>
-      </c>
-      <c r="U44" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA44" s="19"/>
-      <c r="AB44" s="19"/>
-      <c r="AC44" s="19"/>
-      <c r="AD44" s="19"/>
-      <c r="AK44">
-        <v>1</v>
-      </c>
-      <c r="AQ44" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS44">
-        <v>0</v>
-      </c>
-      <c r="AT44" t="s">
-        <v>390</v>
-      </c>
-      <c r="AU44" t="s">
-        <v>390</v>
-      </c>
-      <c r="BC44" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD44" s="28" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE44" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF44" s="28">
-        <v>20</v>
-      </c>
-      <c r="BI44" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ44" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK44">
-        <v>0</v>
-      </c>
-      <c r="BL44" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BM44">
-        <v>0</v>
-      </c>
-      <c r="BN44">
-        <v>0</v>
-      </c>
-      <c r="BO44">
-        <v>0</v>
-      </c>
-      <c r="BP44">
-        <v>2</v>
-      </c>
-      <c r="BQ44" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BR44" s="27">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>384</v>
-      </c>
-      <c r="C45" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" t="s">
-        <v>362</v>
-      </c>
-      <c r="F45" s="17"/>
-      <c r="J45" t="s">
-        <v>66</v>
-      </c>
-      <c r="L45">
-        <v>4</v>
-      </c>
-      <c r="N45">
-        <v>3</v>
-      </c>
-      <c r="O45" t="s">
-        <v>363</v>
-      </c>
-      <c r="P45" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>365</v>
-      </c>
-      <c r="R45" t="s">
-        <v>366</v>
-      </c>
-      <c r="U45" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA45" s="19"/>
-      <c r="AB45" s="19"/>
-      <c r="AC45" s="19"/>
-      <c r="AD45" s="19"/>
-      <c r="AK45">
-        <v>1</v>
-      </c>
-      <c r="AQ45" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS45">
-        <v>0</v>
-      </c>
-      <c r="AT45" t="s">
-        <v>390</v>
-      </c>
-      <c r="AU45" t="s">
-        <v>390</v>
-      </c>
-      <c r="BC45" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD45" s="28" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE45" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF45" s="28">
-        <v>20</v>
-      </c>
-      <c r="BI45" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ45" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK45">
-        <v>0</v>
-      </c>
-      <c r="BL45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BM45">
-        <v>0</v>
-      </c>
-      <c r="BN45">
-        <v>0</v>
-      </c>
-      <c r="BO45">
-        <v>0</v>
-      </c>
-      <c r="BP45">
-        <v>2</v>
-      </c>
-      <c r="BQ45" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BR45" s="27">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>385</v>
-      </c>
-      <c r="C46" t="s">
-        <v>64</v>
-      </c>
-      <c r="D46" t="s">
-        <v>362</v>
-      </c>
-      <c r="F46" s="17"/>
-      <c r="J46" t="s">
-        <v>66</v>
-      </c>
-      <c r="L46">
-        <v>4</v>
-      </c>
-      <c r="N46">
-        <v>3</v>
-      </c>
-      <c r="O46" t="s">
-        <v>363</v>
-      </c>
-      <c r="P46" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>365</v>
-      </c>
-      <c r="R46" t="s">
-        <v>366</v>
-      </c>
-      <c r="U46" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA46" s="19"/>
-      <c r="AB46" s="19"/>
-      <c r="AC46" s="19"/>
-      <c r="AD46" s="19"/>
-      <c r="AK46">
-        <v>1</v>
-      </c>
-      <c r="AQ46" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS46">
-        <v>0</v>
-      </c>
-      <c r="AT46" t="s">
-        <v>390</v>
-      </c>
-      <c r="AU46" t="s">
-        <v>390</v>
-      </c>
-      <c r="BC46" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD46" s="28" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE46" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF46" s="28">
-        <v>20</v>
-      </c>
-      <c r="BI46" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ46" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK46">
-        <v>0</v>
-      </c>
-      <c r="BL46" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BM46">
-        <v>0</v>
-      </c>
-      <c r="BN46">
-        <v>0</v>
-      </c>
-      <c r="BO46">
-        <v>0</v>
-      </c>
-      <c r="BP46">
-        <v>2</v>
-      </c>
-      <c r="BQ46" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BR46" s="27">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>386</v>
-      </c>
-      <c r="C47" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47" t="s">
-        <v>362</v>
-      </c>
-      <c r="F47" s="17"/>
-      <c r="J47" t="s">
-        <v>66</v>
-      </c>
-      <c r="L47">
-        <v>4</v>
-      </c>
-      <c r="N47">
-        <v>3</v>
-      </c>
-      <c r="O47" t="s">
-        <v>363</v>
-      </c>
-      <c r="P47" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>365</v>
-      </c>
-      <c r="R47" t="s">
-        <v>366</v>
-      </c>
-      <c r="U47" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA47" s="19"/>
-      <c r="AB47" s="19"/>
-      <c r="AC47" s="19"/>
-      <c r="AD47" s="19"/>
-      <c r="AK47">
-        <v>1</v>
-      </c>
-      <c r="AQ47" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS47">
-        <v>0</v>
-      </c>
-      <c r="AT47" t="s">
-        <v>390</v>
-      </c>
-      <c r="AU47" t="s">
-        <v>390</v>
-      </c>
-      <c r="BC47" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD47" s="28" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE47" s="28" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF47" s="28">
-        <v>20</v>
-      </c>
-      <c r="BI47" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ47" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK47">
-        <v>0</v>
-      </c>
-      <c r="BL47" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BM47">
-        <v>0</v>
-      </c>
-      <c r="BN47">
-        <v>0</v>
-      </c>
-      <c r="BO47">
-        <v>0</v>
-      </c>
-      <c r="BP47">
-        <v>2</v>
-      </c>
-      <c r="BQ47" s="27">
-        <v>-1</v>
-      </c>
-      <c r="BR47" s="27">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="26" t="s">
-        <v>370</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F48" s="29"/>
-      <c r="J48" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L48" s="26">
-        <v>4</v>
-      </c>
-      <c r="N48" s="26">
-        <v>3</v>
-      </c>
-      <c r="O48" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P48" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q48" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R48" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U48" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA48" s="30"/>
-      <c r="AB48" s="30"/>
-      <c r="AC48" s="30"/>
-      <c r="AD48" s="30"/>
-      <c r="AK48" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ48" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS48" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT48" s="26" t="s">
-        <v>391</v>
-      </c>
-      <c r="AU48" s="26" t="s">
-        <v>391</v>
-      </c>
-      <c r="BC48" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD48" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE48" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF48" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI48" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ48" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK48" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL48" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM48" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN48" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO48" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP48" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ48" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR48" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="26" t="s">
-        <v>376</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D49" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F49" s="29"/>
-      <c r="J49" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L49" s="26">
-        <v>4</v>
-      </c>
-      <c r="N49" s="26">
-        <v>3</v>
-      </c>
-      <c r="O49" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P49" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q49" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R49" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U49" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA49" s="30"/>
-      <c r="AB49" s="30"/>
-      <c r="AC49" s="30"/>
-      <c r="AD49" s="30"/>
-      <c r="AK49" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ49" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS49" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT49" s="26" t="s">
-        <v>391</v>
-      </c>
-      <c r="AU49" s="26" t="s">
-        <v>391</v>
-      </c>
-      <c r="BC49" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD49" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE49" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF49" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI49" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ49" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK49" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL49" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM49" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN49" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO49" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP49" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ49" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR49" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="26" t="s">
-        <v>377</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D50" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F50" s="29"/>
-      <c r="J50" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L50" s="26">
-        <v>4</v>
-      </c>
-      <c r="N50" s="26">
-        <v>3</v>
-      </c>
-      <c r="O50" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P50" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q50" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R50" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U50" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA50" s="30"/>
-      <c r="AB50" s="30"/>
-      <c r="AC50" s="30"/>
-      <c r="AD50" s="30"/>
-      <c r="AK50" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ50" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS50" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT50" s="26" t="s">
-        <v>391</v>
-      </c>
-      <c r="AU50" s="26" t="s">
-        <v>391</v>
-      </c>
-      <c r="BC50" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD50" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE50" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF50" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI50" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ50" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK50" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL50" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM50" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN50" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO50" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP50" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ50" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR50" s="26">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="26" t="s">
-        <v>378</v>
-      </c>
-      <c r="C51" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D51" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="F51" s="29"/>
-      <c r="J51" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="L51" s="26">
-        <v>4</v>
-      </c>
-      <c r="N51" s="26">
-        <v>3</v>
-      </c>
-      <c r="O51" s="26" t="s">
-        <v>363</v>
-      </c>
-      <c r="P51" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q51" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R51" s="26" t="s">
-        <v>366</v>
-      </c>
-      <c r="U51" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="AA51" s="30"/>
-      <c r="AB51" s="30"/>
-      <c r="AC51" s="30"/>
-      <c r="AD51" s="30"/>
-      <c r="AK51" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ51" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS51" s="26">
-        <v>0</v>
-      </c>
-      <c r="AT51" s="26" t="s">
-        <v>391</v>
-      </c>
-      <c r="AU51" s="26" t="s">
-        <v>391</v>
-      </c>
-      <c r="BC51" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD51" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="BE51" s="32" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF51" s="32">
-        <v>20</v>
-      </c>
-      <c r="BI51" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="BJ51" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="BK51" s="26">
-        <v>0</v>
-      </c>
-      <c r="BL51" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BM51" s="26">
-        <v>0</v>
-      </c>
-      <c r="BN51" s="26">
-        <v>0</v>
-      </c>
-      <c r="BO51" s="26">
-        <v>0</v>
-      </c>
-      <c r="BP51" s="26">
-        <v>2</v>
-      </c>
-      <c r="BQ51" s="26">
-        <v>-1</v>
-      </c>
-      <c r="BR51" s="26">
         <v>-1</v>
       </c>
     </row>
@@ -7697,6 +5596,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100879B58D3C23DCA4AAEF47596CA4D8E48" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee8b9d8723b80ccc4cb578ffd4faacc7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02625a54-df84-4a3b-b049-0bb7e92cde0d" xmlns:ns3="c90f9e10-81f0-426e-b8bb-fc89022b3796" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64b8ed4db9a6e136c161da669116b9cc" ns2:_="" ns3:_="">
     <xsd:import namespace="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
@@ -7905,27 +5824,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7942,29 +5866,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed Problem in Commons
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanaBoscolo\source\repos\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A1F4FD-EA29-42EE-8A9C-D8B2A7270167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477F9D4B-B373-48EB-BFA0-A2235A8210B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="9792" yWindow="5952" windowWidth="26112" windowHeight="17352" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -2368,21 +2368,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
   <dimension ref="A1:BR30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD51"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BK30" sqref="BK30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" customWidth="1"/>
-    <col min="27" max="27" width="16.7109375" customWidth="1"/>
-    <col min="46" max="46" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.44140625" customWidth="1"/>
+    <col min="27" max="27" width="16.6640625" customWidth="1"/>
+    <col min="46" max="46" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>127</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>144</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>153</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>171</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>190</v>
       </c>
@@ -4376,7 +4376,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>198</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>205</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>212</v>
       </c>
@@ -4642,7 +4642,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>219</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>227</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>234</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>241</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>248</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>369</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>0</v>
       </c>
       <c r="BO30" s="26">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BP30" s="26">
         <v>2</v>
@@ -5210,24 +5210,24 @@
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>255</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>256</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>262</v>
       </c>
@@ -5270,7 +5270,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
@@ -5283,7 +5283,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
@@ -5293,7 +5293,7 @@
       <c r="E5" s="10"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
@@ -5303,7 +5303,7 @@
       <c r="E6" s="10"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>272</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
@@ -5334,7 +5334,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
@@ -5344,7 +5344,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
@@ -5354,7 +5354,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>279</v>
       </c>
@@ -5372,7 +5372,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
@@ -5382,7 +5382,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
@@ -5392,7 +5392,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>284</v>
       </c>
@@ -5410,7 +5410,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
@@ -5420,7 +5420,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>289</v>
       </c>
@@ -5438,7 +5438,7 @@
       </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
@@ -5448,7 +5448,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
@@ -5458,7 +5458,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
@@ -5468,7 +5468,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>295</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
@@ -5498,7 +5498,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="23.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="23.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
@@ -5508,7 +5508,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
@@ -5518,7 +5518,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>302</v>
       </c>
@@ -5536,7 +5536,7 @@
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
@@ -5546,7 +5546,7 @@
       <c r="E25" s="7"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
@@ -5556,7 +5556,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
@@ -5566,7 +5566,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
@@ -5576,11 +5576,11 @@
       <c r="E28" s="7"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" display="https://www.biwe-bbq.de/weiterbildungsportal/themen/coaching-qualifizierung/einzelansicht/tq-lagerlogistik" xr:uid="{508EE104-A0F6-4678-8237-1AA62422A333}"/>
@@ -5596,6 +5596,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
@@ -5604,15 +5613,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5825,6 +5825,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -5837,14 +5845,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added Feedback to Data and created new files
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D394231-7731-4D0E-9D00-A50302701B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96A18CC-36B8-414E-91B5-29A840E9CA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7704" yWindow="4272" windowWidth="30564" windowHeight="17352" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="372">
   <si>
     <t>ItemID</t>
   </si>
@@ -394,9 +394,6 @@
   </si>
   <si>
     <t>Du willst Paletten einlagern, die mit folgenden Zeichen gekennzeichnet sind. Ordne die Handhabungszeichen ihrer Bedeutung zu.</t>
-  </si>
-  <si>
-    <t>Bitte ziehe die passende Antwort in die Abbildung.</t>
   </si>
   <si>
     <t>4a - 1b - 3c - 2d</t>
@@ -1103,9 +1100,6 @@
     <t xml:space="preserve">Test Fachkraft Lagerlogistik (Fachlagerist) </t>
   </si>
   <si>
-    <t>Mit diesem kurzen Test kannst du deine Fähigkeiten prüfen. Das Ergebniss zeigt dir wie viel Erfahrung du in den verschiedenen Bereichen des Berufes mitbringst. Aufbauend auf deinen Kompetenzen können wir dir passende Vorschläge für Weiterbildungen zeigen.</t>
-  </si>
-  <si>
     <t>Die Fragen beantwortest du, indem du entweder die passende Antwort auswählst, eine richtige Reihenfolge herstellst oder die passenden Paare bildest. Probiere es aus!</t>
   </si>
   <si>
@@ -1115,9 +1109,6 @@
     <t>3a - 1b - 2c - 4d</t>
   </si>
   <si>
-    <t>Bitte bringe die Liste in die richtige Reihenfolge durch ziehen der Antworten auf die Positionsnummer.</t>
-  </si>
-  <si>
     <t>Apollo App</t>
   </si>
   <si>
@@ -1157,7 +1148,16 @@
     <t>Warenwirtschaftliche Prozesse im Onlinehandel durchführen</t>
   </si>
   <si>
-    <t>Mit diesem kurzen Test kannst du deine Fähigkeiten prüfen. Das Ergebnis zeigt dir, wie viel Erfahrung du in den verschiedenen Bereichen des Berufs mitbringst. Aufbauend auf deinen Kompetenzen können wir dir passende Vorschläge für Weiterbildungen zeigen.</t>
+    <t>Ich lege wenige Knöpfe auf die Waage, gebe die Stückzahl ein und wiege anschließend alle Knöpfe</t>
+  </si>
+  <si>
+    <t>Mit diesem kurzen Test kannst du deine Fähigkeiten prüfen. Das Ergebniss zeigt dir, wie viel Erfahrung du in den verschiedenen Bereichen des Berufes mitbringst. Aufbauend auf deinen Kompetenzen können wir dir passende Vorschläge für Weiterbildungen zeigen.</t>
+  </si>
+  <si>
+    <t>Bitte bringe die Liste in die richtige Reihenfolge durch gedrückt halten und ziehen der Antworten auf die Positionsnummer.</t>
+  </si>
+  <si>
+    <t>Bitte ziehe die passende Antwort (durch langes gedrückt halten und ziehen) auf die Abbildung.</t>
   </si>
 </sst>
 </file>
@@ -2371,8 +2371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
   <dimension ref="A1:BR30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BD2" sqref="BD2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2549,52 +2549,52 @@
         <v>53</v>
       </c>
       <c r="BC1" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="BD1" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="BJ1" s="2" t="s">
-        <v>326</v>
-      </c>
       <c r="BK1" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BL1" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="BO1" s="2" t="s">
-        <v>350</v>
-      </c>
       <c r="BP1" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="BQ1" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="BR1" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:70" x14ac:dyDescent="0.25">
@@ -2608,7 +2608,7 @@
         <v>55</v>
       </c>
       <c r="J2" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
       <c r="L2">
         <v>4</v>
@@ -2629,7 +2629,7 @@
         <v>59</v>
       </c>
       <c r="U2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AA2" s="19">
         <v>1</v>
@@ -2659,22 +2659,22 @@
         <v>62</v>
       </c>
       <c r="BC2" s="18" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="BD2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="BE2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="BF2">
         <v>10</v>
       </c>
       <c r="BI2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="BJ2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK2">
         <v>3</v>
@@ -2706,13 +2706,13 @@
         <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D3" t="s">
         <v>65</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J3" t="s">
         <v>66</v>
@@ -2758,13 +2758,13 @@
         <v>72</v>
       </c>
       <c r="BC3" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI3" t="s">
         <v>355</v>
       </c>
-      <c r="BI3" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK3">
         <v>3</v>
@@ -2845,13 +2845,13 @@
         <v>80</v>
       </c>
       <c r="BC4" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI4" t="s">
         <v>355</v>
       </c>
-      <c r="BI4" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK4">
         <v>3</v>
@@ -2933,13 +2933,13 @@
         <v>88</v>
       </c>
       <c r="BC5" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI5" t="s">
         <v>355</v>
       </c>
-      <c r="BI5" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK5">
         <v>3</v>
@@ -2971,13 +2971,13 @@
         <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D6" t="s">
         <v>90</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J6" t="s">
         <v>66</v>
@@ -3023,13 +3023,13 @@
         <v>97</v>
       </c>
       <c r="BC6" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI6" t="s">
         <v>355</v>
       </c>
-      <c r="BI6" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK6">
         <v>3</v>
@@ -3061,13 +3061,13 @@
         <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D7" t="s">
         <v>99</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J7" t="s">
         <v>66</v>
@@ -3113,13 +3113,13 @@
         <v>104</v>
       </c>
       <c r="BC7" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI7" t="s">
         <v>355</v>
       </c>
-      <c r="BI7" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK7">
         <v>3</v>
@@ -3151,7 +3151,7 @@
         <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D8" t="s">
         <v>106</v>
@@ -3166,16 +3166,16 @@
         <v>3</v>
       </c>
       <c r="O8" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="P8" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="P8" s="16" t="s">
+      <c r="Q8" s="16" t="s">
         <v>335</v>
       </c>
-      <c r="Q8" s="16" t="s">
+      <c r="R8" s="16" t="s">
         <v>336</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>337</v>
       </c>
       <c r="U8" t="s">
         <v>87</v>
@@ -3200,13 +3200,13 @@
         <v>107</v>
       </c>
       <c r="BC8" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI8" t="s">
         <v>355</v>
       </c>
-      <c r="BI8" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK8">
         <v>3</v>
@@ -3238,13 +3238,13 @@
         <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D9" t="s">
         <v>109</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="J9" t="s">
         <v>66</v>
@@ -3290,13 +3290,13 @@
         <v>115</v>
       </c>
       <c r="BC9" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI9" t="s">
         <v>355</v>
       </c>
-      <c r="BI9" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK9">
         <v>3</v>
@@ -3334,40 +3334,40 @@
         <v>118</v>
       </c>
       <c r="J10" t="s">
+        <v>371</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10" t="s">
+        <v>120</v>
+      </c>
+      <c r="P10" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>122</v>
+      </c>
+      <c r="R10" t="s">
+        <v>123</v>
+      </c>
+      <c r="U10" t="s">
         <v>119</v>
       </c>
-      <c r="L10">
-        <v>4</v>
-      </c>
-      <c r="N10">
-        <v>4</v>
-      </c>
-      <c r="O10" t="s">
-        <v>121</v>
-      </c>
-      <c r="P10" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>123</v>
-      </c>
-      <c r="R10" t="s">
-        <v>124</v>
-      </c>
-      <c r="U10" t="s">
-        <v>120</v>
-      </c>
       <c r="AA10" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="AB10" s="20" t="s">
         <v>312</v>
       </c>
-      <c r="AB10" s="20" t="s">
+      <c r="AC10" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="AC10" s="20" t="s">
+      <c r="AD10" s="20" t="s">
         <v>314</v>
-      </c>
-      <c r="AD10" s="20" t="s">
-        <v>315</v>
       </c>
       <c r="AK10">
         <v>1</v>
@@ -3379,19 +3379,19 @@
         <v>51312</v>
       </c>
       <c r="AT10" t="s">
+        <v>124</v>
+      </c>
+      <c r="AU10" t="s">
         <v>125</v>
       </c>
-      <c r="AU10" t="s">
-        <v>126</v>
-      </c>
       <c r="BC10" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI10" t="s">
         <v>355</v>
       </c>
-      <c r="BI10" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK10">
         <v>3</v>
@@ -3420,13 +3420,13 @@
     </row>
     <row r="11" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
         <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J11" t="s">
         <v>66</v>
@@ -3438,19 +3438,19 @@
         <v>3</v>
       </c>
       <c r="O11" t="s">
+        <v>307</v>
+      </c>
+      <c r="P11" t="s">
         <v>308</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>309</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>310</v>
       </c>
-      <c r="R11" t="s">
-        <v>311</v>
-      </c>
       <c r="U11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA11" s="19"/>
       <c r="AB11" s="19"/>
@@ -3466,19 +3466,19 @@
         <v>51312</v>
       </c>
       <c r="AT11" t="s">
+        <v>124</v>
+      </c>
+      <c r="AU11" t="s">
         <v>125</v>
       </c>
-      <c r="AU11" t="s">
-        <v>126</v>
-      </c>
       <c r="BC11" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI11" t="s">
         <v>355</v>
       </c>
-      <c r="BI11" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK11">
         <v>3</v>
@@ -3507,16 +3507,16 @@
     </row>
     <row r="12" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D12" t="s">
         <v>130</v>
       </c>
-      <c r="C12" t="s">
-        <v>327</v>
-      </c>
-      <c r="D12" t="s">
-        <v>131</v>
-      </c>
       <c r="F12" s="16" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="J12" t="s">
         <v>66</v>
@@ -3528,13 +3528,16 @@
         <v>3</v>
       </c>
       <c r="O12" t="s">
+        <v>131</v>
+      </c>
+      <c r="P12" t="s">
         <v>132</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>133</v>
       </c>
-      <c r="Q12" t="s">
-        <v>134</v>
+      <c r="R12" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="U12" t="s">
         <v>114</v>
@@ -3553,19 +3556,19 @@
         <v>51312</v>
       </c>
       <c r="AT12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AU12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BC12" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI12" t="s">
         <v>355</v>
       </c>
-      <c r="BI12" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK12">
         <v>3</v>
@@ -3594,13 +3597,13 @@
     </row>
     <row r="13" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C13" t="s">
         <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J13" t="s">
         <v>66</v>
@@ -3612,19 +3615,19 @@
         <v>3</v>
       </c>
       <c r="O13" t="s">
+        <v>137</v>
+      </c>
+      <c r="P13" t="s">
         <v>138</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>139</v>
       </c>
-      <c r="Q13" t="s">
-        <v>140</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="R13" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="U13" t="s">
         <v>141</v>
-      </c>
-      <c r="U13" t="s">
-        <v>142</v>
       </c>
       <c r="AA13" s="19"/>
       <c r="AB13" s="19"/>
@@ -3640,19 +3643,19 @@
         <v>51312</v>
       </c>
       <c r="AT13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AU13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BC13" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI13" t="s">
         <v>355</v>
       </c>
-      <c r="BI13" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK13">
         <v>3</v>
@@ -3681,13 +3684,13 @@
     </row>
     <row r="14" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
         <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J14" t="s">
         <v>66</v>
@@ -3699,19 +3702,19 @@
         <v>3</v>
       </c>
       <c r="O14" t="s">
+        <v>145</v>
+      </c>
+      <c r="P14" t="s">
         <v>146</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>147</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>148</v>
       </c>
-      <c r="R14" t="s">
+      <c r="U14" t="s">
         <v>149</v>
-      </c>
-      <c r="U14" t="s">
-        <v>150</v>
       </c>
       <c r="AA14" s="19"/>
       <c r="AB14" s="19"/>
@@ -3727,19 +3730,19 @@
         <v>51312</v>
       </c>
       <c r="AT14" t="s">
+        <v>150</v>
+      </c>
+      <c r="AU14" t="s">
         <v>151</v>
       </c>
-      <c r="AU14" t="s">
-        <v>152</v>
-      </c>
       <c r="BC14" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI14" t="s">
         <v>355</v>
       </c>
-      <c r="BI14" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK14">
         <v>2</v>
@@ -3768,13 +3771,13 @@
     </row>
     <row r="15" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
         <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J15" t="s">
         <v>66</v>
@@ -3786,19 +3789,19 @@
         <v>3</v>
       </c>
       <c r="O15" t="s">
+        <v>154</v>
+      </c>
+      <c r="P15" t="s">
         <v>155</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>156</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="R15" s="16" t="s">
-        <v>158</v>
-      </c>
       <c r="U15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AA15" s="19"/>
       <c r="AB15" s="19"/>
@@ -3814,19 +3817,19 @@
         <v>51312</v>
       </c>
       <c r="AT15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AU15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BC15" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI15" t="s">
         <v>355</v>
       </c>
-      <c r="BI15" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK15">
         <v>2</v>
@@ -3855,16 +3858,16 @@
     </row>
     <row r="16" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" t="s">
+        <v>326</v>
+      </c>
+      <c r="D16" t="s">
         <v>160</v>
       </c>
-      <c r="C16" t="s">
-        <v>327</v>
-      </c>
-      <c r="D16" t="s">
-        <v>161</v>
-      </c>
       <c r="F16" s="16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J16" t="s">
         <v>66</v>
@@ -3876,19 +3879,19 @@
         <v>3</v>
       </c>
       <c r="O16" t="s">
+        <v>161</v>
+      </c>
+      <c r="P16" t="s">
         <v>162</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>163</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>164</v>
       </c>
-      <c r="R16" t="s">
+      <c r="U16" t="s">
         <v>165</v>
-      </c>
-      <c r="U16" t="s">
-        <v>166</v>
       </c>
       <c r="AA16" s="19"/>
       <c r="AB16" s="19"/>
@@ -3904,19 +3907,19 @@
         <v>51312</v>
       </c>
       <c r="AT16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AU16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BC16" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI16" t="s">
         <v>355</v>
       </c>
-      <c r="BI16" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK16">
         <v>2</v>
@@ -3945,13 +3948,13 @@
     </row>
     <row r="17" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" t="s">
+        <v>327</v>
+      </c>
+      <c r="D17" t="s">
         <v>167</v>
-      </c>
-      <c r="C17" t="s">
-        <v>328</v>
-      </c>
-      <c r="D17" t="s">
-        <v>168</v>
       </c>
       <c r="J17" t="s">
         <v>66</v>
@@ -3963,16 +3966,16 @@
         <v>3</v>
       </c>
       <c r="O17" t="s">
+        <v>337</v>
+      </c>
+      <c r="P17" t="s">
         <v>338</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>339</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>340</v>
-      </c>
-      <c r="R17" t="s">
-        <v>341</v>
       </c>
       <c r="U17" s="16" t="s">
         <v>114</v>
@@ -3991,19 +3994,19 @@
         <v>51312</v>
       </c>
       <c r="AT17" t="s">
+        <v>168</v>
+      </c>
+      <c r="AU17" t="s">
         <v>169</v>
       </c>
-      <c r="AU17" t="s">
-        <v>170</v>
-      </c>
       <c r="BC17" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI17" t="s">
         <v>355</v>
       </c>
-      <c r="BI17" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK17">
         <v>3</v>
@@ -4032,13 +4035,13 @@
     </row>
     <row r="18" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C18" t="s">
         <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J18" t="s">
         <v>66</v>
@@ -4050,19 +4053,19 @@
         <v>3</v>
       </c>
       <c r="O18" t="s">
+        <v>172</v>
+      </c>
+      <c r="P18" t="s">
         <v>173</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>174</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>175</v>
       </c>
-      <c r="R18" t="s">
+      <c r="U18" t="s">
         <v>176</v>
-      </c>
-      <c r="U18" t="s">
-        <v>177</v>
       </c>
       <c r="AA18" s="19"/>
       <c r="AB18" s="19"/>
@@ -4078,19 +4081,19 @@
         <v>51312</v>
       </c>
       <c r="AT18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AU18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="BC18" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI18" t="s">
         <v>355</v>
       </c>
-      <c r="BI18" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK18">
         <v>3</v>
@@ -4119,13 +4122,13 @@
     </row>
     <row r="19" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>178</v>
+      </c>
+      <c r="C19" t="s">
+        <v>327</v>
+      </c>
+      <c r="D19" t="s">
         <v>179</v>
-      </c>
-      <c r="C19" t="s">
-        <v>328</v>
-      </c>
-      <c r="D19" t="s">
-        <v>180</v>
       </c>
       <c r="J19" t="s">
         <v>66</v>
@@ -4137,16 +4140,16 @@
         <v>3</v>
       </c>
       <c r="O19" t="s">
+        <v>341</v>
+      </c>
+      <c r="P19" t="s">
         <v>342</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>343</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>344</v>
-      </c>
-      <c r="R19" t="s">
-        <v>345</v>
       </c>
       <c r="U19" t="s">
         <v>114</v>
@@ -4165,19 +4168,19 @@
         <v>51312</v>
       </c>
       <c r="AT19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AU19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BC19" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI19" t="s">
         <v>355</v>
       </c>
-      <c r="BI19" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK19">
         <v>3</v>
@@ -4206,13 +4209,13 @@
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C20" t="s">
         <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J20" t="s">
         <v>66</v>
@@ -4224,19 +4227,19 @@
         <v>3</v>
       </c>
       <c r="O20" t="s">
+        <v>183</v>
+      </c>
+      <c r="P20" t="s">
         <v>184</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>185</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>186</v>
       </c>
-      <c r="R20" t="s">
+      <c r="U20" t="s">
         <v>187</v>
-      </c>
-      <c r="U20" t="s">
-        <v>188</v>
       </c>
       <c r="AA20" s="19"/>
       <c r="AB20" s="19"/>
@@ -4252,19 +4255,19 @@
         <v>51312</v>
       </c>
       <c r="AT20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AU20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BC20" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI20" t="s">
         <v>355</v>
       </c>
-      <c r="BI20" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK20">
         <v>3</v>
@@ -4293,13 +4296,13 @@
     </row>
     <row r="21" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C21" t="s">
         <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F21" s="17"/>
       <c r="J21" t="s">
@@ -4312,16 +4315,16 @@
         <v>3</v>
       </c>
       <c r="O21" t="s">
+        <v>191</v>
+      </c>
+      <c r="P21" t="s">
         <v>192</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>193</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>194</v>
-      </c>
-      <c r="R21" t="s">
-        <v>195</v>
       </c>
       <c r="U21" t="s">
         <v>95</v>
@@ -4340,19 +4343,19 @@
         <v>51312</v>
       </c>
       <c r="AT21" t="s">
+        <v>195</v>
+      </c>
+      <c r="AU21" t="s">
         <v>196</v>
       </c>
-      <c r="AU21" t="s">
-        <v>197</v>
-      </c>
       <c r="BC21" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI21" t="s">
         <v>355</v>
       </c>
-      <c r="BI21" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK21">
         <v>3</v>
@@ -4381,13 +4384,13 @@
     </row>
     <row r="22" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C22" t="s">
         <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F22" s="17"/>
       <c r="J22" t="s">
@@ -4400,19 +4403,19 @@
         <v>3</v>
       </c>
       <c r="O22" t="s">
+        <v>199</v>
+      </c>
+      <c r="P22" t="s">
         <v>200</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>201</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="R22" t="s">
         <v>202</v>
       </c>
-      <c r="R22" t="s">
-        <v>203</v>
-      </c>
       <c r="U22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AA22" s="19"/>
       <c r="AB22" s="19"/>
@@ -4428,19 +4431,19 @@
         <v>51312</v>
       </c>
       <c r="AT22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AU22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BC22" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI22" t="s">
         <v>355</v>
       </c>
-      <c r="BI22" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK22">
         <v>3</v>
@@ -4469,13 +4472,13 @@
     </row>
     <row r="23" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C23" t="s">
         <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F23" s="17"/>
       <c r="J23" t="s">
@@ -4488,19 +4491,19 @@
         <v>3</v>
       </c>
       <c r="O23" t="s">
+        <v>206</v>
+      </c>
+      <c r="P23" t="s">
         <v>207</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>208</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="R23" t="s">
         <v>209</v>
       </c>
-      <c r="R23" t="s">
-        <v>210</v>
-      </c>
       <c r="U23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA23" s="19"/>
       <c r="AB23" s="19"/>
@@ -4516,19 +4519,19 @@
         <v>51312</v>
       </c>
       <c r="AT23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AU23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="BC23" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI23" t="s">
         <v>355</v>
       </c>
-      <c r="BI23" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ23" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK23">
         <v>3</v>
@@ -4557,16 +4560,16 @@
     </row>
     <row r="24" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>211</v>
+      </c>
+      <c r="C24" t="s">
+        <v>326</v>
+      </c>
+      <c r="D24" t="s">
         <v>212</v>
       </c>
-      <c r="C24" t="s">
-        <v>327</v>
-      </c>
-      <c r="D24" t="s">
-        <v>213</v>
-      </c>
       <c r="F24" s="16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J24" t="s">
         <v>66</v>
@@ -4578,16 +4581,16 @@
         <v>3</v>
       </c>
       <c r="O24" t="s">
+        <v>213</v>
+      </c>
+      <c r="P24" t="s">
         <v>214</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>215</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>216</v>
-      </c>
-      <c r="R24" t="s">
-        <v>217</v>
       </c>
       <c r="U24" t="s">
         <v>114</v>
@@ -4606,19 +4609,19 @@
         <v>51312</v>
       </c>
       <c r="AT24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AU24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="BC24" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI24" t="s">
         <v>355</v>
       </c>
-      <c r="BI24" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK24">
         <v>3</v>
@@ -4647,16 +4650,16 @@
     </row>
     <row r="25" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>218</v>
+      </c>
+      <c r="C25" t="s">
+        <v>326</v>
+      </c>
+      <c r="D25" t="s">
         <v>219</v>
       </c>
-      <c r="C25" t="s">
-        <v>327</v>
-      </c>
-      <c r="D25" t="s">
-        <v>220</v>
-      </c>
       <c r="F25" s="16" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J25" t="s">
         <v>66</v>
@@ -4668,16 +4671,16 @@
         <v>3</v>
       </c>
       <c r="O25" t="s">
+        <v>220</v>
+      </c>
+      <c r="P25" t="s">
         <v>221</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>222</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>223</v>
-      </c>
-      <c r="R25" t="s">
-        <v>224</v>
       </c>
       <c r="U25" t="s">
         <v>114</v>
@@ -4696,19 +4699,19 @@
         <v>51312</v>
       </c>
       <c r="AT25" t="s">
+        <v>224</v>
+      </c>
+      <c r="AU25" t="s">
         <v>225</v>
       </c>
-      <c r="AU25" t="s">
-        <v>226</v>
-      </c>
       <c r="BC25" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI25" t="s">
         <v>355</v>
       </c>
-      <c r="BI25" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK25">
         <v>3</v>
@@ -4737,17 +4740,17 @@
     </row>
     <row r="26" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C26" t="s">
         <v>117</v>
       </c>
       <c r="D26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F26" s="16"/>
       <c r="J26" t="s">
-        <v>357</v>
+        <v>370</v>
       </c>
       <c r="L26">
         <v>4</v>
@@ -4756,19 +4759,19 @@
         <v>4</v>
       </c>
       <c r="O26" t="s">
+        <v>228</v>
+      </c>
+      <c r="P26" t="s">
         <v>229</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>230</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>231</v>
       </c>
-      <c r="R26" t="s">
-        <v>232</v>
-      </c>
       <c r="U26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AA26" s="19">
         <v>1</v>
@@ -4792,19 +4795,19 @@
         <v>51312</v>
       </c>
       <c r="AT26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AU26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="BC26" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI26" t="s">
         <v>355</v>
       </c>
-      <c r="BI26" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK26">
         <v>3</v>
@@ -4833,16 +4836,16 @@
     </row>
     <row r="27" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>233</v>
+      </c>
+      <c r="C27" t="s">
+        <v>326</v>
+      </c>
+      <c r="D27" t="s">
         <v>234</v>
       </c>
-      <c r="C27" t="s">
-        <v>327</v>
-      </c>
-      <c r="D27" t="s">
-        <v>235</v>
-      </c>
       <c r="F27" s="16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J27" t="s">
         <v>66</v>
@@ -4854,19 +4857,19 @@
         <v>3</v>
       </c>
       <c r="O27" t="s">
+        <v>235</v>
+      </c>
+      <c r="P27" t="s">
         <v>236</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>237</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>238</v>
       </c>
-      <c r="R27" t="s">
-        <v>239</v>
-      </c>
       <c r="U27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA27" s="19"/>
       <c r="AB27" s="19"/>
@@ -4882,19 +4885,19 @@
         <v>51312</v>
       </c>
       <c r="AT27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AU27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="BC27" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI27" t="s">
         <v>355</v>
       </c>
-      <c r="BI27" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK27">
         <v>3</v>
@@ -4923,13 +4926,13 @@
     </row>
     <row r="28" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C28" t="s">
         <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F28" s="17"/>
       <c r="J28" t="s">
@@ -4942,19 +4945,19 @@
         <v>3</v>
       </c>
       <c r="O28" t="s">
+        <v>242</v>
+      </c>
+      <c r="P28" t="s">
         <v>243</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>244</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="R28" t="s">
         <v>245</v>
       </c>
-      <c r="R28" t="s">
-        <v>246</v>
-      </c>
       <c r="U28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AA28" s="19"/>
       <c r="AB28" s="19"/>
@@ -4970,19 +4973,19 @@
         <v>51312</v>
       </c>
       <c r="AT28" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AU28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="BC28" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI28" t="s">
         <v>355</v>
       </c>
-      <c r="BI28" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ28" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK28">
         <v>3</v>
@@ -5011,13 +5014,13 @@
     </row>
     <row r="29" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C29" t="s">
         <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F29" s="17"/>
       <c r="J29" t="s">
@@ -5030,19 +5033,19 @@
         <v>3</v>
       </c>
       <c r="O29" t="s">
+        <v>249</v>
+      </c>
+      <c r="P29" t="s">
         <v>250</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>251</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>252</v>
       </c>
-      <c r="R29" t="s">
-        <v>253</v>
-      </c>
       <c r="U29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AA29" s="19"/>
       <c r="AB29" s="19"/>
@@ -5058,19 +5061,19 @@
         <v>51312</v>
       </c>
       <c r="AT29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AU29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="BC29" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="BI29" t="s">
         <v>355</v>
       </c>
-      <c r="BI29" t="s">
-        <v>358</v>
-      </c>
       <c r="BJ29" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BK29">
         <v>3</v>
@@ -5099,13 +5102,13 @@
     </row>
     <row r="30" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>64</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F30" s="28"/>
       <c r="J30" s="26" t="s">
@@ -5118,19 +5121,19 @@
         <v>3</v>
       </c>
       <c r="O30" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="P30" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="Q30" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="R30" s="26" t="s">
         <v>363</v>
       </c>
-      <c r="P30" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q30" s="26" t="s">
-        <v>365</v>
-      </c>
-      <c r="R30" s="26" t="s">
-        <v>366</v>
-      </c>
       <c r="U30" s="26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AA30" s="29"/>
       <c r="AB30" s="29"/>
@@ -5140,34 +5143,34 @@
         <v>1</v>
       </c>
       <c r="AQ30" s="26" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="AS30" s="26">
         <v>0</v>
       </c>
       <c r="AT30" s="26" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="AU30" s="26" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="BC30" s="30" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="BD30" s="31" t="s">
-        <v>353</v>
+        <v>369</v>
       </c>
       <c r="BE30" s="31" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="BF30" s="31">
         <v>20</v>
       </c>
       <c r="BI30" s="26" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="BJ30" s="26" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="BK30" s="26">
         <v>0</v>
@@ -5225,72 +5228,72 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>260</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" s="7">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="B3" s="7">
-        <v>4</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>266</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="10"/>
       <c r="F4" s="6"/>
       <c r="G4" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="10"/>
@@ -5300,7 +5303,7 @@
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="10"/>
@@ -5308,30 +5311,30 @@
     </row>
     <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B7" s="8">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="B7" s="8">
-        <v>4</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>273</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>274</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
@@ -5341,7 +5344,7 @@
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -5351,7 +5354,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
@@ -5359,19 +5362,19 @@
     </row>
     <row r="11" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="B11" s="7">
-        <v>4</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>280</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>281</v>
       </c>
       <c r="F11" s="6"/>
     </row>
@@ -5379,7 +5382,7 @@
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -5389,7 +5392,7 @@
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -5397,19 +5400,19 @@
     </row>
     <row r="14" spans="1:7" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B14" s="8">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="B14" s="8">
-        <v>3</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>286</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>287</v>
       </c>
       <c r="F14" s="6"/>
     </row>
@@ -5417,7 +5420,7 @@
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
@@ -5425,19 +5428,19 @@
     </row>
     <row r="16" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B16" s="7">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="B16" s="7">
-        <v>4</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="D16" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>290</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>291</v>
       </c>
       <c r="F16" s="6"/>
     </row>
@@ -5445,7 +5448,7 @@
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -5455,7 +5458,7 @@
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -5465,7 +5468,7 @@
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -5473,29 +5476,29 @@
     </row>
     <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B20" s="8">
+        <v>4</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="B20" s="8">
-        <v>4</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="F20" s="6" t="s">
         <v>297</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -5505,7 +5508,7 @@
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -5515,7 +5518,7 @@
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -5523,19 +5526,19 @@
     </row>
     <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B24" s="7">
         <v>5</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F24" s="6"/>
     </row>
@@ -5543,7 +5546,7 @@
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -5553,7 +5556,7 @@
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -5563,7 +5566,7 @@
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -5573,7 +5576,7 @@
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -5599,26 +5602,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100879B58D3C23DCA4AAEF47596CA4D8E48" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee8b9d8723b80ccc4cb578ffd4faacc7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02625a54-df84-4a3b-b049-0bb7e92cde0d" xmlns:ns3="c90f9e10-81f0-426e-b8bb-fc89022b3796" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64b8ed4db9a6e136c161da669116b9cc" ns2:_="" ns3:_="">
     <xsd:import namespace="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
@@ -5827,32 +5810,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5869,4 +5847,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed some excel stuff
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patric\Documents\GitHub\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477F9D4B-B373-48EB-BFA0-A2235A8210B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD33BE19-B687-493C-B5DC-7B155E184951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9792" yWindow="5952" windowWidth="26112" windowHeight="17352" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -1161,7 +1161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1236,7 +1236,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1293,18 +1293,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1319,6 +1307,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1413,7 +1419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1466,14 +1472,15 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2368,21 +2375,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
   <dimension ref="A1:BR30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BK30" sqref="BK30"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="BR35" sqref="BR35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.44140625" customWidth="1"/>
-    <col min="27" max="27" width="16.6640625" customWidth="1"/>
-    <col min="46" max="46" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" customWidth="1"/>
+    <col min="46" max="46" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:70" ht="39" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2594,7 +2601,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:70">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2691,14 +2698,10 @@
       <c r="BP2">
         <v>1</v>
       </c>
-      <c r="BQ2" s="21">
-        <v>102</v>
-      </c>
-      <c r="BR2" s="21">
-        <v>203</v>
-      </c>
+      <c r="BQ2" s="21"/>
+      <c r="BR2" s="21"/>
     </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -2781,14 +2784,10 @@
       <c r="BP3">
         <v>1</v>
       </c>
-      <c r="BQ3" s="21">
-        <v>102</v>
-      </c>
-      <c r="BR3" s="21">
-        <v>203</v>
-      </c>
+      <c r="BQ3" s="21"/>
+      <c r="BR3" s="21"/>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:70">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -2868,14 +2867,10 @@
       <c r="BP4">
         <v>1</v>
       </c>
-      <c r="BQ4" s="21">
-        <v>102</v>
-      </c>
-      <c r="BR4" s="21">
-        <v>203</v>
-      </c>
+      <c r="BQ4" s="21"/>
+      <c r="BR4" s="21"/>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:70">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -2956,14 +2951,10 @@
       <c r="BP5">
         <v>1</v>
       </c>
-      <c r="BQ5" s="21">
-        <v>102</v>
-      </c>
-      <c r="BR5" s="21">
-        <v>203</v>
-      </c>
+      <c r="BQ5" s="21"/>
+      <c r="BR5" s="21"/>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -3053,7 +3044,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -3143,7 +3134,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:70">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -3230,7 +3221,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:70">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -3320,7 +3311,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:70">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -3408,14 +3399,10 @@
       <c r="BP10">
         <v>1</v>
       </c>
-      <c r="BQ10" s="23">
-        <v>103</v>
-      </c>
-      <c r="BR10" s="23">
-        <v>205</v>
-      </c>
+      <c r="BQ10" s="23"/>
+      <c r="BR10" s="23"/>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:70">
       <c r="A11" t="s">
         <v>127</v>
       </c>
@@ -3495,14 +3482,10 @@
       <c r="BP11">
         <v>1</v>
       </c>
-      <c r="BQ11" s="23">
-        <v>103</v>
-      </c>
-      <c r="BR11" s="23">
-        <v>205</v>
-      </c>
+      <c r="BQ11" s="23"/>
+      <c r="BR11" s="23"/>
     </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:70">
       <c r="A12" t="s">
         <v>130</v>
       </c>
@@ -3582,14 +3565,10 @@
       <c r="BP12">
         <v>1</v>
       </c>
-      <c r="BQ12" s="23">
-        <v>103</v>
-      </c>
-      <c r="BR12" s="23">
-        <v>205</v>
-      </c>
+      <c r="BQ12" s="23"/>
+      <c r="BR12" s="23"/>
     </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:70">
       <c r="A13" t="s">
         <v>136</v>
       </c>
@@ -3669,14 +3648,10 @@
       <c r="BP13">
         <v>1</v>
       </c>
-      <c r="BQ13" s="23">
-        <v>103</v>
-      </c>
-      <c r="BR13" s="23">
-        <v>205</v>
-      </c>
+      <c r="BQ13" s="23"/>
+      <c r="BR13" s="23"/>
     </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:70">
       <c r="A14" t="s">
         <v>144</v>
       </c>
@@ -3741,7 +3716,7 @@
       <c r="BK14">
         <v>2</v>
       </c>
-      <c r="BL14" s="24">
+      <c r="BL14" s="31">
         <v>4</v>
       </c>
       <c r="BM14">
@@ -3756,14 +3731,14 @@
       <c r="BP14">
         <v>1</v>
       </c>
-      <c r="BQ14" s="24">
+      <c r="BQ14" s="31">
         <v>104</v>
       </c>
-      <c r="BR14" s="24">
+      <c r="BR14" s="31">
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:70">
       <c r="A15" t="s">
         <v>153</v>
       </c>
@@ -3828,7 +3803,7 @@
       <c r="BK15">
         <v>2</v>
       </c>
-      <c r="BL15" s="24">
+      <c r="BL15" s="31">
         <v>4</v>
       </c>
       <c r="BM15">
@@ -3843,14 +3818,14 @@
       <c r="BP15">
         <v>1</v>
       </c>
-      <c r="BQ15" s="24">
+      <c r="BQ15" s="31">
         <v>104</v>
       </c>
-      <c r="BR15" s="24">
+      <c r="BR15" s="31">
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:70">
       <c r="A16" t="s">
         <v>160</v>
       </c>
@@ -3918,7 +3893,7 @@
       <c r="BK16">
         <v>2</v>
       </c>
-      <c r="BL16" s="24">
+      <c r="BL16" s="31">
         <v>4</v>
       </c>
       <c r="BM16">
@@ -3933,14 +3908,14 @@
       <c r="BP16">
         <v>1</v>
       </c>
-      <c r="BQ16" s="24">
+      <c r="BQ16" s="31">
         <v>104</v>
       </c>
-      <c r="BR16" s="24">
+      <c r="BR16" s="31">
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:70">
       <c r="A17" t="s">
         <v>167</v>
       </c>
@@ -4005,7 +3980,7 @@
       <c r="BK17">
         <v>3</v>
       </c>
-      <c r="BL17" s="25">
+      <c r="BL17" s="32">
         <v>5</v>
       </c>
       <c r="BM17">
@@ -4020,14 +3995,14 @@
       <c r="BP17">
         <v>1</v>
       </c>
-      <c r="BQ17" s="25">
+      <c r="BQ17" s="30">
         <v>105</v>
       </c>
-      <c r="BR17" s="25">
+      <c r="BR17" s="30">
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:70">
       <c r="A18" t="s">
         <v>171</v>
       </c>
@@ -4092,7 +4067,7 @@
       <c r="BK18">
         <v>3</v>
       </c>
-      <c r="BL18" s="25">
+      <c r="BL18" s="32">
         <v>5</v>
       </c>
       <c r="BM18">
@@ -4107,14 +4082,14 @@
       <c r="BP18">
         <v>1</v>
       </c>
-      <c r="BQ18" s="25">
+      <c r="BQ18" s="30">
         <v>105</v>
       </c>
-      <c r="BR18" s="25">
+      <c r="BR18" s="30">
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:70">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -4179,7 +4154,7 @@
       <c r="BK19">
         <v>3</v>
       </c>
-      <c r="BL19" s="25">
+      <c r="BL19" s="32">
         <v>5</v>
       </c>
       <c r="BM19">
@@ -4194,14 +4169,14 @@
       <c r="BP19">
         <v>1</v>
       </c>
-      <c r="BQ19" s="25">
+      <c r="BQ19" s="30">
         <v>105</v>
       </c>
-      <c r="BR19" s="25">
+      <c r="BR19" s="30">
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:70">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -4266,7 +4241,7 @@
       <c r="BK20">
         <v>3</v>
       </c>
-      <c r="BL20" s="25">
+      <c r="BL20" s="32">
         <v>5</v>
       </c>
       <c r="BM20">
@@ -4281,14 +4256,14 @@
       <c r="BP20">
         <v>1</v>
       </c>
-      <c r="BQ20" s="25">
+      <c r="BQ20" s="30">
         <v>105</v>
       </c>
-      <c r="BR20" s="25">
+      <c r="BR20" s="30">
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:70">
       <c r="A21" t="s">
         <v>190</v>
       </c>
@@ -4354,7 +4329,7 @@
       <c r="BK21">
         <v>3</v>
       </c>
-      <c r="BL21" s="26">
+      <c r="BL21" s="24">
         <v>6</v>
       </c>
       <c r="BM21">
@@ -4369,14 +4344,10 @@
       <c r="BP21">
         <v>1</v>
       </c>
-      <c r="BQ21" s="26">
-        <v>103</v>
-      </c>
-      <c r="BR21" s="26">
-        <v>205</v>
-      </c>
+      <c r="BQ21" s="24"/>
+      <c r="BR21" s="24"/>
     </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:70">
       <c r="A22" t="s">
         <v>198</v>
       </c>
@@ -4442,7 +4413,7 @@
       <c r="BK22">
         <v>3</v>
       </c>
-      <c r="BL22" s="26">
+      <c r="BL22" s="24">
         <v>6</v>
       </c>
       <c r="BM22">
@@ -4457,14 +4428,10 @@
       <c r="BP22">
         <v>1</v>
       </c>
-      <c r="BQ22" s="26">
-        <v>103</v>
-      </c>
-      <c r="BR22" s="26">
-        <v>205</v>
-      </c>
+      <c r="BQ22" s="24"/>
+      <c r="BR22" s="24"/>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:70">
       <c r="A23" t="s">
         <v>205</v>
       </c>
@@ -4530,7 +4497,7 @@
       <c r="BK23">
         <v>3</v>
       </c>
-      <c r="BL23" s="26">
+      <c r="BL23" s="24">
         <v>6</v>
       </c>
       <c r="BM23">
@@ -4545,14 +4512,10 @@
       <c r="BP23">
         <v>1</v>
       </c>
-      <c r="BQ23" s="26">
-        <v>103</v>
-      </c>
-      <c r="BR23" s="26">
-        <v>205</v>
-      </c>
+      <c r="BQ23" s="24"/>
+      <c r="BR23" s="24"/>
     </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:70">
       <c r="A24" t="s">
         <v>212</v>
       </c>
@@ -4620,7 +4583,7 @@
       <c r="BK24">
         <v>3</v>
       </c>
-      <c r="BL24" s="26">
+      <c r="BL24" s="24">
         <v>6</v>
       </c>
       <c r="BM24">
@@ -4635,14 +4598,10 @@
       <c r="BP24">
         <v>1</v>
       </c>
-      <c r="BQ24" s="26">
-        <v>103</v>
-      </c>
-      <c r="BR24" s="26">
-        <v>205</v>
-      </c>
+      <c r="BQ24" s="24"/>
+      <c r="BR24" s="24"/>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:70">
       <c r="A25" t="s">
         <v>219</v>
       </c>
@@ -4710,7 +4669,7 @@
       <c r="BK25">
         <v>3</v>
       </c>
-      <c r="BL25" s="27">
+      <c r="BL25" s="25">
         <v>6</v>
       </c>
       <c r="BM25">
@@ -4725,14 +4684,10 @@
       <c r="BP25">
         <v>1</v>
       </c>
-      <c r="BQ25" s="27">
-        <v>102</v>
-      </c>
-      <c r="BR25" s="27">
-        <v>203</v>
-      </c>
+      <c r="BQ25" s="25"/>
+      <c r="BR25" s="25"/>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:70">
       <c r="A26" t="s">
         <v>227</v>
       </c>
@@ -4806,7 +4761,7 @@
       <c r="BK26">
         <v>3</v>
       </c>
-      <c r="BL26" s="27">
+      <c r="BL26" s="25">
         <v>6</v>
       </c>
       <c r="BM26">
@@ -4821,14 +4776,10 @@
       <c r="BP26">
         <v>1</v>
       </c>
-      <c r="BQ26" s="27">
-        <v>102</v>
-      </c>
-      <c r="BR26" s="27">
-        <v>203</v>
-      </c>
+      <c r="BQ26" s="25"/>
+      <c r="BR26" s="25"/>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:70">
       <c r="A27" t="s">
         <v>234</v>
       </c>
@@ -4896,7 +4847,7 @@
       <c r="BK27">
         <v>3</v>
       </c>
-      <c r="BL27" s="27">
+      <c r="BL27" s="25">
         <v>6</v>
       </c>
       <c r="BM27">
@@ -4911,14 +4862,10 @@
       <c r="BP27">
         <v>1</v>
       </c>
-      <c r="BQ27" s="27">
-        <v>102</v>
-      </c>
-      <c r="BR27" s="27">
-        <v>203</v>
-      </c>
+      <c r="BQ27" s="25"/>
+      <c r="BR27" s="25"/>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:70">
       <c r="A28" t="s">
         <v>241</v>
       </c>
@@ -4984,7 +4931,7 @@
       <c r="BK28">
         <v>3</v>
       </c>
-      <c r="BL28" s="27">
+      <c r="BL28" s="25">
         <v>6</v>
       </c>
       <c r="BM28">
@@ -4999,14 +4946,10 @@
       <c r="BP28">
         <v>1</v>
       </c>
-      <c r="BQ28" s="27">
-        <v>102</v>
-      </c>
-      <c r="BR28" s="27">
-        <v>203</v>
-      </c>
+      <c r="BQ28" s="25"/>
+      <c r="BR28" s="25"/>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:70">
       <c r="A29" t="s">
         <v>248</v>
       </c>
@@ -5072,7 +5015,7 @@
       <c r="BK29">
         <v>3</v>
       </c>
-      <c r="BL29" s="27">
+      <c r="BL29" s="25">
         <v>6</v>
       </c>
       <c r="BM29">
@@ -5087,107 +5030,103 @@
       <c r="BP29">
         <v>1</v>
       </c>
-      <c r="BQ29" s="27">
-        <v>102</v>
-      </c>
-      <c r="BR29" s="27">
-        <v>203</v>
-      </c>
+      <c r="BQ29" s="25"/>
+      <c r="BR29" s="25"/>
     </row>
-    <row r="30" spans="1:70" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+    <row r="30" spans="1:70" s="24" customFormat="1">
+      <c r="A30" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="24" t="s">
         <v>362</v>
       </c>
-      <c r="F30" s="28"/>
-      <c r="J30" s="26" t="s">
+      <c r="F30" s="26"/>
+      <c r="J30" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="L30" s="26">
-        <v>4</v>
-      </c>
-      <c r="N30" s="26">
-        <v>3</v>
-      </c>
-      <c r="O30" s="26" t="s">
+      <c r="L30" s="24">
+        <v>4</v>
+      </c>
+      <c r="N30" s="24">
+        <v>3</v>
+      </c>
+      <c r="O30" s="24" t="s">
         <v>363</v>
       </c>
-      <c r="P30" s="26" t="s">
+      <c r="P30" s="24" t="s">
         <v>364</v>
       </c>
-      <c r="Q30" s="26" t="s">
+      <c r="Q30" s="24" t="s">
         <v>365</v>
       </c>
-      <c r="R30" s="26" t="s">
+      <c r="R30" s="24" t="s">
         <v>366</v>
       </c>
-      <c r="U30" s="26" t="s">
+      <c r="U30" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="AA30" s="29"/>
-      <c r="AB30" s="29"/>
-      <c r="AC30" s="29"/>
-      <c r="AD30" s="29"/>
-      <c r="AK30" s="26">
-        <v>1</v>
-      </c>
-      <c r="AQ30" s="26" t="s">
+      <c r="AA30" s="27"/>
+      <c r="AB30" s="27"/>
+      <c r="AC30" s="27"/>
+      <c r="AD30" s="27"/>
+      <c r="AK30" s="24">
+        <v>1</v>
+      </c>
+      <c r="AQ30" s="24" t="s">
         <v>367</v>
       </c>
-      <c r="AS30" s="26">
+      <c r="AS30" s="24">
         <v>0</v>
       </c>
-      <c r="AT30" s="26" t="s">
+      <c r="AT30" s="24" t="s">
         <v>370</v>
       </c>
-      <c r="AU30" s="26" t="s">
+      <c r="AU30" s="24" t="s">
         <v>370</v>
       </c>
-      <c r="BC30" s="30" t="s">
+      <c r="BC30" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="BD30" s="31" t="s">
+      <c r="BD30" s="29" t="s">
         <v>353</v>
       </c>
-      <c r="BE30" s="31" t="s">
+      <c r="BE30" s="29" t="s">
         <v>354</v>
       </c>
-      <c r="BF30" s="31">
+      <c r="BF30" s="29">
         <v>20</v>
       </c>
-      <c r="BI30" s="26" t="s">
+      <c r="BI30" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="BJ30" s="26" t="s">
+      <c r="BJ30" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="BK30" s="26">
+      <c r="BK30" s="24">
         <v>0</v>
       </c>
-      <c r="BL30" s="26">
+      <c r="BL30" s="24">
         <v>-1</v>
       </c>
-      <c r="BM30" s="26">
+      <c r="BM30" s="24">
         <v>0</v>
       </c>
-      <c r="BN30" s="26">
+      <c r="BN30" s="24">
         <v>0</v>
       </c>
-      <c r="BO30" s="26">
-        <v>4</v>
-      </c>
-      <c r="BP30" s="26">
+      <c r="BO30" s="24">
+        <v>4</v>
+      </c>
+      <c r="BP30" s="24">
         <v>2</v>
       </c>
-      <c r="BQ30" s="26">
+      <c r="BQ30" s="24">
         <v>-1</v>
       </c>
-      <c r="BR30" s="26">
+      <c r="BR30" s="24">
         <v>-1</v>
       </c>
     </row>
@@ -5210,24 +5149,24 @@
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="15" t="s">
         <v>255</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="38.25">
       <c r="A2" s="14" t="s">
         <v>256</v>
       </c>
@@ -5247,7 +5186,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="51.6" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>262</v>
       </c>
@@ -5270,7 +5209,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="22.5" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
@@ -5283,7 +5222,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="17.649999999999999" customHeight="1">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
@@ -5293,7 +5232,7 @@
       <c r="E5" s="10"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
@@ -5303,7 +5242,7 @@
       <c r="E6" s="10"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>272</v>
       </c>
@@ -5324,7 +5263,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="27" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
@@ -5334,7 +5273,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="17.649999999999999" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
@@ -5344,7 +5283,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="31.5" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
@@ -5354,7 +5293,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="17.649999999999999" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>279</v>
       </c>
@@ -5372,7 +5311,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="20.65" customHeight="1">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
@@ -5382,7 +5321,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="23.1" customHeight="1">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
@@ -5392,7 +5331,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="32.65" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>284</v>
       </c>
@@ -5410,7 +5349,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
@@ -5420,7 +5359,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="20.65" customHeight="1">
       <c r="A16" s="7" t="s">
         <v>289</v>
       </c>
@@ -5438,7 +5377,7 @@
       </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="21" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
@@ -5448,7 +5387,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="22.15" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
@@ -5458,7 +5397,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
@@ -5468,7 +5407,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="32.1" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>295</v>
       </c>
@@ -5488,7 +5427,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="22.15" customHeight="1">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
@@ -5498,7 +5437,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="23.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="23.65" customHeight="1">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
@@ -5508,7 +5447,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="20.65" customHeight="1">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
@@ -5518,7 +5457,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="25.5">
       <c r="A24" s="7" t="s">
         <v>302</v>
       </c>
@@ -5536,7 +5475,7 @@
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
@@ -5546,7 +5485,7 @@
       <c r="E25" s="7"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="20.65" customHeight="1">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
@@ -5556,7 +5495,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="21" customHeight="1">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
@@ -5566,7 +5505,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="19.5" customHeight="1">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
@@ -5576,11 +5515,11 @@
       <c r="E28" s="7"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:6" ht="13.15" customHeight="1"/>
+    <row r="30" spans="1:6" ht="16.149999999999999" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="159" ht="26.25" customHeight="1"/>
+    <row r="163" ht="27" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" display="https://www.biwe-bbq.de/weiterbildungsportal/themen/coaching-qualifizierung/einzelansicht/tq-lagerlogistik" xr:uid="{508EE104-A0F6-4678-8237-1AA62422A333}"/>
@@ -5596,15 +5535,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
@@ -5613,6 +5543,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5825,14 +5764,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -5845,6 +5776,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added NeedsRecommendation to AssessmentCategoryResult
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/Booklet_FK_Lagerlogistik.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C165F1-CC53-40A3-B7EE-A51A516BE942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BE904E-7ABD-435A-B49C-8EED5500DAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
@@ -2371,12 +2371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
   <dimension ref="A1:BR30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="BE2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="AP1" sqref="AP1"/>
-      <selection pane="topRight" activeCell="AV1" sqref="AV1"/>
-      <selection pane="bottomLeft" activeCell="AP2" sqref="AP2"/>
-      <selection pane="bottomRight" activeCell="BR10" sqref="BR10:BR13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5558,15 +5554,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100879B58D3C23DCA4AAEF47596CA4D8E48" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee8b9d8723b80ccc4cb578ffd4faacc7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02625a54-df84-4a3b-b049-0bb7e92cde0d" xmlns:ns3="c90f9e10-81f0-426e-b8bb-fc89022b3796" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64b8ed4db9a6e136c161da669116b9cc" ns2:_="" ns3:_="">
     <xsd:import namespace="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
@@ -5775,6 +5762,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5787,14 +5783,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5809,6 +5797,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>